<commit_message>
datos del dia 4-04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B1832F-9BAC-454B-9B57-D4D76F3D505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19376BB-5D09-4777-A336-CA89E6AFF86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="510" windowWidth="19950" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Usuario</t>
   </si>
@@ -345,6 +345,51 @@
   </si>
   <si>
     <t>Registro Insertado</t>
+  </si>
+  <si>
+    <t>9651</t>
+  </si>
+  <si>
+    <t>Madolche</t>
+  </si>
+  <si>
+    <t>Robar sentido Nivel bajo</t>
+  </si>
+  <si>
+    <t>Rokket</t>
+  </si>
+  <si>
+    <t>Lanzamiento Borre</t>
+  </si>
+  <si>
+    <t>Rose Dragon</t>
+  </si>
+  <si>
+    <t>Conjuro de Rosas</t>
+  </si>
+  <si>
+    <t>Solfachord</t>
+  </si>
+  <si>
+    <t>Péndulos Unidos</t>
+  </si>
+  <si>
+    <t>Synchrons</t>
+  </si>
+  <si>
+    <t>Un Vínculo Ilumina el Futuro</t>
+  </si>
+  <si>
+    <t>Infernoid</t>
+  </si>
+  <si>
+    <t>Aumento de LP alfa</t>
+  </si>
+  <si>
+    <t>Alma Rugiente</t>
+  </si>
+  <si>
+    <t>Resonators</t>
   </si>
 </sst>
 </file>
@@ -679,8 +724,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K8" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -999,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,32 +1092,278 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="6"/>
-      <c r="E2" s="3" t="str">
+      <c r="A2" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3">
         <f>IF($A2="","",$A2-1)</f>
-        <v/>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="K2" s="1" t="str">
+        <v>45020</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
         <f>IFERROR(ROUND((VALUE(TEXT($E2,"DD"))),0),"")</f>
-        <v/>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
+      <c r="A3" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B3" s="6">
+        <v>9881</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3">
+        <f>IF($A3="","",$A3-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E3,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2947</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <f>IF($A4="","",$A4-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E4,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2848</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3">
+        <f>IF($A5="","",$A5-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E5,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B6" s="6">
+        <v>7906</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <f>IF($A6="","",$A6-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E6,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B7" s="6">
+        <v>770</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3">
+        <f>IF($A7="","",$A7-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E7,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3338</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3">
+        <f>IF($A8="","",$A8-1)</f>
+        <v>45020</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E8,"DD"))),0),"")</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J2" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J8" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B8" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
datos dial dia 5-04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19376BB-5D09-4777-A336-CA89E6AFF86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12764FF0-40EF-46EE-AADA-7E76D0630E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Usuario</t>
   </si>
@@ -390,6 +390,78 @@
   </si>
   <si>
     <t>Resonators</t>
+  </si>
+  <si>
+    <t>Odd-Eyes</t>
+  </si>
+  <si>
+    <t>Xiangke y Xiangsheng</t>
+  </si>
+  <si>
+    <t>Phantom Knights</t>
+  </si>
+  <si>
+    <t>Fantasma de la Traición</t>
+  </si>
+  <si>
+    <t>Mermail Atlantean</t>
+  </si>
+  <si>
+    <t>Territorio de Tiburones</t>
+  </si>
+  <si>
+    <t>World Chalice</t>
+  </si>
+  <si>
+    <t>Constructor de Laberinto</t>
+  </si>
+  <si>
+    <t>Railway</t>
+  </si>
+  <si>
+    <t>Tren Imparable</t>
+  </si>
+  <si>
+    <t>Heros</t>
+  </si>
+  <si>
+    <t>Héroe Herido</t>
+  </si>
+  <si>
+    <t>Gouki</t>
+  </si>
+  <si>
+    <t>El Evento Principal Gouki</t>
+  </si>
+  <si>
+    <t>Valkyrie</t>
+  </si>
+  <si>
+    <t>Barrera de Luz</t>
+  </si>
+  <si>
+    <t>Dark Magician</t>
+  </si>
+  <si>
+    <t>Magia del Mago</t>
+  </si>
+  <si>
+    <t>Mekk-Knights</t>
+  </si>
+  <si>
+    <t>Vinculaciones</t>
+  </si>
+  <si>
+    <t>Gimmick Puppet</t>
+  </si>
+  <si>
+    <t>Marioneta Renunciada</t>
+  </si>
+  <si>
+    <t>Red-Eyes</t>
+  </si>
+  <si>
+    <t>Ruleta de Ojos Rojos</t>
   </si>
 </sst>
 </file>
@@ -724,8 +796,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K8" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K31" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1044,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="3">
-        <f>IF($A2="","",$A2-1)</f>
+        <f t="shared" ref="E2:E8" si="0">IF($A2="","",$A2-1)</f>
         <v>45020</v>
       </c>
       <c r="F2" s="4">
@@ -1124,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E2,"DD"))),0),"")</f>
+        <f t="shared" ref="K2:K8" si="1">IFERROR(ROUND((VALUE(TEXT($E2,"DD"))),0),"")</f>
         <v>4</v>
       </c>
     </row>
@@ -1142,7 +1214,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="3">
-        <f>IF($A3="","",$A3-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F3" s="4">
@@ -1161,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E3,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1179,7 +1251,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="3">
-        <f>IF($A4="","",$A4-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F4" s="4">
@@ -1198,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E4,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1216,7 +1288,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="3">
-        <f>IF($A5="","",$A5-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F5" s="4">
@@ -1235,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E5,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1253,7 +1325,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="3">
-        <f>IF($A6="","",$A6-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F6" s="4">
@@ -1272,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E6,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1290,7 +1362,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="3">
-        <f>IF($A7="","",$A7-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F7" s="4">
@@ -1309,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E7,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1327,7 +1399,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="3">
-        <f>IF($A8="","",$A8-1)</f>
+        <f t="shared" si="0"/>
         <v>45020</v>
       </c>
       <c r="F8" s="4">
@@ -1346,24 +1418,872 @@
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E8,"DD"))),0),"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6657</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3">
+        <f>IF($A9="","",$A9-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E9,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B10" s="6">
+        <v>7307</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3">
+        <f>IF($A10="","",$A10-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E10,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1131</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3">
+        <f>IF($A11="","",$A11-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E11,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3137</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3">
+        <f>IF($A12="","",$A12-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E12,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1463</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3">
+        <f>IF($A13="","",$A13-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E13,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B14" s="6">
+        <v>4978</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3">
+        <f>IF($A14="","",$A14-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E14,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B15" s="6">
+        <v>9379</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3">
+        <f>IF($A15="","",$A15-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E15,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1756</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3">
+        <f>IF($A16="","",$A16-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E16,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B17" s="6">
+        <v>7482</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3">
+        <f>IF($A17="","",$A17-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E17,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1458</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="3">
+        <f>IF($A18="","",$A18-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E18,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B19" s="6">
+        <v>8294</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="3">
+        <f>IF($A19="","",$A19-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E19,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3654</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3">
+        <f>IF($A20="","",$A20-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E20,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3261</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="3">
+        <f>IF($A21="","",$A21-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E21,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B22" s="6">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="3">
+        <f>IF($A22="","",$A22-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E22,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B23" s="6">
+        <v>4436</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="3">
+        <f>IF($A23="","",$A23-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E23,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B24" s="6">
+        <v>3494</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3">
+        <f>IF($A24="","",$A24-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E24,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B25" s="6">
+        <v>8751</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="3">
+        <f>IF($A25="","",$A25-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E25,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6637</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="3">
+        <f>IF($A26="","",$A26-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E26,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B27" s="6">
+        <v>7979</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="3">
+        <f>IF($A27="","",$A27-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E27,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2790</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="3">
+        <f>IF($A28="","",$A28-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E28,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B29" s="6">
+        <v>8171</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="3">
+        <f>IF($A29="","",$A29-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E29,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B30" s="6">
+        <v>8811</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="3">
+        <f>IF($A30="","",$A30-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E30,"DD"))),0),"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B31" s="6">
+        <v>3324</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="3">
+        <f>IF($A31="","",$A31-1)</f>
+        <v>45021</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E31,"DD"))),0),"")</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J8" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J31" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B8" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B31" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
datos del dia 6 y algunos del 7
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12764FF0-40EF-46EE-AADA-7E76D0630E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F7ACC-7600-4DFC-8831-1273EC80D605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>Usuario</t>
   </si>
@@ -462,6 +462,63 @@
   </si>
   <si>
     <t>Ruleta de Ojos Rojos</t>
+  </si>
+  <si>
+    <t>Cambios</t>
+  </si>
+  <si>
+    <t>Timelord</t>
+  </si>
+  <si>
+    <t>Starry Knight</t>
+  </si>
+  <si>
+    <t>Sonrisa del Hada</t>
+  </si>
+  <si>
+    <t>Code Talker</t>
+  </si>
+  <si>
+    <t>Codificador Hablador Vivo</t>
+  </si>
+  <si>
+    <t>Vacío, Infinito y Luz Infinita</t>
+  </si>
+  <si>
+    <t>Elemental Heros</t>
+  </si>
+  <si>
+    <t>Alianza de Héroes</t>
+  </si>
+  <si>
+    <t>D/D/D</t>
+  </si>
+  <si>
+    <t>El Mando del Rey de la Perdición</t>
+  </si>
+  <si>
+    <t>Block Dragon</t>
+  </si>
+  <si>
+    <t>Mundo Sonriente</t>
+  </si>
+  <si>
+    <t>Abyss Actor</t>
+  </si>
+  <si>
+    <t>Tumbas Selladas</t>
+  </si>
+  <si>
+    <t>Salamangreat</t>
+  </si>
+  <si>
+    <t>Alzarse desde el Valle de las Llamas</t>
+  </si>
+  <si>
+    <t>Fire King</t>
+  </si>
+  <si>
+    <t>Robo del Destino</t>
   </si>
 </sst>
 </file>
@@ -796,8 +853,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K31" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K66" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K66" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1116,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="3">
-        <f>IF($A9="","",$A9-1)</f>
+        <f t="shared" ref="E9:E31" si="2">IF($A9="","",$A9-1)</f>
         <v>45021</v>
       </c>
       <c r="F9" s="4">
@@ -1455,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E9,"DD"))),0),"")</f>
+        <f t="shared" ref="K9:K31" si="3">IFERROR(ROUND((VALUE(TEXT($E9,"DD"))),0),"")</f>
         <v>5</v>
       </c>
     </row>
@@ -1473,7 +1530,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="3">
-        <f>IF($A10="","",$A10-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F10" s="4">
@@ -1492,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E10,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1510,7 +1567,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="3">
-        <f>IF($A11="","",$A11-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F11" s="4">
@@ -1529,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E11,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1547,7 +1604,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="3">
-        <f>IF($A12="","",$A12-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F12" s="4">
@@ -1566,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E12,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1584,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="3">
-        <f>IF($A13="","",$A13-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F13" s="4">
@@ -1603,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E13,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1621,14 +1678,14 @@
         <v>27</v>
       </c>
       <c r="E14" s="3">
-        <f>IF($A14="","",$A14-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
@@ -1640,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E14,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1658,7 +1715,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="3">
-        <f>IF($A15="","",$A15-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F15" s="4">
@@ -1677,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E15,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1695,7 +1752,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="3">
-        <f>IF($A16="","",$A16-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F16" s="4">
@@ -1714,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E16,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1732,7 +1789,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="3">
-        <f>IF($A17="","",$A17-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F17" s="4">
@@ -1751,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E17,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1769,7 +1826,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="3">
-        <f>IF($A18="","",$A18-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F18" s="4">
@@ -1785,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E18,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1806,7 +1863,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="3">
-        <f>IF($A19="","",$A19-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F19" s="4">
@@ -1825,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E19,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1843,7 +1900,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="3">
-        <f>IF($A20="","",$A20-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F20" s="4">
@@ -1862,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E20,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1880,7 +1937,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="3">
-        <f>IF($A21="","",$A21-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F21" s="4">
@@ -1899,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E21,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1917,7 +1974,7 @@
         <v>43</v>
       </c>
       <c r="E22" s="3">
-        <f>IF($A22="","",$A22-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F22" s="4">
@@ -1936,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E22,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1954,7 +2011,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="3">
-        <f>IF($A23="","",$A23-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F23" s="4">
@@ -1973,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E23,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -1991,7 +2048,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="3">
-        <f>IF($A24="","",$A24-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F24" s="4">
@@ -2010,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E24,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2028,7 +2085,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="3">
-        <f>IF($A25="","",$A25-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F25" s="4">
@@ -2047,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E25,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2065,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="E26" s="3">
-        <f>IF($A26="","",$A26-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F26" s="4">
@@ -2084,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E26,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2102,7 +2159,7 @@
         <v>29</v>
       </c>
       <c r="E27" s="3">
-        <f>IF($A27="","",$A27-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F27" s="4">
@@ -2121,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E27,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2139,7 +2196,7 @@
         <v>47</v>
       </c>
       <c r="E28" s="3">
-        <f>IF($A28="","",$A28-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F28" s="4">
@@ -2158,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E28,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2176,26 +2233,26 @@
         <v>49</v>
       </c>
       <c r="E29" s="3">
-        <f>IF($A29="","",$A29-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
       </c>
       <c r="J29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E29,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2213,7 +2270,7 @@
         <v>24</v>
       </c>
       <c r="E30" s="3">
-        <f>IF($A30="","",$A30-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F30" s="4">
@@ -2232,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E30,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -2250,17 +2307,17 @@
         <v>21</v>
       </c>
       <c r="E31" s="3">
-        <f>IF($A31="","",$A31-1)</f>
+        <f t="shared" si="2"/>
         <v>45021</v>
       </c>
       <c r="F31" s="4">
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1">
         <v>1</v>
@@ -2269,21 +2326,1319 @@
         <v>0</v>
       </c>
       <c r="K31" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E31,"DD"))),0),"")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B32" s="6">
+        <v>6296</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="3">
+        <f>IF($A32="","",$A32-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E32,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B33" s="6">
+        <v>2193</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="3">
+        <f>IF($A33="","",$A33-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E33,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3107</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="3">
+        <f>IF($A34="","",$A34-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E34,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B35" s="6">
+        <v>5575</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="3">
+        <f>IF($A35="","",$A35-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E35,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B36" s="6">
+        <v>2383</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="3">
+        <f>IF($A36="","",$A36-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E36,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B37" s="6">
+        <v>9017</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="3">
+        <f>IF($A37="","",$A37-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E37,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B38" s="6">
+        <v>7330</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="3">
+        <f>IF($A38="","",$A38-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E38,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B39" s="6">
+        <v>2716</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="3">
+        <f>IF($A39="","",$A39-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E39,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B40" s="6">
+        <v>3089</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="3">
+        <f>IF($A40="","",$A40-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F40" s="4">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E40,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B41" s="6">
+        <v>8075</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="3">
+        <f>IF($A41="","",$A41-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F41" s="4">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E41,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B42" s="6">
+        <v>1330</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="3">
+        <f>IF($A42="","",$A42-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E42,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B43" s="6">
+        <v>751</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="3">
+        <f>IF($A43="","",$A43-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E43,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B44" s="6">
+        <v>4021</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="3">
+        <f>IF($A44="","",$A44-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E44,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B45" s="6">
+        <v>8510</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="3">
+        <f>IF($A45="","",$A45-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E45,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B46" s="6">
+        <v>4074</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="3">
+        <f>IF($A46="","",$A46-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E46,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B47" s="6">
+        <v>1082</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="3">
+        <f>IF($A47="","",$A47-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E47,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B48" s="6">
+        <v>9378</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="3">
+        <f>IF($A48="","",$A48-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E48,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B49" s="6">
+        <v>7607</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="3">
+        <f>IF($A49="","",$A49-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E49,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B50" s="6">
+        <v>9186</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="3">
+        <f>IF($A50="","",$A50-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E50,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B51" s="6">
+        <v>4612</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="3">
+        <f>IF($A51="","",$A51-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E51,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B52" s="6">
+        <v>9583</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" s="3">
+        <f>IF($A52="","",$A52-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E52,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B53" s="6">
+        <v>3389</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="3">
+        <f>IF($A53="","",$A53-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E53,"DD"))),0),"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B54" s="6">
+        <v>5279</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="3">
+        <f>IF($A54="","",$A54-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+      <c r="K54" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E54,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B55" s="6">
+        <v>3022</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="3">
+        <f>IF($A55="","",$A55-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F55" s="4">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>1</v>
+      </c>
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+      <c r="K55" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E55,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B56" s="6">
+        <v>3329</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="3">
+        <f>IF($A56="","",$A56-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
+      <c r="K56" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E56,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B57" s="6">
+        <v>8465</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="3">
+        <f>IF($A57="","",$A57-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+      <c r="K57" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E57,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B58" s="6">
+        <v>3755</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" s="3">
+        <f>IF($A58="","",$A58-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+      <c r="K58" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E58,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B59" s="6">
+        <v>8779</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="3">
+        <f>IF($A59="","",$A59-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E59,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B60" s="6">
+        <v>1174</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="3">
+        <f>IF($A60="","",$A60-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>1</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E60,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B61" s="6">
+        <v>8050</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" s="3">
+        <f>IF($A61="","",$A61-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E61,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B62" s="6">
+        <v>9167</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="3">
+        <f>IF($A62="","",$A62-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E62,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B63" s="6">
+        <v>1997</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E63" s="3">
+        <f>IF($A63="","",$A63-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E63,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B64" s="6">
+        <v>2444</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64" s="3">
+        <f>IF($A64="","",$A64-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E64,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B65" s="6">
+        <v>4326</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" s="3">
+        <f>IF($A65="","",$A65-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E65,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B66" s="6">
+        <v>7679</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="3">
+        <f>IF($A66="","",$A66-1)</f>
+        <v>45022</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1">
+        <v>1</v>
+      </c>
+      <c r="K66" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E66,"DD"))),0),"")</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J31" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J66" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B31" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B66" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
datos del dia 7-04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F7ACC-7600-4DFC-8831-1273EC80D605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009604B-81C5-48C9-9FC6-A139BED16FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="7740" yWindow="210" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="85">
   <si>
     <t>Usuario</t>
   </si>
@@ -519,6 +519,54 @@
   </si>
   <si>
     <t>Robo del Destino</t>
+  </si>
+  <si>
+    <t>Harpies</t>
+  </si>
+  <si>
+    <t>Última Voluntad de Arpías</t>
+  </si>
+  <si>
+    <t>CHV ft Salamangreat</t>
+  </si>
+  <si>
+    <t>Vampires</t>
+  </si>
+  <si>
+    <t>Ejército Póstumo</t>
+  </si>
+  <si>
+    <t>Triamids</t>
+  </si>
+  <si>
+    <t>Fish Armor</t>
+  </si>
+  <si>
+    <t>Gemelos Unidos</t>
+  </si>
+  <si>
+    <t>Meklord</t>
+  </si>
+  <si>
+    <t>Refinamiento Meklord</t>
+  </si>
+  <si>
+    <t>Fossil</t>
+  </si>
+  <si>
+    <t>Agujero de Gólem</t>
+  </si>
+  <si>
+    <t>Duelo Favorito</t>
+  </si>
+  <si>
+    <t>Mecanismos Medievales</t>
+  </si>
+  <si>
+    <t>7096</t>
+  </si>
+  <si>
+    <t>Satellarknights</t>
   </si>
 </sst>
 </file>
@@ -853,8 +901,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K66" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K66" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K99" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K99" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1173,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67:G70 H67:H71 G73 J67:J74 G77 H76:H81 H83 H85:H87 G88:G96 I67:I96 F78:F97 J76:J97 F98:G98 I98:J98 F99:I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,7 +2392,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="3">
-        <f>IF($A32="","",$A32-1)</f>
+        <f t="shared" ref="E32:E66" si="4">IF($A32="","",$A32-1)</f>
         <v>45022</v>
       </c>
       <c r="F32" s="4">
@@ -2363,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E32,"DD"))),0),"")</f>
+        <f t="shared" ref="K32:K66" si="5">IFERROR(ROUND((VALUE(TEXT($E32,"DD"))),0),"")</f>
         <v>6</v>
       </c>
     </row>
@@ -2381,7 +2429,7 @@
         <v>50</v>
       </c>
       <c r="E33" s="3">
-        <f>IF($A33="","",$A33-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F33" s="4">
@@ -2400,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E33,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2418,7 +2466,7 @@
         <v>43</v>
       </c>
       <c r="E34" s="3">
-        <f>IF($A34="","",$A34-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F34" s="4">
@@ -2437,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E34,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2455,7 +2503,7 @@
         <v>24</v>
       </c>
       <c r="E35" s="3">
-        <f>IF($A35="","",$A35-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F35" s="4">
@@ -2474,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E35,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2492,7 +2540,7 @@
         <v>29</v>
       </c>
       <c r="E36" s="3">
-        <f>IF($A36="","",$A36-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F36" s="4">
@@ -2511,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E36,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2529,7 +2577,7 @@
         <v>56</v>
       </c>
       <c r="E37" s="3">
-        <f>IF($A37="","",$A37-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F37" s="4">
@@ -2548,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E37,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2566,7 +2614,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="3">
-        <f>IF($A38="","",$A38-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F38" s="4">
@@ -2585,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E38,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2603,7 +2651,7 @@
         <v>53</v>
       </c>
       <c r="E39" s="3">
-        <f>IF($A39="","",$A39-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F39" s="4">
@@ -2622,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E39,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2640,7 +2688,7 @@
         <v>55</v>
       </c>
       <c r="E40" s="3">
-        <f>IF($A40="","",$A40-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F40" s="4">
@@ -2659,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E40,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2677,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="E41" s="3">
-        <f>IF($A41="","",$A41-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F41" s="4">
@@ -2696,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E41,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2714,7 +2762,7 @@
         <v>24</v>
       </c>
       <c r="E42" s="3">
-        <f>IF($A42="","",$A42-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F42" s="4">
@@ -2733,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E42,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2751,7 +2799,7 @@
         <v>56</v>
       </c>
       <c r="E43" s="3">
-        <f>IF($A43="","",$A43-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F43" s="4">
@@ -2770,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E43,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2788,7 +2836,7 @@
         <v>29</v>
       </c>
       <c r="E44" s="3">
-        <f>IF($A44="","",$A44-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F44" s="4">
@@ -2807,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E44,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2825,7 +2873,7 @@
         <v>27</v>
       </c>
       <c r="E45" s="3">
-        <f>IF($A45="","",$A45-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F45" s="4">
@@ -2844,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E45,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2862,7 +2910,7 @@
         <v>58</v>
       </c>
       <c r="E46" s="3">
-        <f>IF($A46="","",$A46-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F46" s="4">
@@ -2881,7 +2929,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E46,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2899,7 +2947,7 @@
         <v>29</v>
       </c>
       <c r="E47" s="3">
-        <f>IF($A47="","",$A47-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F47" s="4">
@@ -2918,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E47,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2936,7 +2984,7 @@
         <v>19</v>
       </c>
       <c r="E48" s="3">
-        <f>IF($A48="","",$A48-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F48" s="4">
@@ -2955,7 +3003,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E48,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -2973,7 +3021,7 @@
         <v>58</v>
       </c>
       <c r="E49" s="3">
-        <f>IF($A49="","",$A49-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F49" s="4">
@@ -2992,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E49,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3010,7 +3058,7 @@
         <v>29</v>
       </c>
       <c r="E50" s="3">
-        <f>IF($A50="","",$A50-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F50" s="4">
@@ -3029,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E50,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3047,7 +3095,7 @@
         <v>60</v>
       </c>
       <c r="E51" s="3">
-        <f>IF($A51="","",$A51-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F51" s="4">
@@ -3066,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E51,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3084,7 +3132,7 @@
         <v>62</v>
       </c>
       <c r="E52" s="3">
-        <f>IF($A52="","",$A52-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F52" s="4">
@@ -3103,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E52,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3121,7 +3169,7 @@
         <v>56</v>
       </c>
       <c r="E53" s="3">
-        <f>IF($A53="","",$A53-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F53" s="4">
@@ -3140,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E53,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3158,7 +3206,7 @@
         <v>21</v>
       </c>
       <c r="E54" s="3">
-        <f>IF($A54="","",$A54-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F54" s="4">
@@ -3177,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E54,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3195,17 +3243,17 @@
         <v>17</v>
       </c>
       <c r="E55" s="3">
-        <f>IF($A55="","",$A55-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F55" s="4">
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="1">
         <v>1</v>
@@ -3214,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="K55" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E55,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3232,17 +3280,17 @@
         <v>21</v>
       </c>
       <c r="E56" s="3">
-        <f>IF($A56="","",$A56-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F56" s="4">
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -3251,7 +3299,7 @@
         <v>1</v>
       </c>
       <c r="K56" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E56,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3269,14 +3317,14 @@
         <v>64</v>
       </c>
       <c r="E57" s="3">
-        <f>IF($A57="","",$A57-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F57" s="4">
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="1">
         <v>0</v>
@@ -3288,7 +3336,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E57,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3306,7 +3354,7 @@
         <v>53</v>
       </c>
       <c r="E58" s="3">
-        <f>IF($A58="","",$A58-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F58" s="4">
@@ -3325,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="K58" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E58,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3343,17 +3391,17 @@
         <v>24</v>
       </c>
       <c r="E59" s="3">
-        <f>IF($A59="","",$A59-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="1">
         <v>1</v>
@@ -3362,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E59,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3380,14 +3428,14 @@
         <v>24</v>
       </c>
       <c r="E60" s="3">
-        <f>IF($A60="","",$A60-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F60" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="1">
         <v>0</v>
@@ -3399,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E60,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3417,17 +3465,17 @@
         <v>66</v>
       </c>
       <c r="E61" s="3">
-        <f>IF($A61="","",$A61-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F61" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="1">
         <v>1</v>
@@ -3436,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E61,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3454,17 +3502,17 @@
         <v>58</v>
       </c>
       <c r="E62" s="3">
-        <f>IF($A62="","",$A62-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F62" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" s="1">
         <v>1</v>
@@ -3473,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="K62" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E62,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3491,7 +3539,7 @@
         <v>39</v>
       </c>
       <c r="E63" s="3">
-        <f>IF($A63="","",$A63-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F63" s="4">
@@ -3501,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="1">
         <v>1</v>
@@ -3510,7 +3558,7 @@
         <v>0</v>
       </c>
       <c r="K63" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E63,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3528,7 +3576,7 @@
         <v>58</v>
       </c>
       <c r="E64" s="3">
-        <f>IF($A64="","",$A64-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F64" s="4">
@@ -3547,7 +3595,7 @@
         <v>0</v>
       </c>
       <c r="K64" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E64,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3565,7 +3613,7 @@
         <v>39</v>
       </c>
       <c r="E65" s="3">
-        <f>IF($A65="","",$A65-1)</f>
+        <f t="shared" si="4"/>
         <v>45023</v>
       </c>
       <c r="F65" s="4">
@@ -3584,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="K65" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E65,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3602,7 +3650,7 @@
         <v>68</v>
       </c>
       <c r="E66" s="3">
-        <f>IF($A66="","",$A66-1)</f>
+        <f t="shared" si="4"/>
         <v>45022</v>
       </c>
       <c r="F66" s="4">
@@ -3621,23 +3669,1244 @@
         <v>1</v>
       </c>
       <c r="K66" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E66,"DD"))),0),"")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B67" s="6">
+        <v>3262</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="3">
+        <f>IF($A67="","",$A67-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F67" s="4">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E67,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B68" s="6">
+        <v>8052</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="3">
+        <f>IF($A68="","",$A68-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E68,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B69" s="6">
+        <v>3355</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" s="3">
+        <f>IF($A69="","",$A69-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0</v>
+      </c>
+      <c r="K69" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E69,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B70" s="6">
+        <v>9885</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="3">
+        <f>IF($A70="","",$A70-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F70" s="4">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E70,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B71" s="6">
+        <v>1894</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E71" s="3">
+        <f>IF($A71="","",$A71-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F71" s="4">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E71,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B72" s="6">
+        <v>803</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" s="3">
+        <f>IF($A72="","",$A72-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F72" s="4">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+      <c r="K72" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E72,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B73" s="6">
+        <v>6451</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="3">
+        <f>IF($A73="","",$A73-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F73" s="4">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E73,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B74" s="6">
+        <v>272</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" s="3">
+        <f>IF($A74="","",$A74-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F74" s="4">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0</v>
+      </c>
+      <c r="J74" s="1">
+        <v>0</v>
+      </c>
+      <c r="K74" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E74,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B75" s="6">
+        <v>2719</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E75" s="3">
+        <f>IF($A75="","",$A75-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0</v>
+      </c>
+      <c r="J75" s="1">
+        <v>1</v>
+      </c>
+      <c r="K75" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E75,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B76" s="6">
+        <v>5852</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E76" s="3">
+        <f>IF($A76="","",$A76-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0</v>
+      </c>
+      <c r="J76" s="1">
+        <v>0</v>
+      </c>
+      <c r="K76" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E76,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B77" s="6">
+        <v>2435</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="3">
+        <f>IF($A77="","",$A77-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F77" s="4">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
+      </c>
+      <c r="J77" s="1">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E77,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B78" s="6">
+        <v>7629</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78" s="3">
+        <f>IF($A78="","",$A78-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F78" s="4">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E78,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B79" s="6">
+        <v>5887</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" s="3">
+        <f>IF($A79="","",$A79-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F79" s="4">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E79,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B80" s="6">
+        <v>7270</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="3">
+        <f>IF($A80="","",$A80-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F80" s="4">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E80,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B81" s="6">
+        <v>3680</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="3">
+        <f>IF($A81="","",$A81-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>1</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0</v>
+      </c>
+      <c r="J81" s="1">
+        <v>0</v>
+      </c>
+      <c r="K81" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E81,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B82" s="6">
+        <v>246</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="3">
+        <f>IF($A82="","",$A82-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F82" s="4">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E82,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B83" s="6">
+        <v>3756</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" s="3">
+        <f>IF($A83="","",$A83-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F83" s="4">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+      <c r="K83" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E83,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B84" s="6">
+        <v>6631</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" s="3">
+        <f>IF($A84="","",$A84-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F84" s="4">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1</v>
+      </c>
+      <c r="H84" s="1">
+        <v>1</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+      <c r="K84" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E84,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B85" s="6">
+        <v>3059</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" s="3">
+        <f>IF($A85="","",$A85-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F85" s="4">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+      <c r="K85" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E85,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B86" s="6">
+        <v>7320</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" s="3">
+        <f>IF($A86="","",$A86-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F86" s="4">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0</v>
+      </c>
+      <c r="K86" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E86,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B87" s="6">
+        <v>1497</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="3">
+        <f>IF($A87="","",$A87-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F87" s="4">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E87,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B88" s="6">
+        <v>8875</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" s="3">
+        <f>IF($A88="","",$A88-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F88" s="4">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0</v>
+      </c>
+      <c r="K88" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E88,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B89" s="6">
+        <v>7116</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E89" s="3">
+        <f>IF($A89="","",$A89-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F89" s="4">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>1</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0</v>
+      </c>
+      <c r="K89" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E89,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B90" s="6">
+        <v>9524</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E90" s="3">
+        <f>IF($A90="","",$A90-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F90" s="4">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0</v>
+      </c>
+      <c r="H90" s="1">
+        <v>1</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E90,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B91" s="6">
+        <v>2303</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E91" s="3">
+        <f>IF($A91="","",$A91-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F91" s="4">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1">
+        <v>1</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1">
+        <v>0</v>
+      </c>
+      <c r="K91" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E91,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B92" s="6">
+        <v>9424</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E92" s="3">
+        <f>IF($A92="","",$A92-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F92" s="4">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>1</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0</v>
+      </c>
+      <c r="K92" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E92,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B93" s="6">
+        <v>7709</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E93" s="3">
+        <f>IF($A93="","",$A93-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F93" s="4">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>1</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1">
+        <v>0</v>
+      </c>
+      <c r="K93" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E93,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B94" s="6">
+        <v>3188</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E94" s="3">
+        <f>IF($A94="","",$A94-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F94" s="4">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>1</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0</v>
+      </c>
+      <c r="J94" s="1">
+        <v>0</v>
+      </c>
+      <c r="K94" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E94,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B95" s="6">
+        <v>5283</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="3">
+        <f>IF($A95="","",$A95-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F95" s="4">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+      <c r="H95" s="1">
+        <v>1</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0</v>
+      </c>
+      <c r="J95" s="1">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E95,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E96" s="3">
+        <f>IF($A96="","",$A96-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F96" s="4">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>1</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+      <c r="K96" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E96,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B97" s="6">
+        <v>6558</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E97" s="3">
+        <f>IF($A97="","",$A97-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F97" s="4">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>1</v>
+      </c>
+      <c r="H97" s="1">
+        <v>1</v>
+      </c>
+      <c r="I97" s="1">
+        <v>1</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0</v>
+      </c>
+      <c r="K97" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E97,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B98" s="6">
+        <v>5398</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="3">
+        <f>IF($A98="","",$A98-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F98" s="4">
+        <v>0</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0</v>
+      </c>
+      <c r="H98" s="1">
+        <v>1</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0</v>
+      </c>
+      <c r="K98" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E98,"DD"))),0),"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B99" s="6">
+        <v>8343</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E99" s="3">
+        <f>IF($A99="","",$A99-1)</f>
+        <v>45023</v>
+      </c>
+      <c r="F99" s="4">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1">
+        <v>1</v>
+      </c>
+      <c r="K99" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E99,"DD"))),0),"")</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J66" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J99" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B66" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B99" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
+    <ignoredError sqref="B2 B96" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
datos del dia 9-04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009604B-81C5-48C9-9FC6-A139BED16FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E19CE1-57B3-4765-979F-F87A7535A79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="210" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="1200" yWindow="330" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="114">
   <si>
     <t>Usuario</t>
   </si>
@@ -567,6 +567,93 @@
   </si>
   <si>
     <t>Satellarknights</t>
+  </si>
+  <si>
+    <t>Elementsabers Invoked</t>
+  </si>
+  <si>
+    <t>Tech Genus</t>
+  </si>
+  <si>
+    <t>Listos Aceleración Delta</t>
+  </si>
+  <si>
+    <t>Refinamiendo Meklord</t>
+  </si>
+  <si>
+    <t>Potenciador de Péndulo</t>
+  </si>
+  <si>
+    <t>Malefic</t>
+  </si>
+  <si>
+    <t>Mundo Repleto de Malicia</t>
+  </si>
+  <si>
+    <t>Conjuros de Rosas</t>
+  </si>
+  <si>
+    <t>Destiny Heros</t>
+  </si>
+  <si>
+    <t>Reloj del Destino</t>
+  </si>
+  <si>
+    <t>Fish Shark</t>
+  </si>
+  <si>
+    <t>El alzamiento de Shark</t>
+  </si>
+  <si>
+    <t>Crusadia</t>
+  </si>
+  <si>
+    <t>Movimiento de Monstruo</t>
+  </si>
+  <si>
+    <t>Guardia Bendita</t>
+  </si>
+  <si>
+    <t>5814</t>
+  </si>
+  <si>
+    <t>Pendulum Magician</t>
+  </si>
+  <si>
+    <t>El Héroe Deslumbrará con su Luz</t>
+  </si>
+  <si>
+    <t>Megalith</t>
+  </si>
+  <si>
+    <t>Maestro de los Rituales Duplicar Nivel</t>
+  </si>
+  <si>
+    <t>Crystrons</t>
+  </si>
+  <si>
+    <t>Habilidad no asignada</t>
+  </si>
+  <si>
+    <t>Lunalight</t>
+  </si>
+  <si>
+    <t>Six Samurais</t>
+  </si>
+  <si>
+    <t>Dinomist</t>
+  </si>
+  <si>
+    <t>Con Valor</t>
+  </si>
+  <si>
+    <t>Maestro de Rituales II</t>
+  </si>
+  <si>
+    <t>Hora de una Fusión</t>
+  </si>
+  <si>
+    <t>Pasa a la acción Invocación por Péndulo</t>
   </si>
 </sst>
 </file>
@@ -901,8 +988,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K99" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K99" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K166" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K166" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1221,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67:G70 H67:H71 G73 J67:J74 G77 H76:H81 H83 H85:H87 G88:G96 I67:I96 F78:F97 J76:J97 F98:G98 I98:J98 F99:I99"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,7 +2745,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
@@ -3687,7 +3774,7 @@
         <v>29</v>
       </c>
       <c r="E67" s="3">
-        <f>IF($A67="","",$A67-1)</f>
+        <f t="shared" ref="E67:E99" si="6">IF($A67="","",$A67-1)</f>
         <v>45023</v>
       </c>
       <c r="F67" s="4">
@@ -3706,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="K67" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E67,"DD"))),0),"")</f>
+        <f t="shared" ref="K67:K99" si="7">IFERROR(ROUND((VALUE(TEXT($E67,"DD"))),0),"")</f>
         <v>7</v>
       </c>
     </row>
@@ -3724,7 +3811,7 @@
         <v>70</v>
       </c>
       <c r="E68" s="3">
-        <f>IF($A68="","",$A68-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F68" s="4">
@@ -3743,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="K68" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E68,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3761,7 +3848,7 @@
         <v>50</v>
       </c>
       <c r="E69" s="3">
-        <f>IF($A69="","",$A69-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F69" s="4">
@@ -3780,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="K69" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E69,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3798,7 +3885,7 @@
         <v>21</v>
       </c>
       <c r="E70" s="3">
-        <f>IF($A70="","",$A70-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F70" s="4">
@@ -3817,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="K70" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E70,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3835,7 +3922,7 @@
         <v>55</v>
       </c>
       <c r="E71" s="3">
-        <f>IF($A71="","",$A71-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F71" s="4">
@@ -3854,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E71,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3872,7 +3959,7 @@
         <v>64</v>
       </c>
       <c r="E72" s="3">
-        <f>IF($A72="","",$A72-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F72" s="4">
@@ -3891,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="K72" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E72,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3909,7 +3996,7 @@
         <v>71</v>
       </c>
       <c r="E73" s="3">
-        <f>IF($A73="","",$A73-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F73" s="4">
@@ -3928,7 +4015,7 @@
         <v>0</v>
       </c>
       <c r="K73" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E73,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3946,7 +4033,7 @@
         <v>73</v>
       </c>
       <c r="E74" s="3">
-        <f>IF($A74="","",$A74-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F74" s="4">
@@ -3965,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="K74" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E74,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -3983,7 +4070,7 @@
         <v>23</v>
       </c>
       <c r="E75" s="3">
-        <f>IF($A75="","",$A75-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F75" s="4">
@@ -4002,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="K75" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E75,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4020,7 +4107,7 @@
         <v>45</v>
       </c>
       <c r="E76" s="3">
-        <f>IF($A76="","",$A76-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F76" s="4">
@@ -4039,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="K76" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E76,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4057,7 +4144,7 @@
         <v>76</v>
       </c>
       <c r="E77" s="3">
-        <f>IF($A77="","",$A77-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F77" s="4">
@@ -4076,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E77,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4094,7 +4181,7 @@
         <v>78</v>
       </c>
       <c r="E78" s="3">
-        <f>IF($A78="","",$A78-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F78" s="4">
@@ -4113,7 +4200,7 @@
         <v>0</v>
       </c>
       <c r="K78" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E78,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4131,7 +4218,7 @@
         <v>80</v>
       </c>
       <c r="E79" s="3">
-        <f>IF($A79="","",$A79-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F79" s="4">
@@ -4150,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="K79" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E79,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4168,7 +4255,7 @@
         <v>23</v>
       </c>
       <c r="E80" s="3">
-        <f>IF($A80="","",$A80-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F80" s="4">
@@ -4187,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E80,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4205,7 +4292,7 @@
         <v>45</v>
       </c>
       <c r="E81" s="3">
-        <f>IF($A81="","",$A81-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F81" s="4">
@@ -4224,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="K81" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E81,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4242,7 +4329,7 @@
         <v>13</v>
       </c>
       <c r="E82" s="3">
-        <f>IF($A82="","",$A82-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F82" s="4">
@@ -4261,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="K82" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E82,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4279,7 +4366,7 @@
         <v>56</v>
       </c>
       <c r="E83" s="3">
-        <f>IF($A83="","",$A83-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F83" s="4">
@@ -4298,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E83,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4316,7 +4403,7 @@
         <v>60</v>
       </c>
       <c r="E84" s="3">
-        <f>IF($A84="","",$A84-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F84" s="4">
@@ -4335,7 +4422,7 @@
         <v>0</v>
       </c>
       <c r="K84" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E84,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4353,7 +4440,7 @@
         <v>24</v>
       </c>
       <c r="E85" s="3">
-        <f>IF($A85="","",$A85-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F85" s="4">
@@ -4372,7 +4459,7 @@
         <v>0</v>
       </c>
       <c r="K85" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E85,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4390,7 +4477,7 @@
         <v>31</v>
       </c>
       <c r="E86" s="3">
-        <f>IF($A86="","",$A86-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F86" s="4">
@@ -4409,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="K86" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E86,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4427,7 +4514,7 @@
         <v>19</v>
       </c>
       <c r="E87" s="3">
-        <f>IF($A87="","",$A87-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F87" s="4">
@@ -4446,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="K87" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E87,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4464,7 +4551,7 @@
         <v>81</v>
       </c>
       <c r="E88" s="3">
-        <f>IF($A88="","",$A88-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F88" s="4">
@@ -4483,7 +4570,7 @@
         <v>0</v>
       </c>
       <c r="K88" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E88,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4501,7 +4588,7 @@
         <v>71</v>
       </c>
       <c r="E89" s="3">
-        <f>IF($A89="","",$A89-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F89" s="4">
@@ -4520,7 +4607,7 @@
         <v>0</v>
       </c>
       <c r="K89" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E89,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4538,7 +4625,7 @@
         <v>45</v>
       </c>
       <c r="E90" s="3">
-        <f>IF($A90="","",$A90-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F90" s="4">
@@ -4557,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="K90" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E90,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4575,7 +4662,7 @@
         <v>58</v>
       </c>
       <c r="E91" s="3">
-        <f>IF($A91="","",$A91-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F91" s="4">
@@ -4594,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="K91" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E91,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4612,7 +4699,7 @@
         <v>58</v>
       </c>
       <c r="E92" s="3">
-        <f>IF($A92="","",$A92-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F92" s="4">
@@ -4631,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="K92" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E92,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4649,7 +4736,7 @@
         <v>58</v>
       </c>
       <c r="E93" s="3">
-        <f>IF($A93="","",$A93-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F93" s="4">
@@ -4668,7 +4755,7 @@
         <v>0</v>
       </c>
       <c r="K93" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E93,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4686,7 +4773,7 @@
         <v>82</v>
       </c>
       <c r="E94" s="3">
-        <f>IF($A94="","",$A94-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F94" s="4">
@@ -4705,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="K94" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E94,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4723,7 +4810,7 @@
         <v>13</v>
       </c>
       <c r="E95" s="3">
-        <f>IF($A95="","",$A95-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F95" s="4">
@@ -4742,7 +4829,7 @@
         <v>0</v>
       </c>
       <c r="K95" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E95,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4760,7 +4847,7 @@
         <v>45</v>
       </c>
       <c r="E96" s="3">
-        <f>IF($A96="","",$A96-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F96" s="4">
@@ -4779,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="K96" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E96,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4797,7 +4884,7 @@
         <v>62</v>
       </c>
       <c r="E97" s="3">
-        <f>IF($A97="","",$A97-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F97" s="4">
@@ -4816,7 +4903,7 @@
         <v>0</v>
       </c>
       <c r="K97" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E97,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4834,7 +4921,7 @@
         <v>31</v>
       </c>
       <c r="E98" s="3">
-        <f>IF($A98="","",$A98-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F98" s="4">
@@ -4853,7 +4940,7 @@
         <v>0</v>
       </c>
       <c r="K98" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E98,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -4871,7 +4958,7 @@
         <v>66</v>
       </c>
       <c r="E99" s="3">
-        <f>IF($A99="","",$A99-1)</f>
+        <f t="shared" si="6"/>
         <v>45023</v>
       </c>
       <c r="F99" s="4">
@@ -4890,23 +4977,2502 @@
         <v>1</v>
       </c>
       <c r="K99" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E99,"DD"))),0),"")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B100" s="6">
+        <v>294</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E100" s="3">
+        <f>IF($A100="","",$A100-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F100" s="4">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0</v>
+      </c>
+      <c r="K100" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E100,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B101" s="6">
+        <v>8246</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E101" s="3">
+        <f>IF($A101="","",$A101-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F101" s="4">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1">
+        <v>1</v>
+      </c>
+      <c r="J101" s="1">
+        <v>0</v>
+      </c>
+      <c r="K101" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E101,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B102" s="6">
+        <v>5681</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E102" s="3">
+        <f>IF($A102="","",$A102-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F102" s="4">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E102,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B103" s="6">
+        <v>2328</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" s="3">
+        <f>IF($A103="","",$A103-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F103" s="4">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E103,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B104" s="6">
+        <v>4774</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E104" s="3">
+        <f>IF($A104="","",$A104-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F104" s="4">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0</v>
+      </c>
+      <c r="I104" s="1">
+        <v>1</v>
+      </c>
+      <c r="J104" s="1">
+        <v>1</v>
+      </c>
+      <c r="K104" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E104,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B105" s="6">
+        <v>6275</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E105" s="3">
+        <f>IF($A105="","",$A105-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F105" s="4">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0</v>
+      </c>
+      <c r="H105" s="1">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0</v>
+      </c>
+      <c r="K105" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E105,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B106" s="6">
+        <v>4537</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" s="3">
+        <f>IF($A106="","",$A106-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F106" s="4">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E106,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B107" s="6">
+        <v>8298</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E107" s="3">
+        <f>IF($A107="","",$A107-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F107" s="4">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0</v>
+      </c>
+      <c r="K107" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E107,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B108" s="6">
+        <v>3086</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E108" s="3">
+        <f>IF($A108="","",$A108-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F108" s="4">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0</v>
+      </c>
+      <c r="H108" s="1">
+        <v>0</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0</v>
+      </c>
+      <c r="K108" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E108,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B109" s="6">
+        <v>5294</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E109" s="3">
+        <f>IF($A109="","",$A109-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F109" s="4">
+        <v>1</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0</v>
+      </c>
+      <c r="H109" s="1">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1">
+        <v>0</v>
+      </c>
+      <c r="J109" s="1">
+        <v>0</v>
+      </c>
+      <c r="K109" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E109,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B110" s="6">
+        <v>5952</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="3">
+        <f>IF($A110="","",$A110-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F110" s="4">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="H110" s="1">
+        <v>1</v>
+      </c>
+      <c r="I110" s="1">
+        <v>1</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E110,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B111" s="6">
+        <v>9540</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E111" s="3">
+        <f>IF($A111="","",$A111-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F111" s="4">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1</v>
+      </c>
+      <c r="H111" s="1">
+        <v>1</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0</v>
+      </c>
+      <c r="K111" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E111,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B112" s="6">
+        <v>8188</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E112" s="3">
+        <f>IF($A112="","",$A112-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F112" s="4">
+        <v>1</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1">
+        <v>1</v>
+      </c>
+      <c r="J112" s="1">
+        <v>0</v>
+      </c>
+      <c r="K112" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E112,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B113" s="6">
+        <v>869</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E113" s="3">
+        <f>IF($A113="","",$A113-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F113" s="4">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1">
+        <v>0</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0</v>
+      </c>
+      <c r="K113" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E113,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B114" s="6">
+        <v>1023</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="3">
+        <f>IF($A114="","",$A114-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F114" s="4">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1">
+        <v>0</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0</v>
+      </c>
+      <c r="K114" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E114,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B115" s="6">
+        <v>7322</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E115" s="3">
+        <f>IF($A115="","",$A115-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F115" s="4">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1</v>
+      </c>
+      <c r="H115" s="1">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1">
+        <v>1</v>
+      </c>
+      <c r="J115" s="1">
+        <v>0</v>
+      </c>
+      <c r="K115" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E115,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B116" s="6">
+        <v>7373</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E116" s="3">
+        <f>IF($A116="","",$A116-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F116" s="4">
+        <v>1</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0</v>
+      </c>
+      <c r="H116" s="1">
+        <v>1</v>
+      </c>
+      <c r="I116" s="1">
+        <v>0</v>
+      </c>
+      <c r="J116" s="1">
+        <v>0</v>
+      </c>
+      <c r="K116" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E116,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B117" s="6">
+        <v>6821</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E117" s="3">
+        <f>IF($A117="","",$A117-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F117" s="4">
+        <v>1</v>
+      </c>
+      <c r="G117" s="1">
+        <v>0</v>
+      </c>
+      <c r="H117" s="1">
+        <v>1</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0</v>
+      </c>
+      <c r="J117" s="1">
+        <v>0</v>
+      </c>
+      <c r="K117" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E117,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B118" s="6">
+        <v>3655</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E118" s="3">
+        <f>IF($A118="","",$A118-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F118" s="4">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1">
+        <v>0</v>
+      </c>
+      <c r="H118" s="1">
+        <v>1</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0</v>
+      </c>
+      <c r="K118" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E118,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B119" s="6">
+        <v>1411</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E119" s="3">
+        <f>IF($A119="","",$A119-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F119" s="4">
+        <v>1</v>
+      </c>
+      <c r="G119" s="1">
+        <v>0</v>
+      </c>
+      <c r="H119" s="1">
+        <v>1</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
+        <v>1</v>
+      </c>
+      <c r="K119" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E119,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B120" s="6">
+        <v>7475</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E120" s="3">
+        <f>IF($A120="","",$A120-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F120" s="4">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1">
+        <v>0</v>
+      </c>
+      <c r="H120" s="1">
+        <v>1</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0</v>
+      </c>
+      <c r="K120" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E120,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B121" s="6">
+        <v>8838</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E121" s="3">
+        <f>IF($A121="","",$A121-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F121" s="4">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0</v>
+      </c>
+      <c r="H121" s="1">
+        <v>0</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0</v>
+      </c>
+      <c r="K121" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E121,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B122" s="6">
+        <v>5189</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E122" s="3">
+        <f>IF($A122="","",$A122-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F122" s="4">
+        <v>1</v>
+      </c>
+      <c r="G122" s="1">
+        <v>0</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0</v>
+      </c>
+      <c r="K122" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E122,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B123" s="6">
+        <v>1513</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E123" s="3">
+        <f>IF($A123="","",$A123-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F123" s="4">
+        <v>1</v>
+      </c>
+      <c r="G123" s="1">
+        <v>0</v>
+      </c>
+      <c r="H123" s="1">
+        <v>0</v>
+      </c>
+      <c r="I123" s="1">
+        <v>1</v>
+      </c>
+      <c r="J123" s="1">
+        <v>0</v>
+      </c>
+      <c r="K123" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E123,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B124" s="6">
+        <v>5817</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E124" s="3">
+        <f>IF($A124="","",$A124-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F124" s="4">
+        <v>1</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0</v>
+      </c>
+      <c r="H124" s="1">
+        <v>0</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1">
+        <v>0</v>
+      </c>
+      <c r="K124" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E124,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B125" s="6">
+        <v>4920</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E125" s="3">
+        <f>IF($A125="","",$A125-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F125" s="4">
+        <v>0</v>
+      </c>
+      <c r="G125" s="1">
+        <v>1</v>
+      </c>
+      <c r="H125" s="1">
+        <v>0</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0</v>
+      </c>
+      <c r="J125" s="1">
+        <v>0</v>
+      </c>
+      <c r="K125" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E125,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B126" s="6">
+        <v>4266</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E126" s="3">
+        <f>IF($A126="","",$A126-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F126" s="4">
+        <v>0</v>
+      </c>
+      <c r="G126" s="1">
+        <v>1</v>
+      </c>
+      <c r="H126" s="1">
+        <v>0</v>
+      </c>
+      <c r="I126" s="1">
+        <v>0</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0</v>
+      </c>
+      <c r="K126" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E126,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B127" s="6">
+        <v>4476</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E127" s="3">
+        <f>IF($A127="","",$A127-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F127" s="4">
+        <v>0</v>
+      </c>
+      <c r="G127" s="1">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1">
+        <v>0</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0</v>
+      </c>
+      <c r="K127" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E127,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B128" s="6">
+        <v>4618</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E128" s="3">
+        <f>IF($A128="","",$A128-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F128" s="4">
+        <v>0</v>
+      </c>
+      <c r="G128" s="1">
+        <v>1</v>
+      </c>
+      <c r="H128" s="1">
+        <v>0</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0</v>
+      </c>
+      <c r="J128" s="1">
+        <v>0</v>
+      </c>
+      <c r="K128" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E128,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B129" s="6">
+        <v>2707</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E129" s="3">
+        <f>IF($A129="","",$A129-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F129" s="4">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1">
+        <v>1</v>
+      </c>
+      <c r="H129" s="1">
+        <v>0</v>
+      </c>
+      <c r="I129" s="1">
+        <v>0</v>
+      </c>
+      <c r="J129" s="1">
+        <v>0</v>
+      </c>
+      <c r="K129" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E129,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B130" s="6">
+        <v>77</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E130" s="3">
+        <f>IF($A130="","",$A130-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F130" s="4">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1">
+        <v>1</v>
+      </c>
+      <c r="H130" s="1">
+        <v>0</v>
+      </c>
+      <c r="I130" s="1">
+        <v>0</v>
+      </c>
+      <c r="J130" s="1">
+        <v>0</v>
+      </c>
+      <c r="K130" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E130,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B131" s="6">
+        <v>7407</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E131" s="3">
+        <f>IF($A131="","",$A131-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F131" s="4">
+        <v>0</v>
+      </c>
+      <c r="G131" s="1">
+        <v>1</v>
+      </c>
+      <c r="H131" s="1">
+        <v>0</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0</v>
+      </c>
+      <c r="J131" s="1">
+        <v>1</v>
+      </c>
+      <c r="K131" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E131,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B132" s="6">
+        <v>2420</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E132" s="3">
+        <f>IF($A132="","",$A132-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F132" s="4">
+        <v>0</v>
+      </c>
+      <c r="G132" s="1">
+        <v>1</v>
+      </c>
+      <c r="H132" s="1">
+        <v>0</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0</v>
+      </c>
+      <c r="J132" s="1">
+        <v>0</v>
+      </c>
+      <c r="K132" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E132,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B133" s="6">
+        <v>8820</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E133" s="3">
+        <f>IF($A133="","",$A133-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F133" s="4">
+        <v>0</v>
+      </c>
+      <c r="G133" s="1">
+        <v>1</v>
+      </c>
+      <c r="H133" s="1">
+        <v>0</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0</v>
+      </c>
+      <c r="J133" s="1">
+        <v>1</v>
+      </c>
+      <c r="K133" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E133,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B134" s="6">
+        <v>9516</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E134" s="3">
+        <f>IF($A134="","",$A134-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F134" s="4">
+        <v>0</v>
+      </c>
+      <c r="G134" s="1">
+        <v>1</v>
+      </c>
+      <c r="H134" s="1">
+        <v>0</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0</v>
+      </c>
+      <c r="K134" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E134,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B135" s="6">
+        <v>3721</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E135" s="3">
+        <f>IF($A135="","",$A135-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F135" s="4">
+        <v>0</v>
+      </c>
+      <c r="G135" s="1">
+        <v>1</v>
+      </c>
+      <c r="H135" s="1">
+        <v>0</v>
+      </c>
+      <c r="I135" s="1">
+        <v>0</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0</v>
+      </c>
+      <c r="K135" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E135,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B136" s="6">
+        <v>2619</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E136" s="3">
+        <f>IF($A136="","",$A136-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F136" s="4">
+        <v>0</v>
+      </c>
+      <c r="G136" s="1">
+        <v>1</v>
+      </c>
+      <c r="H136" s="1">
+        <v>0</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0</v>
+      </c>
+      <c r="J136" s="1">
+        <v>0</v>
+      </c>
+      <c r="K136" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E136,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B137" s="6">
+        <v>1553</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E137" s="3">
+        <f>IF($A137="","",$A137-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F137" s="4">
+        <v>0</v>
+      </c>
+      <c r="G137" s="1">
+        <v>1</v>
+      </c>
+      <c r="H137" s="1">
+        <v>1</v>
+      </c>
+      <c r="I137" s="1">
+        <v>1</v>
+      </c>
+      <c r="J137" s="1">
+        <v>1</v>
+      </c>
+      <c r="K137" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E137,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E138" s="3">
+        <f>IF($A138="","",$A138-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F138" s="4">
+        <v>0</v>
+      </c>
+      <c r="G138" s="1">
+        <v>1</v>
+      </c>
+      <c r="H138" s="1">
+        <v>0</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1">
+        <v>1</v>
+      </c>
+      <c r="K138" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E138,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B139" s="6">
+        <v>196</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E139" s="3">
+        <f>IF($A139="","",$A139-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F139" s="4">
+        <v>0</v>
+      </c>
+      <c r="G139" s="1">
+        <v>1</v>
+      </c>
+      <c r="H139" s="1">
+        <v>0</v>
+      </c>
+      <c r="I139" s="1">
+        <v>0</v>
+      </c>
+      <c r="J139" s="1">
+        <v>0</v>
+      </c>
+      <c r="K139" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E139,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B140" s="6">
+        <v>6504</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E140" s="3">
+        <f>IF($A140="","",$A140-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F140" s="4">
+        <v>0</v>
+      </c>
+      <c r="G140" s="1">
+        <v>1</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1">
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>1</v>
+      </c>
+      <c r="K140" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E140,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B141" s="6">
+        <v>8911</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E141" s="3">
+        <f>IF($A141="","",$A141-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F141" s="4">
+        <v>0</v>
+      </c>
+      <c r="G141" s="1">
+        <v>1</v>
+      </c>
+      <c r="H141" s="1">
+        <v>0</v>
+      </c>
+      <c r="I141" s="1">
+        <v>0</v>
+      </c>
+      <c r="J141" s="1">
+        <v>0</v>
+      </c>
+      <c r="K141" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E141,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B142" s="6">
+        <v>9515</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E142" s="3">
+        <f>IF($A142="","",$A142-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F142" s="4">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1">
+        <v>1</v>
+      </c>
+      <c r="H142" s="1">
+        <v>0</v>
+      </c>
+      <c r="I142" s="1">
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
+        <v>0</v>
+      </c>
+      <c r="K142" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E142,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B143" s="6">
+        <v>3392</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E143" s="3">
+        <f>IF($A143="","",$A143-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F143" s="4">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1">
+        <v>0</v>
+      </c>
+      <c r="H143" s="1">
+        <v>1</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0</v>
+      </c>
+      <c r="J143" s="1">
+        <v>0</v>
+      </c>
+      <c r="K143" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E143,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B144" s="6">
+        <v>701</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E144" s="3">
+        <f>IF($A144="","",$A144-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F144" s="4">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1">
+        <v>0</v>
+      </c>
+      <c r="H144" s="1">
+        <v>1</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0</v>
+      </c>
+      <c r="J144" s="1">
+        <v>0</v>
+      </c>
+      <c r="K144" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E144,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B145" s="6">
+        <v>6895</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E145" s="3">
+        <f>IF($A145="","",$A145-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F145" s="4">
+        <v>0</v>
+      </c>
+      <c r="G145" s="1">
+        <v>0</v>
+      </c>
+      <c r="H145" s="1">
+        <v>1</v>
+      </c>
+      <c r="I145" s="1">
+        <v>0</v>
+      </c>
+      <c r="J145" s="1">
+        <v>0</v>
+      </c>
+      <c r="K145" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E145,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B146" s="6">
+        <v>9025</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E146" s="3">
+        <f>IF($A146="","",$A146-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F146" s="4">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+      <c r="H146" s="1">
+        <v>1</v>
+      </c>
+      <c r="I146" s="1">
+        <v>0</v>
+      </c>
+      <c r="J146" s="1">
+        <v>0</v>
+      </c>
+      <c r="K146" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E146,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B147" s="6">
+        <v>4682</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E147" s="3">
+        <f>IF($A147="","",$A147-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F147" s="4">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1">
+        <v>0</v>
+      </c>
+      <c r="H147" s="1">
+        <v>1</v>
+      </c>
+      <c r="I147" s="1">
+        <v>0</v>
+      </c>
+      <c r="J147" s="1">
+        <v>0</v>
+      </c>
+      <c r="K147" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E147,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B148" s="6">
+        <v>8859</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E148" s="3">
+        <f>IF($A148="","",$A148-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F148" s="4">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1">
+        <v>0</v>
+      </c>
+      <c r="H148" s="1">
+        <v>1</v>
+      </c>
+      <c r="I148" s="1">
+        <v>0</v>
+      </c>
+      <c r="J148" s="1">
+        <v>1</v>
+      </c>
+      <c r="K148" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E148,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B149" s="6">
+        <v>2267</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E149" s="3">
+        <f>IF($A149="","",$A149-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F149" s="4">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+      <c r="H149" s="1">
+        <v>1</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0</v>
+      </c>
+      <c r="J149" s="1">
+        <v>0</v>
+      </c>
+      <c r="K149" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E149,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B150" s="6">
+        <v>9878</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E150" s="3">
+        <f>IF($A150="","",$A150-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F150" s="4">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0</v>
+      </c>
+      <c r="H150" s="1">
+        <v>1</v>
+      </c>
+      <c r="I150" s="1">
+        <v>0</v>
+      </c>
+      <c r="J150" s="1">
+        <v>0</v>
+      </c>
+      <c r="K150" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E150,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B151" s="6">
+        <v>935</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E151" s="3">
+        <f>IF($A151="","",$A151-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F151" s="4">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0</v>
+      </c>
+      <c r="H151" s="1">
+        <v>1</v>
+      </c>
+      <c r="I151" s="1">
+        <v>0</v>
+      </c>
+      <c r="J151" s="1">
+        <v>0</v>
+      </c>
+      <c r="K151" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E151,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B152" s="6">
+        <v>8869</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E152" s="3">
+        <f>IF($A152="","",$A152-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F152" s="4">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1">
+        <v>0</v>
+      </c>
+      <c r="H152" s="1">
+        <v>1</v>
+      </c>
+      <c r="I152" s="1">
+        <v>0</v>
+      </c>
+      <c r="J152" s="1">
+        <v>0</v>
+      </c>
+      <c r="K152" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E152,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B153" s="6">
+        <v>3809</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E153" s="3">
+        <f>IF($A153="","",$A153-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F153" s="4">
+        <v>0</v>
+      </c>
+      <c r="G153" s="1">
+        <v>0</v>
+      </c>
+      <c r="H153" s="1">
+        <v>1</v>
+      </c>
+      <c r="I153" s="1">
+        <v>0</v>
+      </c>
+      <c r="J153" s="1">
+        <v>0</v>
+      </c>
+      <c r="K153" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E153,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B154" s="6">
+        <v>8727</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E154" s="3">
+        <f>IF($A154="","",$A154-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F154" s="4">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1">
+        <v>0</v>
+      </c>
+      <c r="H154" s="1">
+        <v>1</v>
+      </c>
+      <c r="I154" s="1">
+        <v>0</v>
+      </c>
+      <c r="J154" s="1">
+        <v>0</v>
+      </c>
+      <c r="K154" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E154,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B155" s="6">
+        <v>6216</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E155" s="3">
+        <f>IF($A155="","",$A155-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F155" s="4">
+        <v>0</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0</v>
+      </c>
+      <c r="H155" s="1">
+        <v>1</v>
+      </c>
+      <c r="I155" s="1">
+        <v>0</v>
+      </c>
+      <c r="J155" s="1">
+        <v>0</v>
+      </c>
+      <c r="K155" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E155,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B156" s="6">
+        <v>3207</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E156" s="3">
+        <f>IF($A156="","",$A156-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F156" s="4">
+        <v>0</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0</v>
+      </c>
+      <c r="H156" s="1">
+        <v>1</v>
+      </c>
+      <c r="I156" s="1">
+        <v>0</v>
+      </c>
+      <c r="J156" s="1">
+        <v>0</v>
+      </c>
+      <c r="K156" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E156,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B157" s="6">
+        <v>1538</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E157" s="3">
+        <f>IF($A157="","",$A157-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F157" s="4">
+        <v>0</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0</v>
+      </c>
+      <c r="H157" s="1">
+        <v>1</v>
+      </c>
+      <c r="I157" s="1">
+        <v>0</v>
+      </c>
+      <c r="J157" s="1">
+        <v>0</v>
+      </c>
+      <c r="K157" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E157,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B158" s="6">
+        <v>3842</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E158" s="3">
+        <f>IF($A158="","",$A158-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F158" s="4">
+        <v>0</v>
+      </c>
+      <c r="G158" s="1">
+        <v>0</v>
+      </c>
+      <c r="H158" s="1">
+        <v>1</v>
+      </c>
+      <c r="I158" s="1">
+        <v>0</v>
+      </c>
+      <c r="J158" s="1">
+        <v>0</v>
+      </c>
+      <c r="K158" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E158,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B159" s="6">
+        <v>7429</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E159" s="3">
+        <f>IF($A159="","",$A159-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F159" s="4">
+        <v>0</v>
+      </c>
+      <c r="G159" s="1">
+        <v>0</v>
+      </c>
+      <c r="H159" s="1">
+        <v>1</v>
+      </c>
+      <c r="I159" s="1">
+        <v>0</v>
+      </c>
+      <c r="J159" s="1">
+        <v>0</v>
+      </c>
+      <c r="K159" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E159,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B160" s="6">
+        <v>9765</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E160" s="3">
+        <f>IF($A160="","",$A160-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F160" s="4">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0</v>
+      </c>
+      <c r="H160" s="1">
+        <v>1</v>
+      </c>
+      <c r="I160" s="1">
+        <v>0</v>
+      </c>
+      <c r="J160" s="1">
+        <v>0</v>
+      </c>
+      <c r="K160" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E160,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B161" s="6">
+        <v>6289</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E161" s="3">
+        <f>IF($A161="","",$A161-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F161" s="4">
+        <v>0</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0</v>
+      </c>
+      <c r="H161" s="1">
+        <v>1</v>
+      </c>
+      <c r="I161" s="1">
+        <v>0</v>
+      </c>
+      <c r="J161" s="1">
+        <v>0</v>
+      </c>
+      <c r="K161" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E161,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B162" s="6">
+        <v>3129</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E162" s="3">
+        <f>IF($A162="","",$A162-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F162" s="4">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1">
+        <v>0</v>
+      </c>
+      <c r="H162" s="1">
+        <v>1</v>
+      </c>
+      <c r="I162" s="1">
+        <v>0</v>
+      </c>
+      <c r="J162" s="1">
+        <v>0</v>
+      </c>
+      <c r="K162" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E162,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B163" s="6">
+        <v>4557</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E163" s="3">
+        <f>IF($A163="","",$A163-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F163" s="4">
+        <v>0</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0</v>
+      </c>
+      <c r="H163" s="1">
+        <v>1</v>
+      </c>
+      <c r="I163" s="1">
+        <v>0</v>
+      </c>
+      <c r="J163" s="1">
+        <v>0</v>
+      </c>
+      <c r="K163" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E163,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B164" s="6">
+        <v>1132</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E164" s="3">
+        <f>IF($A164="","",$A164-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F164" s="4">
+        <v>0</v>
+      </c>
+      <c r="G164" s="1">
+        <v>0</v>
+      </c>
+      <c r="H164" s="1">
+        <v>0</v>
+      </c>
+      <c r="I164" s="1">
+        <v>0</v>
+      </c>
+      <c r="J164" s="1">
+        <v>1</v>
+      </c>
+      <c r="K164" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E164,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B165" s="6">
+        <v>4556</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E165" s="3">
+        <f>IF($A165="","",$A165-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F165" s="4">
+        <v>0</v>
+      </c>
+      <c r="G165" s="1">
+        <v>0</v>
+      </c>
+      <c r="H165" s="1">
+        <v>0</v>
+      </c>
+      <c r="I165" s="1">
+        <v>1</v>
+      </c>
+      <c r="J165" s="1">
+        <v>0</v>
+      </c>
+      <c r="K165" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E165,"DD"))),0),"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B166" s="6">
+        <v>5498</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E166" s="3">
+        <f>IF($A166="","",$A166-1)</f>
+        <v>45024</v>
+      </c>
+      <c r="F166" s="4">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1">
+        <v>0</v>
+      </c>
+      <c r="H166" s="1">
+        <v>1</v>
+      </c>
+      <c r="I166" s="1">
+        <v>1</v>
+      </c>
+      <c r="J166" s="1">
+        <v>0</v>
+      </c>
+      <c r="K166" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E166,"DD"))),0),"")</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J99" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J166" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B99" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B166" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2 B96" numberStoredAsText="1"/>
+    <ignoredError sqref="B2 B138 B96" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
datos actualizados del 9 y algunos del 10-04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E19CE1-57B3-4765-979F-F87A7535A79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA795B-6531-486D-9FC3-0F8CBE993075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="330" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="540" yWindow="210" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="128">
   <si>
     <t>Usuario</t>
   </si>
@@ -654,6 +654,48 @@
   </si>
   <si>
     <t>Pasa a la acción Invocación por Péndulo</t>
+  </si>
+  <si>
+    <t>Burning Abyss Phantom Knights</t>
+  </si>
+  <si>
+    <t>Mente de la Plana</t>
+  </si>
+  <si>
+    <t>Stromberg</t>
+  </si>
+  <si>
+    <t>Robar sentido Viento</t>
+  </si>
+  <si>
+    <t>Lanzaconjuros</t>
+  </si>
+  <si>
+    <t>Ice Barrier</t>
+  </si>
+  <si>
+    <t>Paliza</t>
+  </si>
+  <si>
+    <t>6916</t>
+  </si>
+  <si>
+    <t>Magnet Warrios</t>
+  </si>
+  <si>
+    <t>Blue-Eyes</t>
+  </si>
+  <si>
+    <t>Dragones Definitivos</t>
+  </si>
+  <si>
+    <t>Estrategia Fantasma</t>
+  </si>
+  <si>
+    <t>Burning Abyss</t>
+  </si>
+  <si>
+    <t>Futuro ft Crystrons</t>
   </si>
 </sst>
 </file>
@@ -988,8 +1030,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K166" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K166" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K232" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K232" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1308,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K166"/>
+  <dimension ref="A1:K232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="G167" sqref="G167 I167:J167 H167:H168 G169:I169 G170:H174 J169:J170 I171:J175 G176:J176 G178:I178 H180:H181 G180:G182 I180:I182 H183:H189 G185:G190 G192 I184:I195 H192:H196 H197:I198 H200 I200:I201 H202:I204 F193:F208 H206:H208 F209:G229 I206:I212 I214:I217 J178:J218 I219:J229 F230:I231 F232:H232 J232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4003,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="1">
         <v>1</v>
@@ -4995,7 +5037,7 @@
         <v>68</v>
       </c>
       <c r="E100" s="3">
-        <f>IF($A100="","",$A100-1)</f>
+        <f t="shared" ref="E100:E131" si="8">IF($A100="","",$A100-1)</f>
         <v>45024</v>
       </c>
       <c r="F100" s="4">
@@ -5014,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="K100" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E100,"DD"))),0),"")</f>
+        <f t="shared" ref="K100:K131" si="9">IFERROR(ROUND((VALUE(TEXT($E100,"DD"))),0),"")</f>
         <v>8</v>
       </c>
     </row>
@@ -5032,7 +5074,7 @@
         <v>49</v>
       </c>
       <c r="E101" s="3">
-        <f>IF($A101="","",$A101-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F101" s="4">
@@ -5051,7 +5093,7 @@
         <v>0</v>
       </c>
       <c r="K101" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E101,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5069,7 +5111,7 @@
         <v>49</v>
       </c>
       <c r="E102" s="3">
-        <f>IF($A102="","",$A102-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F102" s="4">
@@ -5088,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="K102" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E102,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5106,7 +5148,7 @@
         <v>87</v>
       </c>
       <c r="E103" s="3">
-        <f>IF($A103="","",$A103-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F103" s="4">
@@ -5125,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="K103" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E103,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5143,7 +5185,7 @@
         <v>58</v>
       </c>
       <c r="E104" s="3">
-        <f>IF($A104="","",$A104-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F104" s="4">
@@ -5162,7 +5204,7 @@
         <v>1</v>
       </c>
       <c r="K104" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E104,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5180,7 +5222,7 @@
         <v>62</v>
       </c>
       <c r="E105" s="3">
-        <f>IF($A105="","",$A105-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F105" s="4">
@@ -5199,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="K105" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E105,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5217,7 +5259,7 @@
         <v>56</v>
       </c>
       <c r="E106" s="3">
-        <f>IF($A106="","",$A106-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F106" s="4">
@@ -5236,7 +5278,7 @@
         <v>0</v>
       </c>
       <c r="K106" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E106,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5254,7 +5296,7 @@
         <v>58</v>
       </c>
       <c r="E107" s="3">
-        <f>IF($A107="","",$A107-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F107" s="4">
@@ -5273,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="K107" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E107,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5291,7 +5333,7 @@
         <v>88</v>
       </c>
       <c r="E108" s="3">
-        <f>IF($A108="","",$A108-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F108" s="4">
@@ -5310,7 +5352,7 @@
         <v>0</v>
       </c>
       <c r="K108" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E108,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5328,7 +5370,7 @@
         <v>35</v>
       </c>
       <c r="E109" s="3">
-        <f>IF($A109="","",$A109-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F109" s="4">
@@ -5347,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="K109" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E109,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5365,7 +5407,7 @@
         <v>24</v>
       </c>
       <c r="E110" s="3">
-        <f>IF($A110="","",$A110-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F110" s="4">
@@ -5384,7 +5426,7 @@
         <v>0</v>
       </c>
       <c r="K110" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E110,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5402,7 +5444,7 @@
         <v>58</v>
       </c>
       <c r="E111" s="3">
-        <f>IF($A111="","",$A111-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F111" s="4">
@@ -5421,7 +5463,7 @@
         <v>0</v>
       </c>
       <c r="K111" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E111,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5439,7 +5481,7 @@
         <v>89</v>
       </c>
       <c r="E112" s="3">
-        <f>IF($A112="","",$A112-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F112" s="4">
@@ -5449,7 +5491,7 @@
         <v>1</v>
       </c>
       <c r="H112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112" s="1">
         <v>1</v>
@@ -5458,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="K112" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E112,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5476,7 +5518,7 @@
         <v>19</v>
       </c>
       <c r="E113" s="3">
-        <f>IF($A113="","",$A113-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F113" s="4">
@@ -5495,7 +5537,7 @@
         <v>0</v>
       </c>
       <c r="K113" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E113,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5513,7 +5555,7 @@
         <v>17</v>
       </c>
       <c r="E114" s="3">
-        <f>IF($A114="","",$A114-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F114" s="4">
@@ -5532,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="K114" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E114,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5550,7 +5592,7 @@
         <v>17</v>
       </c>
       <c r="E115" s="3">
-        <f>IF($A115="","",$A115-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F115" s="4">
@@ -5569,7 +5611,7 @@
         <v>0</v>
       </c>
       <c r="K115" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E115,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5587,7 +5629,7 @@
         <v>43</v>
       </c>
       <c r="E116" s="3">
-        <f>IF($A116="","",$A116-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F116" s="4">
@@ -5606,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="K116" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E116,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5624,7 +5666,7 @@
         <v>58</v>
       </c>
       <c r="E117" s="3">
-        <f>IF($A117="","",$A117-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F117" s="4">
@@ -5643,7 +5685,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E117,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5661,7 +5703,7 @@
         <v>62</v>
       </c>
       <c r="E118" s="3">
-        <f>IF($A118="","",$A118-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F118" s="4">
@@ -5680,7 +5722,7 @@
         <v>0</v>
       </c>
       <c r="K118" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E118,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5698,7 +5740,7 @@
         <v>87</v>
       </c>
       <c r="E119" s="3">
-        <f>IF($A119="","",$A119-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F119" s="4">
@@ -5717,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="K119" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E119,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5735,7 +5777,7 @@
         <v>91</v>
       </c>
       <c r="E120" s="3">
-        <f>IF($A120="","",$A120-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F120" s="4">
@@ -5754,7 +5796,7 @@
         <v>0</v>
       </c>
       <c r="K120" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E120,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5772,7 +5814,7 @@
         <v>31</v>
       </c>
       <c r="E121" s="3">
-        <f>IF($A121="","",$A121-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F121" s="4">
@@ -5791,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="K121" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E121,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5809,7 +5851,7 @@
         <v>92</v>
       </c>
       <c r="E122" s="3">
-        <f>IF($A122="","",$A122-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F122" s="4">
@@ -5828,7 +5870,7 @@
         <v>0</v>
       </c>
       <c r="K122" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E122,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5846,7 +5888,7 @@
         <v>58</v>
       </c>
       <c r="E123" s="3">
-        <f>IF($A123="","",$A123-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F123" s="4">
@@ -5865,7 +5907,7 @@
         <v>0</v>
       </c>
       <c r="K123" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E123,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5883,7 +5925,7 @@
         <v>68</v>
       </c>
       <c r="E124" s="3">
-        <f>IF($A124="","",$A124-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F124" s="4">
@@ -5902,7 +5944,7 @@
         <v>0</v>
       </c>
       <c r="K124" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E124,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5920,7 +5962,7 @@
         <v>94</v>
       </c>
       <c r="E125" s="3">
-        <f>IF($A125="","",$A125-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F125" s="4">
@@ -5939,7 +5981,7 @@
         <v>0</v>
       </c>
       <c r="K125" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E125,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5957,7 +5999,7 @@
         <v>49</v>
       </c>
       <c r="E126" s="3">
-        <f>IF($A126="","",$A126-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F126" s="4">
@@ -5976,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="K126" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E126,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -5994,7 +6036,7 @@
         <v>24</v>
       </c>
       <c r="E127" s="3">
-        <f>IF($A127="","",$A127-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F127" s="4">
@@ -6013,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="K127" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E127,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -6031,7 +6073,7 @@
         <v>24</v>
       </c>
       <c r="E128" s="3">
-        <f>IF($A128="","",$A128-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F128" s="4">
@@ -6050,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="K128" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E128,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -6068,7 +6110,7 @@
         <v>96</v>
       </c>
       <c r="E129" s="3">
-        <f>IF($A129="","",$A129-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F129" s="4">
@@ -6087,7 +6129,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E129,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -6105,7 +6147,7 @@
         <v>98</v>
       </c>
       <c r="E130" s="3">
-        <f>IF($A130="","",$A130-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F130" s="4">
@@ -6124,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="K130" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E130,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -6142,7 +6184,7 @@
         <v>29</v>
       </c>
       <c r="E131" s="3">
-        <f>IF($A131="","",$A131-1)</f>
+        <f t="shared" si="8"/>
         <v>45024</v>
       </c>
       <c r="F131" s="4">
@@ -6161,7 +6203,7 @@
         <v>1</v>
       </c>
       <c r="K131" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E131,"DD"))),0),"")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
     </row>
@@ -6179,7 +6221,7 @@
         <v>19</v>
       </c>
       <c r="E132" s="3">
-        <f>IF($A132="","",$A132-1)</f>
+        <f t="shared" ref="E132:E166" si="10">IF($A132="","",$A132-1)</f>
         <v>45024</v>
       </c>
       <c r="F132" s="4">
@@ -6198,7 +6240,7 @@
         <v>0</v>
       </c>
       <c r="K132" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E132,"DD"))),0),"")</f>
+        <f t="shared" ref="K132:K166" si="11">IFERROR(ROUND((VALUE(TEXT($E132,"DD"))),0),"")</f>
         <v>8</v>
       </c>
     </row>
@@ -6216,7 +6258,7 @@
         <v>99</v>
       </c>
       <c r="E133" s="3">
-        <f>IF($A133="","",$A133-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F133" s="4">
@@ -6235,7 +6277,7 @@
         <v>1</v>
       </c>
       <c r="K133" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E133,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6253,7 +6295,7 @@
         <v>35</v>
       </c>
       <c r="E134" s="3">
-        <f>IF($A134="","",$A134-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F134" s="4">
@@ -6272,7 +6314,7 @@
         <v>0</v>
       </c>
       <c r="K134" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E134,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6290,7 +6332,7 @@
         <v>19</v>
       </c>
       <c r="E135" s="3">
-        <f>IF($A135="","",$A135-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F135" s="4">
@@ -6309,7 +6351,7 @@
         <v>0</v>
       </c>
       <c r="K135" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E135,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6327,7 +6369,7 @@
         <v>21</v>
       </c>
       <c r="E136" s="3">
-        <f>IF($A136="","",$A136-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F136" s="4">
@@ -6346,7 +6388,7 @@
         <v>0</v>
       </c>
       <c r="K136" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E136,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6364,7 +6406,7 @@
         <v>33</v>
       </c>
       <c r="E137" s="3">
-        <f>IF($A137="","",$A137-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F137" s="4">
@@ -6383,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="K137" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E137,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6401,7 +6443,7 @@
         <v>17</v>
       </c>
       <c r="E138" s="3">
-        <f>IF($A138="","",$A138-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F138" s="4">
@@ -6420,7 +6462,7 @@
         <v>1</v>
       </c>
       <c r="K138" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E138,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6438,7 +6480,7 @@
         <v>102</v>
       </c>
       <c r="E139" s="3">
-        <f>IF($A139="","",$A139-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F139" s="4">
@@ -6457,7 +6499,7 @@
         <v>0</v>
       </c>
       <c r="K139" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E139,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6475,7 +6517,7 @@
         <v>47</v>
       </c>
       <c r="E140" s="3">
-        <f>IF($A140="","",$A140-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F140" s="4">
@@ -6494,7 +6536,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E140,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6512,7 +6554,7 @@
         <v>104</v>
       </c>
       <c r="E141" s="3">
-        <f>IF($A141="","",$A141-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F141" s="4">
@@ -6531,7 +6573,7 @@
         <v>0</v>
       </c>
       <c r="K141" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E141,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6549,7 +6591,7 @@
         <v>98</v>
       </c>
       <c r="E142" s="3">
-        <f>IF($A142="","",$A142-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F142" s="4">
@@ -6568,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="K142" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E142,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6586,7 +6628,7 @@
         <v>31</v>
       </c>
       <c r="E143" s="3">
-        <f>IF($A143="","",$A143-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F143" s="4">
@@ -6605,7 +6647,7 @@
         <v>0</v>
       </c>
       <c r="K143" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E143,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6623,7 +6665,7 @@
         <v>106</v>
       </c>
       <c r="E144" s="3">
-        <f>IF($A144="","",$A144-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F144" s="4">
@@ -6642,7 +6684,7 @@
         <v>0</v>
       </c>
       <c r="K144" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E144,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6660,7 +6702,7 @@
         <v>29</v>
       </c>
       <c r="E145" s="3">
-        <f>IF($A145="","",$A145-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F145" s="4">
@@ -6679,7 +6721,7 @@
         <v>0</v>
       </c>
       <c r="K145" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E145,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6697,7 +6739,7 @@
         <v>58</v>
       </c>
       <c r="E146" s="3">
-        <f>IF($A146="","",$A146-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F146" s="4">
@@ -6716,7 +6758,7 @@
         <v>0</v>
       </c>
       <c r="K146" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E146,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6734,7 +6776,7 @@
         <v>29</v>
       </c>
       <c r="E147" s="3">
-        <f>IF($A147="","",$A147-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F147" s="4">
@@ -6753,7 +6795,7 @@
         <v>0</v>
       </c>
       <c r="K147" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E147,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6771,7 +6813,7 @@
         <v>68</v>
       </c>
       <c r="E148" s="3">
-        <f>IF($A148="","",$A148-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F148" s="4">
@@ -6790,7 +6832,7 @@
         <v>1</v>
       </c>
       <c r="K148" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E148,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6808,7 +6850,7 @@
         <v>31</v>
       </c>
       <c r="E149" s="3">
-        <f>IF($A149="","",$A149-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F149" s="4">
@@ -6827,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="K149" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E149,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6845,7 +6887,7 @@
         <v>35</v>
       </c>
       <c r="E150" s="3">
-        <f>IF($A150="","",$A150-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F150" s="4">
@@ -6864,7 +6906,7 @@
         <v>0</v>
       </c>
       <c r="K150" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E150,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6882,7 +6924,7 @@
         <v>45</v>
       </c>
       <c r="E151" s="3">
-        <f>IF($A151="","",$A151-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F151" s="4">
@@ -6901,7 +6943,7 @@
         <v>0</v>
       </c>
       <c r="K151" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E151,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6919,7 +6961,7 @@
         <v>81</v>
       </c>
       <c r="E152" s="3">
-        <f>IF($A152="","",$A152-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F152" s="4">
@@ -6938,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="K152" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E152,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6956,7 +6998,7 @@
         <v>19</v>
       </c>
       <c r="E153" s="3">
-        <f>IF($A153="","",$A153-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F153" s="4">
@@ -6975,7 +7017,7 @@
         <v>0</v>
       </c>
       <c r="K153" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E153,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -6993,7 +7035,7 @@
         <v>62</v>
       </c>
       <c r="E154" s="3">
-        <f>IF($A154="","",$A154-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F154" s="4">
@@ -7012,7 +7054,7 @@
         <v>0</v>
       </c>
       <c r="K154" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E154,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7030,7 +7072,7 @@
         <v>106</v>
       </c>
       <c r="E155" s="3">
-        <f>IF($A155="","",$A155-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F155" s="4">
@@ -7049,7 +7091,7 @@
         <v>0</v>
       </c>
       <c r="K155" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E155,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7067,7 +7109,7 @@
         <v>27</v>
       </c>
       <c r="E156" s="3">
-        <f>IF($A156="","",$A156-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F156" s="4">
@@ -7086,7 +7128,7 @@
         <v>0</v>
       </c>
       <c r="K156" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E156,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7104,7 +7146,7 @@
         <v>19</v>
       </c>
       <c r="E157" s="3">
-        <f>IF($A157="","",$A157-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F157" s="4">
@@ -7123,7 +7165,7 @@
         <v>0</v>
       </c>
       <c r="K157" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E157,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7141,7 +7183,7 @@
         <v>110</v>
       </c>
       <c r="E158" s="3">
-        <f>IF($A158="","",$A158-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F158" s="4">
@@ -7160,7 +7202,7 @@
         <v>0</v>
       </c>
       <c r="K158" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E158,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7178,7 +7220,7 @@
         <v>60</v>
       </c>
       <c r="E159" s="3">
-        <f>IF($A159="","",$A159-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F159" s="4">
@@ -7197,7 +7239,7 @@
         <v>0</v>
       </c>
       <c r="K159" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E159,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7215,7 +7257,7 @@
         <v>62</v>
       </c>
       <c r="E160" s="3">
-        <f>IF($A160="","",$A160-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F160" s="4">
@@ -7234,7 +7276,7 @@
         <v>0</v>
       </c>
       <c r="K160" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E160,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7252,7 +7294,7 @@
         <v>111</v>
       </c>
       <c r="E161" s="3">
-        <f>IF($A161="","",$A161-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F161" s="4">
@@ -7271,7 +7313,7 @@
         <v>0</v>
       </c>
       <c r="K161" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E161,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7289,7 +7331,7 @@
         <v>112</v>
       </c>
       <c r="E162" s="3">
-        <f>IF($A162="","",$A162-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F162" s="4">
@@ -7308,7 +7350,7 @@
         <v>0</v>
       </c>
       <c r="K162" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E162,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7326,7 +7368,7 @@
         <v>29</v>
       </c>
       <c r="E163" s="3">
-        <f>IF($A163="","",$A163-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F163" s="4">
@@ -7345,7 +7387,7 @@
         <v>0</v>
       </c>
       <c r="K163" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E163,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7363,7 +7405,7 @@
         <v>113</v>
       </c>
       <c r="E164" s="3">
-        <f>IF($A164="","",$A164-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F164" s="4">
@@ -7382,7 +7424,7 @@
         <v>1</v>
       </c>
       <c r="K164" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E164,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7400,7 +7442,7 @@
         <v>27</v>
       </c>
       <c r="E165" s="3">
-        <f>IF($A165="","",$A165-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F165" s="4">
@@ -7419,7 +7461,7 @@
         <v>0</v>
       </c>
       <c r="K165" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E165,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
@@ -7437,7 +7479,7 @@
         <v>56</v>
       </c>
       <c r="E166" s="3">
-        <f>IF($A166="","",$A166-1)</f>
+        <f t="shared" si="10"/>
         <v>45024</v>
       </c>
       <c r="F166" s="4">
@@ -7456,23 +7498,2465 @@
         <v>0</v>
       </c>
       <c r="K166" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E166,"DD"))),0),"")</f>
+        <f t="shared" si="11"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B167" s="6">
+        <v>3836</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E167" s="3">
+        <f>IF($A167="","",$A167-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F167" s="4">
+        <v>1</v>
+      </c>
+      <c r="G167" s="1">
+        <v>0</v>
+      </c>
+      <c r="H167" s="1">
+        <v>0</v>
+      </c>
+      <c r="I167" s="1">
+        <v>0</v>
+      </c>
+      <c r="J167" s="1">
+        <v>0</v>
+      </c>
+      <c r="K167" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E167,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B168" s="6">
+        <v>3251</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E168" s="3">
+        <f>IF($A168="","",$A168-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F168" s="4">
+        <v>1</v>
+      </c>
+      <c r="G168" s="1">
+        <v>1</v>
+      </c>
+      <c r="H168" s="1">
+        <v>0</v>
+      </c>
+      <c r="I168" s="1">
+        <v>1</v>
+      </c>
+      <c r="J168" s="1">
+        <v>1</v>
+      </c>
+      <c r="K168" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E168,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B169" s="6">
+        <v>2711</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E169" s="3">
+        <f>IF($A169="","",$A169-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F169" s="4">
+        <v>1</v>
+      </c>
+      <c r="G169" s="1">
+        <v>0</v>
+      </c>
+      <c r="H169" s="1">
+        <v>0</v>
+      </c>
+      <c r="I169" s="1">
+        <v>0</v>
+      </c>
+      <c r="J169" s="1">
+        <v>0</v>
+      </c>
+      <c r="K169" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E169,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B170" s="6">
+        <v>5281</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E170" s="3">
+        <f>IF($A170="","",$A170-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F170" s="4">
+        <v>1</v>
+      </c>
+      <c r="G170" s="1">
+        <v>0</v>
+      </c>
+      <c r="H170" s="1">
+        <v>0</v>
+      </c>
+      <c r="I170" s="1">
+        <v>1</v>
+      </c>
+      <c r="J170" s="1">
+        <v>0</v>
+      </c>
+      <c r="K170" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E170,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B171" s="6">
+        <v>3318</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E171" s="3">
+        <f>IF($A171="","",$A171-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F171" s="4">
+        <v>1</v>
+      </c>
+      <c r="G171" s="1">
+        <v>0</v>
+      </c>
+      <c r="H171" s="1">
+        <v>0</v>
+      </c>
+      <c r="I171" s="1">
+        <v>0</v>
+      </c>
+      <c r="J171" s="1">
+        <v>0</v>
+      </c>
+      <c r="K171" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E171,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B172" s="6">
+        <v>3024</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E172" s="3">
+        <f>IF($A172="","",$A172-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F172" s="4">
+        <v>1</v>
+      </c>
+      <c r="G172" s="1">
+        <v>0</v>
+      </c>
+      <c r="H172" s="1">
+        <v>0</v>
+      </c>
+      <c r="I172" s="1">
+        <v>0</v>
+      </c>
+      <c r="J172" s="1">
+        <v>0</v>
+      </c>
+      <c r="K172" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E172,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B173" s="6">
+        <v>8026</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E173" s="3">
+        <f>IF($A173="","",$A173-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F173" s="4">
+        <v>1</v>
+      </c>
+      <c r="G173" s="1">
+        <v>0</v>
+      </c>
+      <c r="H173" s="1">
+        <v>0</v>
+      </c>
+      <c r="I173" s="1">
+        <v>0</v>
+      </c>
+      <c r="J173" s="1">
+        <v>0</v>
+      </c>
+      <c r="K173" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E173,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B174" s="6">
+        <v>7281</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E174" s="3">
+        <f>IF($A174="","",$A174-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F174" s="4">
+        <v>1</v>
+      </c>
+      <c r="G174" s="1">
+        <v>0</v>
+      </c>
+      <c r="H174" s="1">
+        <v>0</v>
+      </c>
+      <c r="I174" s="1">
+        <v>0</v>
+      </c>
+      <c r="J174" s="1">
+        <v>0</v>
+      </c>
+      <c r="K174" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E174,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B175" s="6">
+        <v>1277</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E175" s="3">
+        <f>IF($A175="","",$A175-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F175" s="4">
+        <v>1</v>
+      </c>
+      <c r="G175" s="1">
+        <v>1</v>
+      </c>
+      <c r="H175" s="1">
+        <v>1</v>
+      </c>
+      <c r="I175" s="1">
+        <v>0</v>
+      </c>
+      <c r="J175" s="1">
+        <v>0</v>
+      </c>
+      <c r="K175" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E175,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B176" s="6">
+        <v>6628</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" s="3">
+        <f>IF($A176="","",$A176-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F176" s="4">
+        <v>1</v>
+      </c>
+      <c r="G176" s="1">
+        <v>0</v>
+      </c>
+      <c r="H176" s="1">
+        <v>0</v>
+      </c>
+      <c r="I176" s="1">
+        <v>0</v>
+      </c>
+      <c r="J176" s="1">
+        <v>0</v>
+      </c>
+      <c r="K176" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E176,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B177" s="6">
+        <v>6622</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E177" s="3">
+        <f>IF($A177="","",$A177-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F177" s="4">
+        <v>1</v>
+      </c>
+      <c r="G177" s="1">
+        <v>1</v>
+      </c>
+      <c r="H177" s="1">
+        <v>1</v>
+      </c>
+      <c r="I177" s="1">
+        <v>1</v>
+      </c>
+      <c r="J177" s="1">
+        <v>1</v>
+      </c>
+      <c r="K177" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E177,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B178" s="6">
+        <v>4003</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E178" s="3">
+        <f>IF($A178="","",$A178-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F178" s="4">
+        <v>1</v>
+      </c>
+      <c r="G178" s="1">
+        <v>0</v>
+      </c>
+      <c r="H178" s="1">
+        <v>0</v>
+      </c>
+      <c r="I178" s="1">
+        <v>0</v>
+      </c>
+      <c r="J178" s="1">
+        <v>0</v>
+      </c>
+      <c r="K178" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E178,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B179" s="6">
+        <v>1746</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E179" s="3">
+        <f>IF($A179="","",$A179-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F179" s="4">
+        <v>1</v>
+      </c>
+      <c r="G179" s="1">
+        <v>1</v>
+      </c>
+      <c r="H179" s="1">
+        <v>1</v>
+      </c>
+      <c r="I179" s="1">
+        <v>1</v>
+      </c>
+      <c r="J179" s="1">
+        <v>0</v>
+      </c>
+      <c r="K179" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E179,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B180" s="6">
+        <v>1762</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E180" s="3">
+        <f>IF($A180="","",$A180-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F180" s="4">
+        <v>1</v>
+      </c>
+      <c r="G180" s="1">
+        <v>0</v>
+      </c>
+      <c r="H180" s="1">
+        <v>0</v>
+      </c>
+      <c r="I180" s="1">
+        <v>0</v>
+      </c>
+      <c r="J180" s="1">
+        <v>0</v>
+      </c>
+      <c r="K180" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E180,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B181" s="6">
+        <v>2349</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E181" s="3">
+        <f>IF($A181="","",$A181-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F181" s="4">
+        <v>1</v>
+      </c>
+      <c r="G181" s="1">
+        <v>0</v>
+      </c>
+      <c r="H181" s="1">
+        <v>0</v>
+      </c>
+      <c r="I181" s="1">
+        <v>0</v>
+      </c>
+      <c r="J181" s="1">
+        <v>0</v>
+      </c>
+      <c r="K181" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E181,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B182" s="6">
+        <v>9632</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E182" s="3">
+        <f>IF($A182="","",$A182-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F182" s="4">
+        <v>1</v>
+      </c>
+      <c r="G182" s="1">
+        <v>0</v>
+      </c>
+      <c r="H182" s="1">
+        <v>1</v>
+      </c>
+      <c r="I182" s="1">
+        <v>0</v>
+      </c>
+      <c r="J182" s="1">
+        <v>0</v>
+      </c>
+      <c r="K182" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E182,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B183" s="6">
+        <v>1209</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E183" s="3">
+        <f>IF($A183="","",$A183-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F183" s="4">
+        <v>1</v>
+      </c>
+      <c r="G183" s="1">
+        <v>1</v>
+      </c>
+      <c r="H183" s="1">
+        <v>0</v>
+      </c>
+      <c r="I183" s="1">
+        <v>1</v>
+      </c>
+      <c r="J183" s="1">
+        <v>0</v>
+      </c>
+      <c r="K183" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E183,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B184" s="6">
+        <v>8511</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E184" s="3">
+        <f>IF($A184="","",$A184-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F184" s="4">
+        <v>1</v>
+      </c>
+      <c r="G184" s="1">
+        <v>1</v>
+      </c>
+      <c r="H184" s="1">
+        <v>0</v>
+      </c>
+      <c r="I184" s="1">
+        <v>0</v>
+      </c>
+      <c r="J184" s="1">
+        <v>0</v>
+      </c>
+      <c r="K184" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E184,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B185" s="6">
+        <v>5494</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E185" s="3">
+        <f>IF($A185="","",$A185-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F185" s="4">
+        <v>1</v>
+      </c>
+      <c r="G185" s="1">
+        <v>0</v>
+      </c>
+      <c r="H185" s="1">
+        <v>0</v>
+      </c>
+      <c r="I185" s="1">
+        <v>0</v>
+      </c>
+      <c r="J185" s="1">
+        <v>0</v>
+      </c>
+      <c r="K185" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E185,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B186" s="6">
+        <v>7277</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E186" s="3">
+        <f>IF($A186="","",$A186-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F186" s="4">
+        <v>1</v>
+      </c>
+      <c r="G186" s="1">
+        <v>0</v>
+      </c>
+      <c r="H186" s="1">
+        <v>0</v>
+      </c>
+      <c r="I186" s="1">
+        <v>0</v>
+      </c>
+      <c r="J186" s="1">
+        <v>0</v>
+      </c>
+      <c r="K186" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E186,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B187" s="6">
+        <v>9731</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E187" s="3">
+        <f>IF($A187="","",$A187-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F187" s="4">
+        <v>1</v>
+      </c>
+      <c r="G187" s="1">
+        <v>0</v>
+      </c>
+      <c r="H187" s="1">
+        <v>0</v>
+      </c>
+      <c r="I187" s="1">
+        <v>0</v>
+      </c>
+      <c r="J187" s="1">
+        <v>0</v>
+      </c>
+      <c r="K187" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E187,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B188" s="6">
+        <v>268</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E188" s="3">
+        <f>IF($A188="","",$A188-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F188" s="4">
+        <v>1</v>
+      </c>
+      <c r="G188" s="1">
+        <v>0</v>
+      </c>
+      <c r="H188" s="1">
+        <v>0</v>
+      </c>
+      <c r="I188" s="1">
+        <v>0</v>
+      </c>
+      <c r="J188" s="1">
+        <v>0</v>
+      </c>
+      <c r="K188" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E188,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B189" s="6">
+        <v>5838</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E189" s="3">
+        <f>IF($A189="","",$A189-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F189" s="4">
+        <v>1</v>
+      </c>
+      <c r="G189" s="1">
+        <v>0</v>
+      </c>
+      <c r="H189" s="1">
+        <v>0</v>
+      </c>
+      <c r="I189" s="1">
+        <v>0</v>
+      </c>
+      <c r="J189" s="1">
+        <v>0</v>
+      </c>
+      <c r="K189" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E189,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B190" s="6">
+        <v>7744</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E190" s="3">
+        <f>IF($A190="","",$A190-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F190" s="4">
+        <v>1</v>
+      </c>
+      <c r="G190" s="1">
+        <v>0</v>
+      </c>
+      <c r="H190" s="1">
+        <v>1</v>
+      </c>
+      <c r="I190" s="1">
+        <v>0</v>
+      </c>
+      <c r="J190" s="1">
+        <v>0</v>
+      </c>
+      <c r="K190" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E190,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B191" s="6">
+        <v>22</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E191" s="3">
+        <f>IF($A191="","",$A191-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F191" s="4">
+        <v>1</v>
+      </c>
+      <c r="G191" s="1">
+        <v>1</v>
+      </c>
+      <c r="H191" s="1">
+        <v>1</v>
+      </c>
+      <c r="I191" s="1">
+        <v>0</v>
+      </c>
+      <c r="J191" s="1">
+        <v>0</v>
+      </c>
+      <c r="K191" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E191,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B192" s="6">
+        <v>8496</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E192" s="3">
+        <f>IF($A192="","",$A192-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F192" s="4">
+        <v>1</v>
+      </c>
+      <c r="G192" s="1">
+        <v>0</v>
+      </c>
+      <c r="H192" s="1">
+        <v>0</v>
+      </c>
+      <c r="I192" s="1">
+        <v>0</v>
+      </c>
+      <c r="J192" s="1">
+        <v>0</v>
+      </c>
+      <c r="K192" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E192,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B193" s="6">
+        <v>6412</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E193" s="3">
+        <f>IF($A193="","",$A193-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F193" s="4">
+        <v>0</v>
+      </c>
+      <c r="G193" s="1">
+        <v>1</v>
+      </c>
+      <c r="H193" s="1">
+        <v>0</v>
+      </c>
+      <c r="I193" s="1">
+        <v>0</v>
+      </c>
+      <c r="J193" s="1">
+        <v>0</v>
+      </c>
+      <c r="K193" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E193,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B194" s="6">
+        <v>747</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E194" s="3">
+        <f>IF($A194="","",$A194-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F194" s="4">
+        <v>0</v>
+      </c>
+      <c r="G194" s="1">
+        <v>1</v>
+      </c>
+      <c r="H194" s="1">
+        <v>0</v>
+      </c>
+      <c r="I194" s="1">
+        <v>0</v>
+      </c>
+      <c r="J194" s="1">
+        <v>0</v>
+      </c>
+      <c r="K194" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E194,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B195" s="6">
+        <v>1728</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E195" s="3">
+        <f>IF($A195="","",$A195-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F195" s="4">
+        <v>0</v>
+      </c>
+      <c r="G195" s="1">
+        <v>1</v>
+      </c>
+      <c r="H195" s="1">
+        <v>0</v>
+      </c>
+      <c r="I195" s="1">
+        <v>0</v>
+      </c>
+      <c r="J195" s="1">
+        <v>0</v>
+      </c>
+      <c r="K195" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E195,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B196" s="6">
+        <v>1048</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E196" s="3">
+        <f>IF($A196="","",$A196-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F196" s="4">
+        <v>0</v>
+      </c>
+      <c r="G196" s="1">
+        <v>1</v>
+      </c>
+      <c r="H196" s="1">
+        <v>0</v>
+      </c>
+      <c r="I196" s="1">
+        <v>1</v>
+      </c>
+      <c r="J196" s="1">
+        <v>0</v>
+      </c>
+      <c r="K196" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E196,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B197" s="6">
+        <v>1387</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E197" s="3">
+        <f>IF($A197="","",$A197-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F197" s="4">
+        <v>0</v>
+      </c>
+      <c r="G197" s="1">
+        <v>1</v>
+      </c>
+      <c r="H197" s="1">
+        <v>0</v>
+      </c>
+      <c r="I197" s="1">
+        <v>0</v>
+      </c>
+      <c r="J197" s="1">
+        <v>0</v>
+      </c>
+      <c r="K197" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E197,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E198" s="3">
+        <f>IF($A198="","",$A198-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F198" s="4">
+        <v>0</v>
+      </c>
+      <c r="G198" s="1">
+        <v>1</v>
+      </c>
+      <c r="H198" s="1">
+        <v>0</v>
+      </c>
+      <c r="I198" s="1">
+        <v>0</v>
+      </c>
+      <c r="J198" s="1">
+        <v>0</v>
+      </c>
+      <c r="K198" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E198,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B199" s="6">
+        <v>8834</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E199" s="3">
+        <f>IF($A199="","",$A199-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F199" s="4">
+        <v>0</v>
+      </c>
+      <c r="G199" s="1">
+        <v>1</v>
+      </c>
+      <c r="H199" s="1">
+        <v>1</v>
+      </c>
+      <c r="I199" s="1">
+        <v>1</v>
+      </c>
+      <c r="J199" s="1">
+        <v>0</v>
+      </c>
+      <c r="K199" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E199,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B200" s="6">
+        <v>3771</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E200" s="3">
+        <f>IF($A200="","",$A200-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F200" s="4">
+        <v>0</v>
+      </c>
+      <c r="G200" s="1">
+        <v>1</v>
+      </c>
+      <c r="H200" s="1">
+        <v>0</v>
+      </c>
+      <c r="I200" s="1">
+        <v>0</v>
+      </c>
+      <c r="J200" s="1">
+        <v>0</v>
+      </c>
+      <c r="K200" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E200,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B201" s="6">
+        <v>4691</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E201" s="3">
+        <f>IF($A201="","",$A201-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F201" s="4">
+        <v>0</v>
+      </c>
+      <c r="G201" s="1">
+        <v>1</v>
+      </c>
+      <c r="H201" s="1">
+        <v>1</v>
+      </c>
+      <c r="I201" s="1">
+        <v>0</v>
+      </c>
+      <c r="J201" s="1">
+        <v>0</v>
+      </c>
+      <c r="K201" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E201,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B202" s="6">
+        <v>4698</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E202" s="3">
+        <f>IF($A202="","",$A202-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F202" s="4">
+        <v>0</v>
+      </c>
+      <c r="G202" s="1">
+        <v>1</v>
+      </c>
+      <c r="H202" s="1">
+        <v>0</v>
+      </c>
+      <c r="I202" s="1">
+        <v>0</v>
+      </c>
+      <c r="J202" s="1">
+        <v>0</v>
+      </c>
+      <c r="K202" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E202,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B203" s="6">
+        <v>7024</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E203" s="3">
+        <f>IF($A203="","",$A203-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F203" s="4">
+        <v>0</v>
+      </c>
+      <c r="G203" s="1">
+        <v>1</v>
+      </c>
+      <c r="H203" s="1">
+        <v>0</v>
+      </c>
+      <c r="I203" s="1">
+        <v>0</v>
+      </c>
+      <c r="J203" s="1">
+        <v>0</v>
+      </c>
+      <c r="K203" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E203,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B204" s="6">
+        <v>4150</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E204" s="3">
+        <f>IF($A204="","",$A204-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F204" s="4">
+        <v>0</v>
+      </c>
+      <c r="G204" s="1">
+        <v>1</v>
+      </c>
+      <c r="H204" s="1">
+        <v>0</v>
+      </c>
+      <c r="I204" s="1">
+        <v>0</v>
+      </c>
+      <c r="J204" s="1">
+        <v>0</v>
+      </c>
+      <c r="K204" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E204,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B205" s="6">
+        <v>5168</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E205" s="3">
+        <f>IF($A205="","",$A205-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F205" s="4">
+        <v>0</v>
+      </c>
+      <c r="G205" s="1">
+        <v>1</v>
+      </c>
+      <c r="H205" s="1">
+        <v>1</v>
+      </c>
+      <c r="I205" s="1">
+        <v>1</v>
+      </c>
+      <c r="J205" s="1">
+        <v>0</v>
+      </c>
+      <c r="K205" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E205,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B206" s="6">
+        <v>7382</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E206" s="3">
+        <f>IF($A206="","",$A206-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F206" s="4">
+        <v>0</v>
+      </c>
+      <c r="G206" s="1">
+        <v>1</v>
+      </c>
+      <c r="H206" s="1">
+        <v>0</v>
+      </c>
+      <c r="I206" s="1">
+        <v>0</v>
+      </c>
+      <c r="J206" s="1">
+        <v>0</v>
+      </c>
+      <c r="K206" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E206,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B207" s="6">
+        <v>7396</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E207" s="3">
+        <f>IF($A207="","",$A207-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F207" s="4">
+        <v>0</v>
+      </c>
+      <c r="G207" s="1">
+        <v>1</v>
+      </c>
+      <c r="H207" s="1">
+        <v>0</v>
+      </c>
+      <c r="I207" s="1">
+        <v>0</v>
+      </c>
+      <c r="J207" s="1">
+        <v>0</v>
+      </c>
+      <c r="K207" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E207,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B208" s="6">
+        <v>6353</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E208" s="3">
+        <f>IF($A208="","",$A208-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F208" s="4">
+        <v>0</v>
+      </c>
+      <c r="G208" s="1">
+        <v>1</v>
+      </c>
+      <c r="H208" s="1">
+        <v>0</v>
+      </c>
+      <c r="I208" s="1">
+        <v>0</v>
+      </c>
+      <c r="J208" s="1">
+        <v>0</v>
+      </c>
+      <c r="K208" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E208,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B209" s="6">
+        <v>4171</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E209" s="3">
+        <f>IF($A209="","",$A209-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F209" s="4">
+        <v>0</v>
+      </c>
+      <c r="G209" s="1">
+        <v>0</v>
+      </c>
+      <c r="H209" s="1">
+        <v>1</v>
+      </c>
+      <c r="I209" s="1">
+        <v>0</v>
+      </c>
+      <c r="J209" s="1">
+        <v>0</v>
+      </c>
+      <c r="K209" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E209,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B210" s="6">
+        <v>4587</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E210" s="3">
+        <f>IF($A210="","",$A210-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F210" s="4">
+        <v>0</v>
+      </c>
+      <c r="G210" s="1">
+        <v>0</v>
+      </c>
+      <c r="H210" s="1">
+        <v>1</v>
+      </c>
+      <c r="I210" s="1">
+        <v>0</v>
+      </c>
+      <c r="J210" s="1">
+        <v>0</v>
+      </c>
+      <c r="K210" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E210,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B211" s="6">
+        <v>5848</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E211" s="3">
+        <f>IF($A211="","",$A211-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F211" s="4">
+        <v>0</v>
+      </c>
+      <c r="G211" s="1">
+        <v>0</v>
+      </c>
+      <c r="H211" s="1">
+        <v>1</v>
+      </c>
+      <c r="I211" s="1">
+        <v>0</v>
+      </c>
+      <c r="J211" s="1">
+        <v>0</v>
+      </c>
+      <c r="K211" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E211,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B212" s="6">
+        <v>5284</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E212" s="3">
+        <f>IF($A212="","",$A212-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F212" s="4">
+        <v>0</v>
+      </c>
+      <c r="G212" s="1">
+        <v>0</v>
+      </c>
+      <c r="H212" s="1">
+        <v>1</v>
+      </c>
+      <c r="I212" s="1">
+        <v>0</v>
+      </c>
+      <c r="J212" s="1">
+        <v>0</v>
+      </c>
+      <c r="K212" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E212,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B213" s="6">
+        <v>9774</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E213" s="3">
+        <f>IF($A213="","",$A213-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F213" s="4">
+        <v>0</v>
+      </c>
+      <c r="G213" s="1">
+        <v>0</v>
+      </c>
+      <c r="H213" s="1">
+        <v>1</v>
+      </c>
+      <c r="I213" s="1">
+        <v>1</v>
+      </c>
+      <c r="J213" s="1">
+        <v>0</v>
+      </c>
+      <c r="K213" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E213,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B214" s="6">
+        <v>1307</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E214" s="3">
+        <f>IF($A214="","",$A214-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F214" s="4">
+        <v>0</v>
+      </c>
+      <c r="G214" s="1">
+        <v>0</v>
+      </c>
+      <c r="H214" s="1">
+        <v>1</v>
+      </c>
+      <c r="I214" s="1">
+        <v>0</v>
+      </c>
+      <c r="J214" s="1">
+        <v>0</v>
+      </c>
+      <c r="K214" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E214,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B215" s="6">
+        <v>7398</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E215" s="3">
+        <f>IF($A215="","",$A215-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F215" s="4">
+        <v>0</v>
+      </c>
+      <c r="G215" s="1">
+        <v>0</v>
+      </c>
+      <c r="H215" s="1">
+        <v>1</v>
+      </c>
+      <c r="I215" s="1">
+        <v>0</v>
+      </c>
+      <c r="J215" s="1">
+        <v>0</v>
+      </c>
+      <c r="K215" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E215,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B216" s="6">
+        <v>6013</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E216" s="3">
+        <f>IF($A216="","",$A216-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F216" s="4">
+        <v>0</v>
+      </c>
+      <c r="G216" s="1">
+        <v>0</v>
+      </c>
+      <c r="H216" s="1">
+        <v>1</v>
+      </c>
+      <c r="I216" s="1">
+        <v>0</v>
+      </c>
+      <c r="J216" s="1">
+        <v>0</v>
+      </c>
+      <c r="K216" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E216,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B217" s="6">
+        <v>3867</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E217" s="3">
+        <f>IF($A217="","",$A217-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F217" s="4">
+        <v>0</v>
+      </c>
+      <c r="G217" s="1">
+        <v>0</v>
+      </c>
+      <c r="H217" s="1">
+        <v>1</v>
+      </c>
+      <c r="I217" s="1">
+        <v>0</v>
+      </c>
+      <c r="J217" s="1">
+        <v>0</v>
+      </c>
+      <c r="K217" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E217,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B218" s="6">
+        <v>1705</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E218" s="3">
+        <f>IF($A218="","",$A218-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F218" s="4">
+        <v>0</v>
+      </c>
+      <c r="G218" s="1">
+        <v>0</v>
+      </c>
+      <c r="H218" s="1">
+        <v>1</v>
+      </c>
+      <c r="I218" s="1">
+        <v>1</v>
+      </c>
+      <c r="J218" s="1">
+        <v>0</v>
+      </c>
+      <c r="K218" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E218,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B219" s="6">
+        <v>1859</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E219" s="3">
+        <f>IF($A219="","",$A219-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F219" s="4">
+        <v>0</v>
+      </c>
+      <c r="G219" s="1">
+        <v>0</v>
+      </c>
+      <c r="H219" s="1">
+        <v>1</v>
+      </c>
+      <c r="I219" s="1">
+        <v>0</v>
+      </c>
+      <c r="J219" s="1">
+        <v>0</v>
+      </c>
+      <c r="K219" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E219,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B220" s="6">
+        <v>9115</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E220" s="3">
+        <f>IF($A220="","",$A220-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F220" s="4">
+        <v>0</v>
+      </c>
+      <c r="G220" s="1">
+        <v>0</v>
+      </c>
+      <c r="H220" s="1">
+        <v>1</v>
+      </c>
+      <c r="I220" s="1">
+        <v>0</v>
+      </c>
+      <c r="J220" s="1">
+        <v>0</v>
+      </c>
+      <c r="K220" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E220,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B221" s="6">
+        <v>9252</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E221" s="3">
+        <f>IF($A221="","",$A221-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F221" s="4">
+        <v>0</v>
+      </c>
+      <c r="G221" s="1">
+        <v>0</v>
+      </c>
+      <c r="H221" s="1">
+        <v>1</v>
+      </c>
+      <c r="I221" s="1">
+        <v>0</v>
+      </c>
+      <c r="J221" s="1">
+        <v>0</v>
+      </c>
+      <c r="K221" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E221,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B222" s="6">
+        <v>4388</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E222" s="3">
+        <f>IF($A222="","",$A222-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F222" s="4">
+        <v>0</v>
+      </c>
+      <c r="G222" s="1">
+        <v>0</v>
+      </c>
+      <c r="H222" s="1">
+        <v>1</v>
+      </c>
+      <c r="I222" s="1">
+        <v>0</v>
+      </c>
+      <c r="J222" s="1">
+        <v>0</v>
+      </c>
+      <c r="K222" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E222,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B223" s="6">
+        <v>2687</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E223" s="3">
+        <f>IF($A223="","",$A223-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F223" s="4">
+        <v>0</v>
+      </c>
+      <c r="G223" s="1">
+        <v>0</v>
+      </c>
+      <c r="H223" s="1">
+        <v>1</v>
+      </c>
+      <c r="I223" s="1">
+        <v>0</v>
+      </c>
+      <c r="J223" s="1">
+        <v>0</v>
+      </c>
+      <c r="K223" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E223,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B224" s="6">
+        <v>4332</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E224" s="3">
+        <f>IF($A224="","",$A224-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F224" s="4">
+        <v>0</v>
+      </c>
+      <c r="G224" s="1">
+        <v>0</v>
+      </c>
+      <c r="H224" s="1">
+        <v>1</v>
+      </c>
+      <c r="I224" s="1">
+        <v>0</v>
+      </c>
+      <c r="J224" s="1">
+        <v>0</v>
+      </c>
+      <c r="K224" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E224,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B225" s="6">
+        <v>4929</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E225" s="3">
+        <f>IF($A225="","",$A225-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F225" s="4">
+        <v>0</v>
+      </c>
+      <c r="G225" s="1">
+        <v>0</v>
+      </c>
+      <c r="H225" s="1">
+        <v>1</v>
+      </c>
+      <c r="I225" s="1">
+        <v>0</v>
+      </c>
+      <c r="J225" s="1">
+        <v>0</v>
+      </c>
+      <c r="K225" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E225,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B226" s="6">
+        <v>3957</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E226" s="3">
+        <f>IF($A226="","",$A226-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F226" s="4">
+        <v>0</v>
+      </c>
+      <c r="G226" s="1">
+        <v>0</v>
+      </c>
+      <c r="H226" s="1">
+        <v>1</v>
+      </c>
+      <c r="I226" s="1">
+        <v>0</v>
+      </c>
+      <c r="J226" s="1">
+        <v>0</v>
+      </c>
+      <c r="K226" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E226,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B227" s="6">
+        <v>7448</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E227" s="3">
+        <f>IF($A227="","",$A227-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F227" s="4">
+        <v>0</v>
+      </c>
+      <c r="G227" s="1">
+        <v>0</v>
+      </c>
+      <c r="H227" s="1">
+        <v>1</v>
+      </c>
+      <c r="I227" s="1">
+        <v>0</v>
+      </c>
+      <c r="J227" s="1">
+        <v>0</v>
+      </c>
+      <c r="K227" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E227,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B228" s="6">
+        <v>3579</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E228" s="3">
+        <f>IF($A228="","",$A228-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F228" s="4">
+        <v>0</v>
+      </c>
+      <c r="G228" s="1">
+        <v>0</v>
+      </c>
+      <c r="H228" s="1">
+        <v>1</v>
+      </c>
+      <c r="I228" s="1">
+        <v>0</v>
+      </c>
+      <c r="J228" s="1">
+        <v>0</v>
+      </c>
+      <c r="K228" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E228,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B229" s="6">
+        <v>8461</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E229" s="3">
+        <f>IF($A229="","",$A229-1)</f>
+        <v>45026</v>
+      </c>
+      <c r="F229" s="4">
+        <v>0</v>
+      </c>
+      <c r="G229" s="1">
+        <v>0</v>
+      </c>
+      <c r="H229" s="1">
+        <v>1</v>
+      </c>
+      <c r="I229" s="1">
+        <v>0</v>
+      </c>
+      <c r="J229" s="1">
+        <v>0</v>
+      </c>
+      <c r="K229" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E229,"DD"))),0),"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B230" s="6">
+        <v>8699</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E230" s="3">
+        <f>IF($A230="","",$A230-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F230" s="4">
+        <v>0</v>
+      </c>
+      <c r="G230" s="1">
+        <v>0</v>
+      </c>
+      <c r="H230" s="1">
+        <v>0</v>
+      </c>
+      <c r="I230" s="1">
+        <v>0</v>
+      </c>
+      <c r="J230" s="1">
+        <v>1</v>
+      </c>
+      <c r="K230" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E230,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B231" s="6">
+        <v>3474</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E231" s="3">
+        <f>IF($A231="","",$A231-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F231" s="4">
+        <v>0</v>
+      </c>
+      <c r="G231" s="1">
+        <v>0</v>
+      </c>
+      <c r="H231" s="1">
+        <v>0</v>
+      </c>
+      <c r="I231" s="1">
+        <v>0</v>
+      </c>
+      <c r="J231" s="1">
+        <v>1</v>
+      </c>
+      <c r="K231" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E231,"DD"))),0),"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B232" s="6">
+        <v>2518</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E232" s="3">
+        <f>IF($A232="","",$A232-1)</f>
+        <v>45025</v>
+      </c>
+      <c r="F232" s="4">
+        <v>0</v>
+      </c>
+      <c r="G232" s="1">
+        <v>0</v>
+      </c>
+      <c r="H232" s="1">
+        <v>0</v>
+      </c>
+      <c r="I232" s="1">
+        <v>1</v>
+      </c>
+      <c r="J232" s="1">
+        <v>0</v>
+      </c>
+      <c r="K232" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E232,"DD"))),0),"")</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J166" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J232" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B166" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B232" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2 B138 B96" numberStoredAsText="1"/>
+    <ignoredError sqref="B2 B138 B96 B198" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
datos del dia 13/04
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DD40D3-4467-49A9-BD42-73F25CFA8423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176F96B9-0261-4F04-AB4D-34445B8256EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="1950" yWindow="810" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="163">
   <si>
     <t>Usuario</t>
   </si>
@@ -784,6 +784,24 @@
   <si>
     <t>Despedida Demoníaca</t>
   </si>
+  <si>
+    <t>Evil Eye</t>
+  </si>
+  <si>
+    <t>Rápido como el Viento</t>
+  </si>
+  <si>
+    <t>Camino de la Estrella Fugaz</t>
+  </si>
+  <si>
+    <t>Campos de Guerrero</t>
+  </si>
+  <si>
+    <t>Amazoness</t>
+  </si>
+  <si>
+    <t>Robo de Magia Trampa</t>
+  </si>
 </sst>
 </file>
 
@@ -1117,8 +1135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K375" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K375" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K408" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K408" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1437,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K375"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="G233" sqref="G233:G235 I233:I235 H233:H236 H237:I237 G237:G239 H239:H240 G241:H241 I239:I243 H243:H244 H245:I250 G244:G247 J233:J252 H253:J254 I256 H256:H260 G261 I258:I270 F248:F277 H271:H277 G263:G289 G291:G294 I278:I294 H279:H296 G296:G297 H298 I296:I299 H300:I300 G299:G302 H302:I307 H309:H315 J256:J327 H329 I309:I330 F303:F335 J331:J335 I336:J349 G316:G343 H331:H348 H350:J355 G345:G351 H357:H360 J357:J360 F352:F363 H362:H363 F364:G371 I357:I369 J362:J370 I371:J371 F372:I374 F375:H375 J375"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G413" sqref="G413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10045,7 +10063,7 @@
         <v>21</v>
       </c>
       <c r="E233" s="3">
-        <f>IF($A233="","",$A233-1)</f>
+        <f t="shared" ref="E233:E264" si="16">IF($A233="","",$A233-1)</f>
         <v>45026</v>
       </c>
       <c r="F233" s="4">
@@ -10064,7 +10082,7 @@
         <v>0</v>
       </c>
       <c r="K233" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E233,"DD"))),0),"")</f>
+        <f t="shared" ref="K233:K264" si="17">IFERROR(ROUND((VALUE(TEXT($E233,"DD"))),0),"")</f>
         <v>10</v>
       </c>
     </row>
@@ -10082,7 +10100,7 @@
         <v>19</v>
       </c>
       <c r="E234" s="3">
-        <f>IF($A234="","",$A234-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F234" s="4">
@@ -10101,7 +10119,7 @@
         <v>0</v>
       </c>
       <c r="K234" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E234,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10119,7 +10137,7 @@
         <v>58</v>
       </c>
       <c r="E235" s="3">
-        <f>IF($A235="","",$A235-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F235" s="4">
@@ -10138,7 +10156,7 @@
         <v>0</v>
       </c>
       <c r="K235" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E235,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10156,7 +10174,7 @@
         <v>29</v>
       </c>
       <c r="E236" s="3">
-        <f>IF($A236="","",$A236-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F236" s="4">
@@ -10175,7 +10193,7 @@
         <v>0</v>
       </c>
       <c r="K236" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E236,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10193,7 +10211,7 @@
         <v>23</v>
       </c>
       <c r="E237" s="3">
-        <f>IF($A237="","",$A237-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F237" s="4">
@@ -10212,7 +10230,7 @@
         <v>0</v>
       </c>
       <c r="K237" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E237,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10230,7 +10248,7 @@
         <v>29</v>
       </c>
       <c r="E238" s="3">
-        <f>IF($A238="","",$A238-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F238" s="4">
@@ -10249,7 +10267,7 @@
         <v>0</v>
       </c>
       <c r="K238" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E238,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10267,7 +10285,7 @@
         <v>60</v>
       </c>
       <c r="E239" s="3">
-        <f>IF($A239="","",$A239-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F239" s="4">
@@ -10286,7 +10304,7 @@
         <v>0</v>
       </c>
       <c r="K239" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E239,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10304,7 +10322,7 @@
         <v>35</v>
       </c>
       <c r="E240" s="3">
-        <f>IF($A240="","",$A240-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F240" s="4">
@@ -10323,7 +10341,7 @@
         <v>0</v>
       </c>
       <c r="K240" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E240,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10341,7 +10359,7 @@
         <v>33</v>
       </c>
       <c r="E241" s="3">
-        <f>IF($A241="","",$A241-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F241" s="4">
@@ -10360,7 +10378,7 @@
         <v>0</v>
       </c>
       <c r="K241" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E241,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10378,7 +10396,7 @@
         <v>58</v>
       </c>
       <c r="E242" s="3">
-        <f>IF($A242="","",$A242-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F242" s="4">
@@ -10397,7 +10415,7 @@
         <v>0</v>
       </c>
       <c r="K242" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E242,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10415,7 +10433,7 @@
         <v>80</v>
       </c>
       <c r="E243" s="3">
-        <f>IF($A243="","",$A243-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F243" s="4">
@@ -10434,7 +10452,7 @@
         <v>0</v>
       </c>
       <c r="K243" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E243,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10452,7 +10470,7 @@
         <v>82</v>
       </c>
       <c r="E244" s="3">
-        <f>IF($A244="","",$A244-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F244" s="4">
@@ -10471,7 +10489,7 @@
         <v>0</v>
       </c>
       <c r="K244" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E244,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10489,7 +10507,7 @@
         <v>98</v>
       </c>
       <c r="E245" s="3">
-        <f>IF($A245="","",$A245-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F245" s="4">
@@ -10508,7 +10526,7 @@
         <v>0</v>
       </c>
       <c r="K245" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E245,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10526,7 +10544,7 @@
         <v>29</v>
       </c>
       <c r="E246" s="3">
-        <f>IF($A246="","",$A246-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F246" s="4">
@@ -10545,7 +10563,7 @@
         <v>0</v>
       </c>
       <c r="K246" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E246,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10563,7 +10581,7 @@
         <v>81</v>
       </c>
       <c r="E247" s="3">
-        <f>IF($A247="","",$A247-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F247" s="4">
@@ -10582,7 +10600,7 @@
         <v>0</v>
       </c>
       <c r="K247" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E247,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10600,7 +10618,7 @@
         <v>49</v>
       </c>
       <c r="E248" s="3">
-        <f>IF($A248="","",$A248-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F248" s="4">
@@ -10619,7 +10637,7 @@
         <v>0</v>
       </c>
       <c r="K248" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E248,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10637,7 +10655,7 @@
         <v>43</v>
       </c>
       <c r="E249" s="3">
-        <f>IF($A249="","",$A249-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F249" s="4">
@@ -10656,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="K249" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E249,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10674,7 +10692,7 @@
         <v>45</v>
       </c>
       <c r="E250" s="3">
-        <f>IF($A250="","",$A250-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F250" s="4">
@@ -10693,7 +10711,7 @@
         <v>0</v>
       </c>
       <c r="K250" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E250,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10711,7 +10729,7 @@
         <v>17</v>
       </c>
       <c r="E251" s="3">
-        <f>IF($A251="","",$A251-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F251" s="4">
@@ -10730,7 +10748,7 @@
         <v>0</v>
       </c>
       <c r="K251" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E251,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10748,7 +10766,7 @@
         <v>128</v>
       </c>
       <c r="E252" s="3">
-        <f>IF($A252="","",$A252-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F252" s="4">
@@ -10767,7 +10785,7 @@
         <v>0</v>
       </c>
       <c r="K252" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E252,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10785,7 +10803,7 @@
         <v>130</v>
       </c>
       <c r="E253" s="3">
-        <f>IF($A253="","",$A253-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F253" s="4">
@@ -10804,7 +10822,7 @@
         <v>0</v>
       </c>
       <c r="K253" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E253,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10822,7 +10840,7 @@
         <v>98</v>
       </c>
       <c r="E254" s="3">
-        <f>IF($A254="","",$A254-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F254" s="4">
@@ -10841,7 +10859,7 @@
         <v>0</v>
       </c>
       <c r="K254" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E254,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10859,7 +10877,7 @@
         <v>43</v>
       </c>
       <c r="E255" s="3">
-        <f>IF($A255="","",$A255-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F255" s="4">
@@ -10878,7 +10896,7 @@
         <v>1</v>
       </c>
       <c r="K255" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E255,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10896,7 +10914,7 @@
         <v>24</v>
       </c>
       <c r="E256" s="3">
-        <f>IF($A256="","",$A256-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F256" s="4">
@@ -10915,7 +10933,7 @@
         <v>0</v>
       </c>
       <c r="K256" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E256,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10933,7 +10951,7 @@
         <v>15</v>
       </c>
       <c r="E257" s="3">
-        <f>IF($A257="","",$A257-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F257" s="4">
@@ -10952,7 +10970,7 @@
         <v>0</v>
       </c>
       <c r="K257" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E257,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -10970,7 +10988,7 @@
         <v>60</v>
       </c>
       <c r="E258" s="3">
-        <f>IF($A258="","",$A258-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F258" s="4">
@@ -10989,7 +11007,7 @@
         <v>0</v>
       </c>
       <c r="K258" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E258,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11007,7 +11025,7 @@
         <v>58</v>
       </c>
       <c r="E259" s="3">
-        <f>IF($A259="","",$A259-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F259" s="4">
@@ -11026,7 +11044,7 @@
         <v>0</v>
       </c>
       <c r="K259" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E259,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11044,7 +11062,7 @@
         <v>58</v>
       </c>
       <c r="E260" s="3">
-        <f>IF($A260="","",$A260-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F260" s="4">
@@ -11063,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="K260" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E260,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11081,7 +11099,7 @@
         <v>71</v>
       </c>
       <c r="E261" s="3">
-        <f>IF($A261="","",$A261-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F261" s="4">
@@ -11100,7 +11118,7 @@
         <v>0</v>
       </c>
       <c r="K261" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E261,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11118,7 +11136,7 @@
         <v>132</v>
       </c>
       <c r="E262" s="3">
-        <f>IF($A262="","",$A262-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F262" s="4">
@@ -11137,7 +11155,7 @@
         <v>0</v>
       </c>
       <c r="K262" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E262,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11155,7 +11173,7 @@
         <v>24</v>
       </c>
       <c r="E263" s="3">
-        <f>IF($A263="","",$A263-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F263" s="4">
@@ -11174,7 +11192,7 @@
         <v>0</v>
       </c>
       <c r="K263" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E263,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11192,7 +11210,7 @@
         <v>29</v>
       </c>
       <c r="E264" s="3">
-        <f>IF($A264="","",$A264-1)</f>
+        <f t="shared" si="16"/>
         <v>45026</v>
       </c>
       <c r="F264" s="4">
@@ -11211,7 +11229,7 @@
         <v>0</v>
       </c>
       <c r="K264" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E264,"DD"))),0),"")</f>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
     </row>
@@ -11229,7 +11247,7 @@
         <v>58</v>
       </c>
       <c r="E265" s="3">
-        <f>IF($A265="","",$A265-1)</f>
+        <f t="shared" ref="E265:E296" si="18">IF($A265="","",$A265-1)</f>
         <v>45026</v>
       </c>
       <c r="F265" s="4">
@@ -11248,7 +11266,7 @@
         <v>0</v>
       </c>
       <c r="K265" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E265,"DD"))),0),"")</f>
+        <f t="shared" ref="K265:K296" si="19">IFERROR(ROUND((VALUE(TEXT($E265,"DD"))),0),"")</f>
         <v>10</v>
       </c>
     </row>
@@ -11266,7 +11284,7 @@
         <v>45</v>
       </c>
       <c r="E266" s="3">
-        <f>IF($A266="","",$A266-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F266" s="4">
@@ -11285,7 +11303,7 @@
         <v>0</v>
       </c>
       <c r="K266" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E266,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11303,7 +11321,7 @@
         <v>134</v>
       </c>
       <c r="E267" s="3">
-        <f>IF($A267="","",$A267-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F267" s="4">
@@ -11322,7 +11340,7 @@
         <v>0</v>
       </c>
       <c r="K267" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E267,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11340,7 +11358,7 @@
         <v>58</v>
       </c>
       <c r="E268" s="3">
-        <f>IF($A268="","",$A268-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F268" s="4">
@@ -11359,7 +11377,7 @@
         <v>0</v>
       </c>
       <c r="K268" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E268,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11377,7 +11395,7 @@
         <v>56</v>
       </c>
       <c r="E269" s="3">
-        <f>IF($A269="","",$A269-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F269" s="4">
@@ -11396,7 +11414,7 @@
         <v>0</v>
       </c>
       <c r="K269" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E269,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11414,7 +11432,7 @@
         <v>45</v>
       </c>
       <c r="E270" s="3">
-        <f>IF($A270="","",$A270-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F270" s="4">
@@ -11433,7 +11451,7 @@
         <v>0</v>
       </c>
       <c r="K270" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E270,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11451,7 +11469,7 @@
         <v>81</v>
       </c>
       <c r="E271" s="3">
-        <f>IF($A271="","",$A271-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F271" s="4">
@@ -11470,7 +11488,7 @@
         <v>0</v>
       </c>
       <c r="K271" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E271,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11488,7 +11506,7 @@
         <v>98</v>
       </c>
       <c r="E272" s="3">
-        <f>IF($A272="","",$A272-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F272" s="4">
@@ -11507,7 +11525,7 @@
         <v>0</v>
       </c>
       <c r="K272" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E272,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11525,7 +11543,7 @@
         <v>29</v>
       </c>
       <c r="E273" s="3">
-        <f>IF($A273="","",$A273-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F273" s="4">
@@ -11544,7 +11562,7 @@
         <v>0</v>
       </c>
       <c r="K273" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E273,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11562,7 +11580,7 @@
         <v>27</v>
       </c>
       <c r="E274" s="3">
-        <f>IF($A274="","",$A274-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F274" s="4">
@@ -11581,7 +11599,7 @@
         <v>0</v>
       </c>
       <c r="K274" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E274,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11599,7 +11617,7 @@
         <v>136</v>
       </c>
       <c r="E275" s="3">
-        <f>IF($A275="","",$A275-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F275" s="4">
@@ -11618,7 +11636,7 @@
         <v>0</v>
       </c>
       <c r="K275" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E275,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11636,7 +11654,7 @@
         <v>17</v>
       </c>
       <c r="E276" s="3">
-        <f>IF($A276="","",$A276-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F276" s="4">
@@ -11655,7 +11673,7 @@
         <v>0</v>
       </c>
       <c r="K276" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E276,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11673,7 +11691,7 @@
         <v>80</v>
       </c>
       <c r="E277" s="3">
-        <f>IF($A277="","",$A277-1)</f>
+        <f t="shared" si="18"/>
         <v>45026</v>
       </c>
       <c r="F277" s="4">
@@ -11692,7 +11710,7 @@
         <v>0</v>
       </c>
       <c r="K277" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E277,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
     </row>
@@ -11710,7 +11728,7 @@
         <v>137</v>
       </c>
       <c r="E278" s="3">
-        <f>IF($A278="","",$A278-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F278" s="4">
@@ -11729,7 +11747,7 @@
         <v>0</v>
       </c>
       <c r="K278" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E278,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11747,7 +11765,7 @@
         <v>139</v>
       </c>
       <c r="E279" s="3">
-        <f>IF($A279="","",$A279-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F279" s="4">
@@ -11766,7 +11784,7 @@
         <v>0</v>
       </c>
       <c r="K279" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E279,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11784,7 +11802,7 @@
         <v>19</v>
       </c>
       <c r="E280" s="3">
-        <f>IF($A280="","",$A280-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F280" s="4">
@@ -11803,7 +11821,7 @@
         <v>0</v>
       </c>
       <c r="K280" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E280,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11821,7 +11839,7 @@
         <v>45</v>
       </c>
       <c r="E281" s="3">
-        <f>IF($A281="","",$A281-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F281" s="4">
@@ -11840,7 +11858,7 @@
         <v>0</v>
       </c>
       <c r="K281" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E281,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11858,7 +11876,7 @@
         <v>140</v>
       </c>
       <c r="E282" s="3">
-        <f>IF($A282="","",$A282-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F282" s="4">
@@ -11877,7 +11895,7 @@
         <v>0</v>
       </c>
       <c r="K282" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E282,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11895,7 +11913,7 @@
         <v>141</v>
       </c>
       <c r="E283" s="3">
-        <f>IF($A283="","",$A283-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F283" s="4">
@@ -11914,7 +11932,7 @@
         <v>0</v>
       </c>
       <c r="K283" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E283,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11932,7 +11950,7 @@
         <v>24</v>
       </c>
       <c r="E284" s="3">
-        <f>IF($A284="","",$A284-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F284" s="4">
@@ -11951,7 +11969,7 @@
         <v>0</v>
       </c>
       <c r="K284" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E284,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -11969,7 +11987,7 @@
         <v>62</v>
       </c>
       <c r="E285" s="3">
-        <f>IF($A285="","",$A285-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F285" s="4">
@@ -11988,7 +12006,7 @@
         <v>0</v>
       </c>
       <c r="K285" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E285,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12006,7 +12024,7 @@
         <v>21</v>
       </c>
       <c r="E286" s="3">
-        <f>IF($A286="","",$A286-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F286" s="4">
@@ -12025,7 +12043,7 @@
         <v>0</v>
       </c>
       <c r="K286" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E286,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12043,7 +12061,7 @@
         <v>66</v>
       </c>
       <c r="E287" s="3">
-        <f>IF($A287="","",$A287-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F287" s="4">
@@ -12062,7 +12080,7 @@
         <v>0</v>
       </c>
       <c r="K287" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E287,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12080,7 +12098,7 @@
         <v>45</v>
       </c>
       <c r="E288" s="3">
-        <f>IF($A288="","",$A288-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F288" s="4">
@@ -12099,7 +12117,7 @@
         <v>0</v>
       </c>
       <c r="K288" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E288,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12117,7 +12135,7 @@
         <v>24</v>
       </c>
       <c r="E289" s="3">
-        <f>IF($A289="","",$A289-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F289" s="4">
@@ -12136,7 +12154,7 @@
         <v>0</v>
       </c>
       <c r="K289" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E289,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12154,7 +12172,7 @@
         <v>55</v>
       </c>
       <c r="E290" s="3">
-        <f>IF($A290="","",$A290-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F290" s="4">
@@ -12173,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="K290" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E290,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12191,7 +12209,7 @@
         <v>60</v>
       </c>
       <c r="E291" s="3">
-        <f>IF($A291="","",$A291-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F291" s="4">
@@ -12210,7 +12228,7 @@
         <v>0</v>
       </c>
       <c r="K291" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E291,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12228,7 +12246,7 @@
         <v>39</v>
       </c>
       <c r="E292" s="3">
-        <f>IF($A292="","",$A292-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F292" s="4">
@@ -12247,7 +12265,7 @@
         <v>0</v>
       </c>
       <c r="K292" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E292,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12265,7 +12283,7 @@
         <v>98</v>
       </c>
       <c r="E293" s="3">
-        <f>IF($A293="","",$A293-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F293" s="4">
@@ -12284,7 +12302,7 @@
         <v>0</v>
       </c>
       <c r="K293" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E293,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12302,7 +12320,7 @@
         <v>58</v>
       </c>
       <c r="E294" s="3">
-        <f>IF($A294="","",$A294-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F294" s="4">
@@ -12321,7 +12339,7 @@
         <v>0</v>
       </c>
       <c r="K294" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E294,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12339,7 +12357,7 @@
         <v>39</v>
       </c>
       <c r="E295" s="3">
-        <f>IF($A295="","",$A295-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F295" s="4">
@@ -12358,7 +12376,7 @@
         <v>0</v>
       </c>
       <c r="K295" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E295,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12376,7 +12394,7 @@
         <v>29</v>
       </c>
       <c r="E296" s="3">
-        <f>IF($A296="","",$A296-1)</f>
+        <f t="shared" si="18"/>
         <v>45027</v>
       </c>
       <c r="F296" s="4">
@@ -12395,7 +12413,7 @@
         <v>0</v>
       </c>
       <c r="K296" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E296,"DD"))),0),"")</f>
+        <f t="shared" si="19"/>
         <v>11</v>
       </c>
     </row>
@@ -12413,7 +12431,7 @@
         <v>23</v>
       </c>
       <c r="E297" s="3">
-        <f>IF($A297="","",$A297-1)</f>
+        <f t="shared" ref="E297:E328" si="20">IF($A297="","",$A297-1)</f>
         <v>45027</v>
       </c>
       <c r="F297" s="4">
@@ -12432,7 +12450,7 @@
         <v>0</v>
       </c>
       <c r="K297" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E297,"DD"))),0),"")</f>
+        <f t="shared" ref="K297:K328" si="21">IFERROR(ROUND((VALUE(TEXT($E297,"DD"))),0),"")</f>
         <v>11</v>
       </c>
     </row>
@@ -12450,7 +12468,7 @@
         <v>142</v>
       </c>
       <c r="E298" s="3">
-        <f>IF($A298="","",$A298-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F298" s="4">
@@ -12469,7 +12487,7 @@
         <v>0</v>
       </c>
       <c r="K298" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E298,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12487,7 +12505,7 @@
         <v>144</v>
       </c>
       <c r="E299" s="3">
-        <f>IF($A299="","",$A299-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F299" s="4">
@@ -12506,7 +12524,7 @@
         <v>0</v>
       </c>
       <c r="K299" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E299,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12524,7 +12542,7 @@
         <v>146</v>
       </c>
       <c r="E300" s="3">
-        <f>IF($A300="","",$A300-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F300" s="4">
@@ -12543,7 +12561,7 @@
         <v>0</v>
       </c>
       <c r="K300" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E300,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12561,7 +12579,7 @@
         <v>144</v>
       </c>
       <c r="E301" s="3">
-        <f>IF($A301="","",$A301-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F301" s="4">
@@ -12580,7 +12598,7 @@
         <v>0</v>
       </c>
       <c r="K301" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E301,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12598,7 +12616,7 @@
         <v>45</v>
       </c>
       <c r="E302" s="3">
-        <f>IF($A302="","",$A302-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F302" s="4">
@@ -12617,7 +12635,7 @@
         <v>0</v>
       </c>
       <c r="K302" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E302,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12635,7 +12653,7 @@
         <v>29</v>
       </c>
       <c r="E303" s="3">
-        <f>IF($A303="","",$A303-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F303" s="4">
@@ -12654,7 +12672,7 @@
         <v>0</v>
       </c>
       <c r="K303" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E303,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12672,7 +12690,7 @@
         <v>39</v>
       </c>
       <c r="E304" s="3">
-        <f>IF($A304="","",$A304-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F304" s="4">
@@ -12691,7 +12709,7 @@
         <v>0</v>
       </c>
       <c r="K304" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E304,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12709,7 +12727,7 @@
         <v>62</v>
       </c>
       <c r="E305" s="3">
-        <f>IF($A305="","",$A305-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F305" s="4">
@@ -12728,7 +12746,7 @@
         <v>0</v>
       </c>
       <c r="K305" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E305,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12746,7 +12764,7 @@
         <v>19</v>
       </c>
       <c r="E306" s="3">
-        <f>IF($A306="","",$A306-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F306" s="4">
@@ -12765,7 +12783,7 @@
         <v>0</v>
       </c>
       <c r="K306" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E306,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12783,7 +12801,7 @@
         <v>98</v>
       </c>
       <c r="E307" s="3">
-        <f>IF($A307="","",$A307-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F307" s="4">
@@ -12802,7 +12820,7 @@
         <v>0</v>
       </c>
       <c r="K307" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E307,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12820,7 +12838,7 @@
         <v>24</v>
       </c>
       <c r="E308" s="3">
-        <f>IF($A308="","",$A308-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F308" s="4">
@@ -12839,7 +12857,7 @@
         <v>0</v>
       </c>
       <c r="K308" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E308,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12857,7 +12875,7 @@
         <v>45</v>
       </c>
       <c r="E309" s="3">
-        <f>IF($A309="","",$A309-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F309" s="4">
@@ -12876,7 +12894,7 @@
         <v>0</v>
       </c>
       <c r="K309" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E309,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12894,7 +12912,7 @@
         <v>33</v>
       </c>
       <c r="E310" s="3">
-        <f>IF($A310="","",$A310-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F310" s="4">
@@ -12913,7 +12931,7 @@
         <v>0</v>
       </c>
       <c r="K310" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E310,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12931,7 +12949,7 @@
         <v>23</v>
       </c>
       <c r="E311" s="3">
-        <f>IF($A311="","",$A311-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F311" s="4">
@@ -12950,7 +12968,7 @@
         <v>0</v>
       </c>
       <c r="K311" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E311,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -12968,7 +12986,7 @@
         <v>33</v>
       </c>
       <c r="E312" s="3">
-        <f>IF($A312="","",$A312-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F312" s="4">
@@ -12987,7 +13005,7 @@
         <v>0</v>
       </c>
       <c r="K312" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E312,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13005,7 +13023,7 @@
         <v>29</v>
       </c>
       <c r="E313" s="3">
-        <f>IF($A313="","",$A313-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F313" s="4">
@@ -13024,7 +13042,7 @@
         <v>0</v>
       </c>
       <c r="K313" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E313,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13042,7 +13060,7 @@
         <v>29</v>
       </c>
       <c r="E314" s="3">
-        <f>IF($A314="","",$A314-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F314" s="4">
@@ -13061,7 +13079,7 @@
         <v>0</v>
       </c>
       <c r="K314" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E314,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13079,7 +13097,7 @@
         <v>58</v>
       </c>
       <c r="E315" s="3">
-        <f>IF($A315="","",$A315-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F315" s="4">
@@ -13098,7 +13116,7 @@
         <v>0</v>
       </c>
       <c r="K315" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E315,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13116,7 +13134,7 @@
         <v>45</v>
       </c>
       <c r="E316" s="3">
-        <f>IF($A316="","",$A316-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F316" s="4">
@@ -13135,7 +13153,7 @@
         <v>0</v>
       </c>
       <c r="K316" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E316,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13153,7 +13171,7 @@
         <v>24</v>
       </c>
       <c r="E317" s="3">
-        <f>IF($A317="","",$A317-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F317" s="4">
@@ -13172,7 +13190,7 @@
         <v>0</v>
       </c>
       <c r="K317" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E317,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13190,7 +13208,7 @@
         <v>128</v>
       </c>
       <c r="E318" s="3">
-        <f>IF($A318="","",$A318-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F318" s="4">
@@ -13209,7 +13227,7 @@
         <v>0</v>
       </c>
       <c r="K318" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E318,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13227,7 +13245,7 @@
         <v>148</v>
       </c>
       <c r="E319" s="3">
-        <f>IF($A319="","",$A319-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F319" s="4">
@@ -13246,7 +13264,7 @@
         <v>0</v>
       </c>
       <c r="K319" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E319,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13264,7 +13282,7 @@
         <v>39</v>
       </c>
       <c r="E320" s="3">
-        <f>IF($A320="","",$A320-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F320" s="4">
@@ -13283,7 +13301,7 @@
         <v>0</v>
       </c>
       <c r="K320" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E320,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13301,7 +13319,7 @@
         <v>60</v>
       </c>
       <c r="E321" s="3">
-        <f>IF($A321="","",$A321-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F321" s="4">
@@ -13320,7 +13338,7 @@
         <v>0</v>
       </c>
       <c r="K321" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E321,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13338,7 +13356,7 @@
         <v>58</v>
       </c>
       <c r="E322" s="3">
-        <f>IF($A322="","",$A322-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F322" s="4">
@@ -13357,7 +13375,7 @@
         <v>0</v>
       </c>
       <c r="K322" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E322,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13375,7 +13393,7 @@
         <v>43</v>
       </c>
       <c r="E323" s="3">
-        <f>IF($A323="","",$A323-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F323" s="4">
@@ -13394,7 +13412,7 @@
         <v>0</v>
       </c>
       <c r="K323" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E323,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13412,7 +13430,7 @@
         <v>24</v>
       </c>
       <c r="E324" s="3">
-        <f>IF($A324="","",$A324-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F324" s="4">
@@ -13431,7 +13449,7 @@
         <v>0</v>
       </c>
       <c r="K324" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E324,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13449,7 +13467,7 @@
         <v>62</v>
       </c>
       <c r="E325" s="3">
-        <f>IF($A325="","",$A325-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F325" s="4">
@@ -13468,7 +13486,7 @@
         <v>0</v>
       </c>
       <c r="K325" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E325,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13486,7 +13504,7 @@
         <v>31</v>
       </c>
       <c r="E326" s="3">
-        <f>IF($A326="","",$A326-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F326" s="4">
@@ -13505,7 +13523,7 @@
         <v>0</v>
       </c>
       <c r="K326" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E326,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13523,7 +13541,7 @@
         <v>68</v>
       </c>
       <c r="E327" s="3">
-        <f>IF($A327="","",$A327-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F327" s="4">
@@ -13542,7 +13560,7 @@
         <v>0</v>
       </c>
       <c r="K327" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E327,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13560,7 +13578,7 @@
         <v>35</v>
       </c>
       <c r="E328" s="3">
-        <f>IF($A328="","",$A328-1)</f>
+        <f t="shared" si="20"/>
         <v>45027</v>
       </c>
       <c r="F328" s="4">
@@ -13579,7 +13597,7 @@
         <v>1</v>
       </c>
       <c r="K328" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E328,"DD"))),0),"")</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -13597,7 +13615,7 @@
         <v>111</v>
       </c>
       <c r="E329" s="3">
-        <f>IF($A329="","",$A329-1)</f>
+        <f t="shared" ref="E329:E360" si="22">IF($A329="","",$A329-1)</f>
         <v>45027</v>
       </c>
       <c r="F329" s="4">
@@ -13616,7 +13634,7 @@
         <v>1</v>
       </c>
       <c r="K329" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E329,"DD"))),0),"")</f>
+        <f t="shared" ref="K329:K360" si="23">IFERROR(ROUND((VALUE(TEXT($E329,"DD"))),0),"")</f>
         <v>11</v>
       </c>
     </row>
@@ -13634,7 +13652,7 @@
         <v>124</v>
       </c>
       <c r="E330" s="3">
-        <f>IF($A330="","",$A330-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F330" s="4">
@@ -13653,7 +13671,7 @@
         <v>1</v>
       </c>
       <c r="K330" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E330,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13671,7 +13689,7 @@
         <v>29</v>
       </c>
       <c r="E331" s="3">
-        <f>IF($A331="","",$A331-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F331" s="4">
@@ -13690,7 +13708,7 @@
         <v>0</v>
       </c>
       <c r="K331" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E331,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13708,7 +13726,7 @@
         <v>39</v>
       </c>
       <c r="E332" s="3">
-        <f>IF($A332="","",$A332-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F332" s="4">
@@ -13727,7 +13745,7 @@
         <v>0</v>
       </c>
       <c r="K332" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E332,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13745,7 +13763,7 @@
         <v>92</v>
       </c>
       <c r="E333" s="3">
-        <f>IF($A333="","",$A333-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F333" s="4">
@@ -13764,7 +13782,7 @@
         <v>0</v>
       </c>
       <c r="K333" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E333,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13782,7 +13800,7 @@
         <v>68</v>
       </c>
       <c r="E334" s="3">
-        <f>IF($A334="","",$A334-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F334" s="4">
@@ -13801,7 +13819,7 @@
         <v>0</v>
       </c>
       <c r="K334" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E334,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13819,7 +13837,7 @@
         <v>24</v>
       </c>
       <c r="E335" s="3">
-        <f>IF($A335="","",$A335-1)</f>
+        <f t="shared" si="22"/>
         <v>45027</v>
       </c>
       <c r="F335" s="4">
@@ -13838,7 +13856,7 @@
         <v>0</v>
       </c>
       <c r="K335" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E335,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>11</v>
       </c>
     </row>
@@ -13856,7 +13874,7 @@
         <v>43</v>
       </c>
       <c r="E336" s="3">
-        <f>IF($A336="","",$A336-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F336" s="4">
@@ -13875,7 +13893,7 @@
         <v>0</v>
       </c>
       <c r="K336" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E336,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -13893,7 +13911,7 @@
         <v>94</v>
       </c>
       <c r="E337" s="3">
-        <f>IF($A337="","",$A337-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F337" s="4">
@@ -13912,7 +13930,7 @@
         <v>0</v>
       </c>
       <c r="K337" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E337,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -13930,7 +13948,7 @@
         <v>29</v>
       </c>
       <c r="E338" s="3">
-        <f>IF($A338="","",$A338-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F338" s="4">
@@ -13949,7 +13967,7 @@
         <v>0</v>
       </c>
       <c r="K338" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E338,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -13967,7 +13985,7 @@
         <v>81</v>
       </c>
       <c r="E339" s="3">
-        <f>IF($A339="","",$A339-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F339" s="4">
@@ -13986,7 +14004,7 @@
         <v>0</v>
       </c>
       <c r="K339" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E339,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14004,7 +14022,7 @@
         <v>106</v>
       </c>
       <c r="E340" s="3">
-        <f>IF($A340="","",$A340-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F340" s="4">
@@ -14023,7 +14041,7 @@
         <v>0</v>
       </c>
       <c r="K340" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E340,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14041,7 +14059,7 @@
         <v>130</v>
       </c>
       <c r="E341" s="3">
-        <f>IF($A341="","",$A341-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F341" s="4">
@@ -14060,7 +14078,7 @@
         <v>0</v>
       </c>
       <c r="K341" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E341,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14078,7 +14096,7 @@
         <v>60</v>
       </c>
       <c r="E342" s="3">
-        <f>IF($A342="","",$A342-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F342" s="4">
@@ -14097,7 +14115,7 @@
         <v>0</v>
       </c>
       <c r="K342" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E342,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14115,7 +14133,7 @@
         <v>45</v>
       </c>
       <c r="E343" s="3">
-        <f>IF($A343="","",$A343-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F343" s="4">
@@ -14134,7 +14152,7 @@
         <v>0</v>
       </c>
       <c r="K343" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E343,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14152,7 +14170,7 @@
         <v>45</v>
       </c>
       <c r="E344" s="3">
-        <f>IF($A344="","",$A344-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F344" s="4">
@@ -14171,7 +14189,7 @@
         <v>0</v>
       </c>
       <c r="K344" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E344,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14189,7 +14207,7 @@
         <v>58</v>
       </c>
       <c r="E345" s="3">
-        <f>IF($A345="","",$A345-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F345" s="4">
@@ -14208,7 +14226,7 @@
         <v>0</v>
       </c>
       <c r="K345" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E345,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14226,7 +14244,7 @@
         <v>29</v>
       </c>
       <c r="E346" s="3">
-        <f>IF($A346="","",$A346-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F346" s="4">
@@ -14245,7 +14263,7 @@
         <v>0</v>
       </c>
       <c r="K346" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E346,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14263,7 +14281,7 @@
         <v>106</v>
       </c>
       <c r="E347" s="3">
-        <f>IF($A347="","",$A347-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F347" s="4">
@@ -14282,7 +14300,7 @@
         <v>0</v>
       </c>
       <c r="K347" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E347,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14300,7 +14318,7 @@
         <v>29</v>
       </c>
       <c r="E348" s="3">
-        <f>IF($A348="","",$A348-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F348" s="4">
@@ -14319,7 +14337,7 @@
         <v>0</v>
       </c>
       <c r="K348" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E348,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14337,7 +14355,7 @@
         <v>23</v>
       </c>
       <c r="E349" s="3">
-        <f>IF($A349="","",$A349-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F349" s="4">
@@ -14356,7 +14374,7 @@
         <v>0</v>
       </c>
       <c r="K349" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E349,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14374,7 +14392,7 @@
         <v>27</v>
       </c>
       <c r="E350" s="3">
-        <f>IF($A350="","",$A350-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F350" s="4">
@@ -14393,7 +14411,7 @@
         <v>0</v>
       </c>
       <c r="K350" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E350,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14411,7 +14429,7 @@
         <v>60</v>
       </c>
       <c r="E351" s="3">
-        <f>IF($A351="","",$A351-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F351" s="4">
@@ -14430,7 +14448,7 @@
         <v>0</v>
       </c>
       <c r="K351" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E351,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14448,7 +14466,7 @@
         <v>29</v>
       </c>
       <c r="E352" s="3">
-        <f>IF($A352="","",$A352-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F352" s="4">
@@ -14467,7 +14485,7 @@
         <v>0</v>
       </c>
       <c r="K352" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E352,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14485,7 +14503,7 @@
         <v>55</v>
       </c>
       <c r="E353" s="3">
-        <f>IF($A353="","",$A353-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F353" s="4">
@@ -14504,7 +14522,7 @@
         <v>0</v>
       </c>
       <c r="K353" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E353,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14522,7 +14540,7 @@
         <v>23</v>
       </c>
       <c r="E354" s="3">
-        <f>IF($A354="","",$A354-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F354" s="4">
@@ -14541,7 +14559,7 @@
         <v>0</v>
       </c>
       <c r="K354" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E354,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14559,7 +14577,7 @@
         <v>17</v>
       </c>
       <c r="E355" s="3">
-        <f>IF($A355="","",$A355-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F355" s="4">
@@ -14578,7 +14596,7 @@
         <v>0</v>
       </c>
       <c r="K355" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E355,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14596,7 +14614,7 @@
         <v>98</v>
       </c>
       <c r="E356" s="3">
-        <f>IF($A356="","",$A356-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F356" s="4">
@@ -14615,7 +14633,7 @@
         <v>1</v>
       </c>
       <c r="K356" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E356,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14633,7 +14651,7 @@
         <v>13</v>
       </c>
       <c r="E357" s="3">
-        <f>IF($A357="","",$A357-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F357" s="4">
@@ -14652,7 +14670,7 @@
         <v>0</v>
       </c>
       <c r="K357" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E357,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14670,7 +14688,7 @@
         <v>98</v>
       </c>
       <c r="E358" s="3">
-        <f>IF($A358="","",$A358-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F358" s="4">
@@ -14689,7 +14707,7 @@
         <v>0</v>
       </c>
       <c r="K358" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E358,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14707,7 +14725,7 @@
         <v>31</v>
       </c>
       <c r="E359" s="3">
-        <f>IF($A359="","",$A359-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F359" s="4">
@@ -14726,7 +14744,7 @@
         <v>0</v>
       </c>
       <c r="K359" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E359,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14744,7 +14762,7 @@
         <v>56</v>
       </c>
       <c r="E360" s="3">
-        <f>IF($A360="","",$A360-1)</f>
+        <f t="shared" si="22"/>
         <v>45028</v>
       </c>
       <c r="F360" s="4">
@@ -14763,7 +14781,7 @@
         <v>0</v>
       </c>
       <c r="K360" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E360,"DD"))),0),"")</f>
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
     </row>
@@ -14781,7 +14799,7 @@
         <v>91</v>
       </c>
       <c r="E361" s="3">
-        <f>IF($A361="","",$A361-1)</f>
+        <f t="shared" ref="E361:E375" si="24">IF($A361="","",$A361-1)</f>
         <v>45028</v>
       </c>
       <c r="F361" s="4">
@@ -14800,7 +14818,7 @@
         <v>1</v>
       </c>
       <c r="K361" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E361,"DD"))),0),"")</f>
+        <f t="shared" ref="K361:K375" si="25">IFERROR(ROUND((VALUE(TEXT($E361,"DD"))),0),"")</f>
         <v>12</v>
       </c>
     </row>
@@ -14818,7 +14836,7 @@
         <v>15</v>
       </c>
       <c r="E362" s="3">
-        <f>IF($A362="","",$A362-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F362" s="4">
@@ -14837,7 +14855,7 @@
         <v>0</v>
       </c>
       <c r="K362" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E362,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -14855,7 +14873,7 @@
         <v>141</v>
       </c>
       <c r="E363" s="3">
-        <f>IF($A363="","",$A363-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F363" s="4">
@@ -14874,7 +14892,7 @@
         <v>0</v>
       </c>
       <c r="K363" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E363,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -14892,7 +14910,7 @@
         <v>71</v>
       </c>
       <c r="E364" s="3">
-        <f>IF($A364="","",$A364-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F364" s="4">
@@ -14911,7 +14929,7 @@
         <v>0</v>
       </c>
       <c r="K364" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E364,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -14929,7 +14947,7 @@
         <v>153</v>
       </c>
       <c r="E365" s="3">
-        <f>IF($A365="","",$A365-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F365" s="4">
@@ -14948,7 +14966,7 @@
         <v>0</v>
       </c>
       <c r="K365" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E365,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -14966,7 +14984,7 @@
         <v>23</v>
       </c>
       <c r="E366" s="3">
-        <f>IF($A366="","",$A366-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F366" s="4">
@@ -14985,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="K366" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E366,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15003,7 +15021,7 @@
         <v>58</v>
       </c>
       <c r="E367" s="3">
-        <f>IF($A367="","",$A367-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F367" s="4">
@@ -15022,7 +15040,7 @@
         <v>0</v>
       </c>
       <c r="K367" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E367,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15040,7 +15058,7 @@
         <v>53</v>
       </c>
       <c r="E368" s="3">
-        <f>IF($A368="","",$A368-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F368" s="4">
@@ -15059,7 +15077,7 @@
         <v>0</v>
       </c>
       <c r="K368" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E368,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15077,7 +15095,7 @@
         <v>58</v>
       </c>
       <c r="E369" s="3">
-        <f>IF($A369="","",$A369-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F369" s="4">
@@ -15096,7 +15114,7 @@
         <v>0</v>
       </c>
       <c r="K369" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E369,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15114,7 +15132,7 @@
         <v>62</v>
       </c>
       <c r="E370" s="3">
-        <f>IF($A370="","",$A370-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F370" s="4">
@@ -15133,7 +15151,7 @@
         <v>0</v>
       </c>
       <c r="K370" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E370,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15151,7 +15169,7 @@
         <v>155</v>
       </c>
       <c r="E371" s="3">
-        <f>IF($A371="","",$A371-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F371" s="4">
@@ -15170,7 +15188,7 @@
         <v>0</v>
       </c>
       <c r="K371" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E371,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15188,7 +15206,7 @@
         <v>43</v>
       </c>
       <c r="E372" s="3">
-        <f>IF($A372="","",$A372-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F372" s="4">
@@ -15207,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="K372" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E372,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15225,7 +15243,7 @@
         <v>156</v>
       </c>
       <c r="E373" s="3">
-        <f>IF($A373="","",$A373-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F373" s="4">
@@ -15244,7 +15262,7 @@
         <v>1</v>
       </c>
       <c r="K373" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E373,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15262,7 +15280,7 @@
         <v>56</v>
       </c>
       <c r="E374" s="3">
-        <f>IF($A374="","",$A374-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F374" s="4">
@@ -15281,7 +15299,7 @@
         <v>1</v>
       </c>
       <c r="K374" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E374,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
     </row>
@@ -15299,7 +15317,7 @@
         <v>19</v>
       </c>
       <c r="E375" s="3">
-        <f>IF($A375="","",$A375-1)</f>
+        <f t="shared" si="24"/>
         <v>45028</v>
       </c>
       <c r="F375" s="4">
@@ -15318,17 +15336,1238 @@
         <v>0</v>
       </c>
       <c r="K375" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E375,"DD"))),0),"")</f>
+        <f t="shared" si="25"/>
         <v>12</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A376" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B376" s="6">
+        <v>349</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E376" s="3">
+        <f>IF($A376="","",$A376-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F376" s="4">
+        <v>1</v>
+      </c>
+      <c r="G376" s="1">
+        <v>1</v>
+      </c>
+      <c r="H376" s="1">
+        <v>1</v>
+      </c>
+      <c r="I376" s="1">
+        <v>0</v>
+      </c>
+      <c r="J376" s="1">
+        <v>0</v>
+      </c>
+      <c r="K376" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E376,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A377" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B377" s="6">
+        <v>311</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E377" s="3">
+        <f>IF($A377="","",$A377-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F377" s="4">
+        <v>1</v>
+      </c>
+      <c r="G377" s="1">
+        <v>0</v>
+      </c>
+      <c r="H377" s="1">
+        <v>0</v>
+      </c>
+      <c r="I377" s="1">
+        <v>0</v>
+      </c>
+      <c r="J377" s="1">
+        <v>0</v>
+      </c>
+      <c r="K377" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E377,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A378" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B378" s="6">
+        <v>5077</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E378" s="3">
+        <f>IF($A378="","",$A378-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F378" s="4">
+        <v>1</v>
+      </c>
+      <c r="G378" s="1">
+        <v>0</v>
+      </c>
+      <c r="H378" s="1">
+        <v>0</v>
+      </c>
+      <c r="I378" s="1">
+        <v>0</v>
+      </c>
+      <c r="J378" s="1">
+        <v>0</v>
+      </c>
+      <c r="K378" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E378,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A379" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B379" s="6">
+        <v>7455</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E379" s="3">
+        <f>IF($A379="","",$A379-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F379" s="4">
+        <v>1</v>
+      </c>
+      <c r="G379" s="1">
+        <v>0</v>
+      </c>
+      <c r="H379" s="1">
+        <v>0</v>
+      </c>
+      <c r="I379" s="1">
+        <v>0</v>
+      </c>
+      <c r="J379" s="1">
+        <v>0</v>
+      </c>
+      <c r="K379" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E379,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A380" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B380" s="6">
+        <v>2102</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E380" s="3">
+        <f>IF($A380="","",$A380-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F380" s="4">
+        <v>1</v>
+      </c>
+      <c r="G380" s="1">
+        <v>0</v>
+      </c>
+      <c r="H380" s="1">
+        <v>1</v>
+      </c>
+      <c r="I380" s="1">
+        <v>0</v>
+      </c>
+      <c r="J380" s="1">
+        <v>0</v>
+      </c>
+      <c r="K380" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E380,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A381" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B381" s="6">
+        <v>3874</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E381" s="3">
+        <f>IF($A381="","",$A381-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F381" s="4">
+        <v>1</v>
+      </c>
+      <c r="G381" s="1">
+        <v>0</v>
+      </c>
+      <c r="H381" s="1">
+        <v>1</v>
+      </c>
+      <c r="I381" s="1">
+        <v>0</v>
+      </c>
+      <c r="J381" s="1">
+        <v>0</v>
+      </c>
+      <c r="K381" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E381,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A382" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B382" s="6">
+        <v>2007</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E382" s="3">
+        <f>IF($A382="","",$A382-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F382" s="4">
+        <v>1</v>
+      </c>
+      <c r="G382" s="1">
+        <v>0</v>
+      </c>
+      <c r="H382" s="1">
+        <v>0</v>
+      </c>
+      <c r="I382" s="1">
+        <v>0</v>
+      </c>
+      <c r="J382" s="1">
+        <v>0</v>
+      </c>
+      <c r="K382" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E382,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A383" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B383" s="6">
+        <v>7928</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E383" s="3">
+        <f>IF($A383="","",$A383-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F383" s="4">
+        <v>1</v>
+      </c>
+      <c r="G383" s="1">
+        <v>0</v>
+      </c>
+      <c r="H383" s="1">
+        <v>0</v>
+      </c>
+      <c r="I383" s="1">
+        <v>0</v>
+      </c>
+      <c r="J383" s="1">
+        <v>0</v>
+      </c>
+      <c r="K383" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E383,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A384" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B384" s="6">
+        <v>2117</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E384" s="3">
+        <f>IF($A384="","",$A384-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F384" s="4">
+        <v>1</v>
+      </c>
+      <c r="G384" s="1">
+        <v>0</v>
+      </c>
+      <c r="H384" s="1">
+        <v>0</v>
+      </c>
+      <c r="I384" s="1">
+        <v>0</v>
+      </c>
+      <c r="J384" s="1">
+        <v>0</v>
+      </c>
+      <c r="K384" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E384,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B385" s="6">
+        <v>2401</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E385" s="3">
+        <f>IF($A385="","",$A385-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F385" s="4">
+        <v>1</v>
+      </c>
+      <c r="G385" s="1">
+        <v>0</v>
+      </c>
+      <c r="H385" s="1">
+        <v>0</v>
+      </c>
+      <c r="I385" s="1">
+        <v>0</v>
+      </c>
+      <c r="J385" s="1">
+        <v>0</v>
+      </c>
+      <c r="K385" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E385,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A386" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B386" s="6">
+        <v>8673</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E386" s="3">
+        <f>IF($A386="","",$A386-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F386" s="4">
+        <v>1</v>
+      </c>
+      <c r="G386" s="1">
+        <v>0</v>
+      </c>
+      <c r="H386" s="1">
+        <v>0</v>
+      </c>
+      <c r="I386" s="1">
+        <v>0</v>
+      </c>
+      <c r="J386" s="1">
+        <v>0</v>
+      </c>
+      <c r="K386" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E386,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A387" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B387" s="6">
+        <v>1965</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E387" s="3">
+        <f>IF($A387="","",$A387-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F387" s="4">
+        <v>1</v>
+      </c>
+      <c r="G387" s="1">
+        <v>0</v>
+      </c>
+      <c r="H387" s="1">
+        <v>1</v>
+      </c>
+      <c r="I387" s="1">
+        <v>0</v>
+      </c>
+      <c r="J387" s="1">
+        <v>0</v>
+      </c>
+      <c r="K387" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E387,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A388" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B388" s="6">
+        <v>3523</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E388" s="3">
+        <f>IF($A388="","",$A388-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F388" s="4">
+        <v>0</v>
+      </c>
+      <c r="G388" s="1">
+        <v>1</v>
+      </c>
+      <c r="H388" s="1">
+        <v>0</v>
+      </c>
+      <c r="I388" s="1">
+        <v>0</v>
+      </c>
+      <c r="J388" s="1">
+        <v>0</v>
+      </c>
+      <c r="K388" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E388,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A389" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B389" s="6">
+        <v>3181</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E389" s="3">
+        <f>IF($A389="","",$A389-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F389" s="4">
+        <v>0</v>
+      </c>
+      <c r="G389" s="1">
+        <v>1</v>
+      </c>
+      <c r="H389" s="1">
+        <v>0</v>
+      </c>
+      <c r="I389" s="1">
+        <v>0</v>
+      </c>
+      <c r="J389" s="1">
+        <v>0</v>
+      </c>
+      <c r="K389" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E389,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A390" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B390" s="6">
+        <v>2841</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E390" s="3">
+        <f>IF($A390="","",$A390-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F390" s="4">
+        <v>0</v>
+      </c>
+      <c r="G390" s="1">
+        <v>1</v>
+      </c>
+      <c r="H390" s="1">
+        <v>0</v>
+      </c>
+      <c r="I390" s="1">
+        <v>0</v>
+      </c>
+      <c r="J390" s="1">
+        <v>0</v>
+      </c>
+      <c r="K390" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E390,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A391" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B391" s="6">
+        <v>9310</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E391" s="3">
+        <f>IF($A391="","",$A391-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F391" s="4">
+        <v>0</v>
+      </c>
+      <c r="G391" s="1">
+        <v>1</v>
+      </c>
+      <c r="H391" s="1">
+        <v>0</v>
+      </c>
+      <c r="I391" s="1">
+        <v>0</v>
+      </c>
+      <c r="J391" s="1">
+        <v>0</v>
+      </c>
+      <c r="K391" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E391,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A392" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B392" s="6">
+        <v>7964</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E392" s="3">
+        <f>IF($A392="","",$A392-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F392" s="4">
+        <v>0</v>
+      </c>
+      <c r="G392" s="1">
+        <v>1</v>
+      </c>
+      <c r="H392" s="1">
+        <v>0</v>
+      </c>
+      <c r="I392" s="1">
+        <v>0</v>
+      </c>
+      <c r="J392" s="1">
+        <v>0</v>
+      </c>
+      <c r="K392" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E392,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A393" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B393" s="6">
+        <v>8504</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E393" s="3">
+        <f>IF($A393="","",$A393-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F393" s="4">
+        <v>0</v>
+      </c>
+      <c r="G393" s="1">
+        <v>1</v>
+      </c>
+      <c r="H393" s="1">
+        <v>0</v>
+      </c>
+      <c r="I393" s="1">
+        <v>0</v>
+      </c>
+      <c r="J393" s="1">
+        <v>0</v>
+      </c>
+      <c r="K393" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E393,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A394" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B394" s="6">
+        <v>4067</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E394" s="3">
+        <f>IF($A394="","",$A394-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F394" s="4">
+        <v>0</v>
+      </c>
+      <c r="G394" s="1">
+        <v>1</v>
+      </c>
+      <c r="H394" s="1">
+        <v>0</v>
+      </c>
+      <c r="I394" s="1">
+        <v>0</v>
+      </c>
+      <c r="J394" s="1">
+        <v>0</v>
+      </c>
+      <c r="K394" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E394,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A395" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B395" s="6">
+        <v>1068</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E395" s="3">
+        <f>IF($A395="","",$A395-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F395" s="4">
+        <v>0</v>
+      </c>
+      <c r="G395" s="1">
+        <v>1</v>
+      </c>
+      <c r="H395" s="1">
+        <v>0</v>
+      </c>
+      <c r="I395" s="1">
+        <v>0</v>
+      </c>
+      <c r="J395" s="1">
+        <v>0</v>
+      </c>
+      <c r="K395" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E395,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A396" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B396" s="6">
+        <v>8214</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E396" s="3">
+        <f>IF($A396="","",$A396-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F396" s="4">
+        <v>0</v>
+      </c>
+      <c r="G396" s="1">
+        <v>1</v>
+      </c>
+      <c r="H396" s="1">
+        <v>0</v>
+      </c>
+      <c r="I396" s="1">
+        <v>0</v>
+      </c>
+      <c r="J396" s="1">
+        <v>0</v>
+      </c>
+      <c r="K396" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E396,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A397" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B397" s="6">
+        <v>254</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E397" s="3">
+        <f>IF($A397="","",$A397-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F397" s="4">
+        <v>0</v>
+      </c>
+      <c r="G397" s="1">
+        <v>1</v>
+      </c>
+      <c r="H397" s="1">
+        <v>0</v>
+      </c>
+      <c r="I397" s="1">
+        <v>0</v>
+      </c>
+      <c r="J397" s="1">
+        <v>0</v>
+      </c>
+      <c r="K397" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E397,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A398" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B398" s="6">
+        <v>5209</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E398" s="3">
+        <f>IF($A398="","",$A398-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F398" s="4">
+        <v>0</v>
+      </c>
+      <c r="G398" s="1">
+        <v>1</v>
+      </c>
+      <c r="H398" s="1">
+        <v>0</v>
+      </c>
+      <c r="I398" s="1">
+        <v>0</v>
+      </c>
+      <c r="J398" s="1">
+        <v>0</v>
+      </c>
+      <c r="K398" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E398,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A399" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B399" s="6">
+        <v>7437</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E399" s="3">
+        <f>IF($A399="","",$A399-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F399" s="4">
+        <v>0</v>
+      </c>
+      <c r="G399" s="1">
+        <v>0</v>
+      </c>
+      <c r="H399" s="1">
+        <v>1</v>
+      </c>
+      <c r="I399" s="1">
+        <v>0</v>
+      </c>
+      <c r="J399" s="1">
+        <v>0</v>
+      </c>
+      <c r="K399" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E399,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A400" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B400" s="6">
+        <v>1831</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E400" s="3">
+        <f>IF($A400="","",$A400-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F400" s="4">
+        <v>0</v>
+      </c>
+      <c r="G400" s="1">
+        <v>0</v>
+      </c>
+      <c r="H400" s="1">
+        <v>1</v>
+      </c>
+      <c r="I400" s="1">
+        <v>0</v>
+      </c>
+      <c r="J400" s="1">
+        <v>0</v>
+      </c>
+      <c r="K400" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E400,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A401" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B401" s="6">
+        <v>9718</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E401" s="3">
+        <f>IF($A401="","",$A401-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F401" s="4">
+        <v>0</v>
+      </c>
+      <c r="G401" s="1">
+        <v>0</v>
+      </c>
+      <c r="H401" s="1">
+        <v>1</v>
+      </c>
+      <c r="I401" s="1">
+        <v>0</v>
+      </c>
+      <c r="J401" s="1">
+        <v>0</v>
+      </c>
+      <c r="K401" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E401,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B402" s="6">
+        <v>6704</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E402" s="3">
+        <f>IF($A402="","",$A402-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F402" s="4">
+        <v>0</v>
+      </c>
+      <c r="G402" s="1">
+        <v>0</v>
+      </c>
+      <c r="H402" s="1">
+        <v>1</v>
+      </c>
+      <c r="I402" s="1">
+        <v>0</v>
+      </c>
+      <c r="J402" s="1">
+        <v>0</v>
+      </c>
+      <c r="K402" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E402,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B403" s="6">
+        <v>6026</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D403" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E403" s="3">
+        <f>IF($A403="","",$A403-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F403" s="4">
+        <v>0</v>
+      </c>
+      <c r="G403" s="1">
+        <v>0</v>
+      </c>
+      <c r="H403" s="1">
+        <v>1</v>
+      </c>
+      <c r="I403" s="1">
+        <v>0</v>
+      </c>
+      <c r="J403" s="1">
+        <v>0</v>
+      </c>
+      <c r="K403" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E403,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B404" s="6">
+        <v>1206</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E404" s="3">
+        <f>IF($A404="","",$A404-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F404" s="4">
+        <v>0</v>
+      </c>
+      <c r="G404" s="1">
+        <v>0</v>
+      </c>
+      <c r="H404" s="1">
+        <v>1</v>
+      </c>
+      <c r="I404" s="1">
+        <v>0</v>
+      </c>
+      <c r="J404" s="1">
+        <v>0</v>
+      </c>
+      <c r="K404" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E404,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B405" s="6">
+        <v>2009</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E405" s="3">
+        <f>IF($A405="","",$A405-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F405" s="4">
+        <v>0</v>
+      </c>
+      <c r="G405" s="1">
+        <v>0</v>
+      </c>
+      <c r="H405" s="1">
+        <v>1</v>
+      </c>
+      <c r="I405" s="1">
+        <v>0</v>
+      </c>
+      <c r="J405" s="1">
+        <v>0</v>
+      </c>
+      <c r="K405" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E405,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A406" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B406" s="6">
+        <v>7531</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E406" s="3">
+        <f>IF($A406="","",$A406-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F406" s="4">
+        <v>0</v>
+      </c>
+      <c r="G406" s="1">
+        <v>0</v>
+      </c>
+      <c r="H406" s="1">
+        <v>1</v>
+      </c>
+      <c r="I406" s="1">
+        <v>0</v>
+      </c>
+      <c r="J406" s="1">
+        <v>0</v>
+      </c>
+      <c r="K406" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E406,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A407" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B407" s="6">
+        <v>2171</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E407" s="3">
+        <f>IF($A407="","",$A407-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F407" s="4">
+        <v>0</v>
+      </c>
+      <c r="G407" s="1">
+        <v>0</v>
+      </c>
+      <c r="H407" s="1">
+        <v>1</v>
+      </c>
+      <c r="I407" s="1">
+        <v>0</v>
+      </c>
+      <c r="J407" s="1">
+        <v>0</v>
+      </c>
+      <c r="K407" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E407,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B408" s="6">
+        <v>7590</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E408" s="3">
+        <f>IF($A408="","",$A408-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F408" s="4">
+        <v>1</v>
+      </c>
+      <c r="G408" s="1">
+        <v>0</v>
+      </c>
+      <c r="H408" s="1">
+        <v>0</v>
+      </c>
+      <c r="I408" s="1">
+        <v>0</v>
+      </c>
+      <c r="J408" s="1">
+        <v>0</v>
+      </c>
+      <c r="K408" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E408,"DD"))),0),"")</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J375" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J408" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B375" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B408" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
       <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
datos de los dias 14 y 15
</commit_message>
<xml_diff>
--- a/kcapril23.xlsx
+++ b/kcapril23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\lucelprojects\reportes-KC\april-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176F96B9-0261-4F04-AB4D-34445B8256EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F0886E-4507-490D-B471-A3780F63515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="810" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="12750" windowHeight="10710" xr2:uid="{984710A1-F493-455E-BFAC-E04028477DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseKC" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="170">
   <si>
     <t>Usuario</t>
   </si>
@@ -802,6 +802,27 @@
   <si>
     <t>Robo de Magia Trampa</t>
   </si>
+  <si>
+    <t>Qliphort</t>
+  </si>
+  <si>
+    <t>Borre Explosivo</t>
+  </si>
+  <si>
+    <t>Buster Blader</t>
+  </si>
+  <si>
+    <t>6107</t>
+  </si>
+  <si>
+    <t>Onomat</t>
+  </si>
+  <si>
+    <t>Carga de Ataque</t>
+  </si>
+  <si>
+    <t>Resonancia Demoníaca</t>
+  </si>
 </sst>
 </file>
 
@@ -1135,8 +1156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K408" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K408" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}" name="kcapril23" displayName="kcapril23" ref="A1:K453" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K453" xr:uid="{36430D63-CF3A-436C-963D-3ABC1624405B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{15450D09-0A7B-494C-AA5C-944D6334AF73}" name="Registro Insertado" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4E592176-A1D7-4E6C-ABFF-82B903A2C483}" name="Usuario" dataDxfId="9"/>
@@ -1455,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8F445-F0CB-4732-BEA9-5D3B18714E30}">
-  <dimension ref="A1:K408"/>
+  <dimension ref="A1:K453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G413" sqref="G413"/>
+    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
+      <selection activeCell="F452" sqref="F452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13887,7 +13908,7 @@
         <v>0</v>
       </c>
       <c r="I336" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J336" s="1">
         <v>0</v>
@@ -15354,7 +15375,7 @@
         <v>158</v>
       </c>
       <c r="E376" s="3">
-        <f>IF($A376="","",$A376-1)</f>
+        <f t="shared" ref="E376:E408" si="26">IF($A376="","",$A376-1)</f>
         <v>45029</v>
       </c>
       <c r="F376" s="4">
@@ -15373,7 +15394,7 @@
         <v>0</v>
       </c>
       <c r="K376" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E376,"DD"))),0),"")</f>
+        <f t="shared" ref="K376:K408" si="27">IFERROR(ROUND((VALUE(TEXT($E376,"DD"))),0),"")</f>
         <v>13</v>
       </c>
     </row>
@@ -15391,7 +15412,7 @@
         <v>23</v>
       </c>
       <c r="E377" s="3">
-        <f>IF($A377="","",$A377-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F377" s="4">
@@ -15410,7 +15431,7 @@
         <v>0</v>
       </c>
       <c r="K377" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E377,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15428,7 +15449,7 @@
         <v>159</v>
       </c>
       <c r="E378" s="3">
-        <f>IF($A378="","",$A378-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F378" s="4">
@@ -15447,7 +15468,7 @@
         <v>0</v>
       </c>
       <c r="K378" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E378,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15465,7 +15486,7 @@
         <v>58</v>
       </c>
       <c r="E379" s="3">
-        <f>IF($A379="","",$A379-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F379" s="4">
@@ -15484,7 +15505,7 @@
         <v>0</v>
       </c>
       <c r="K379" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E379,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15502,7 +15523,7 @@
         <v>71</v>
       </c>
       <c r="E380" s="3">
-        <f>IF($A380="","",$A380-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F380" s="4">
@@ -15515,13 +15536,13 @@
         <v>1</v>
       </c>
       <c r="I380" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J380" s="1">
         <v>0</v>
       </c>
       <c r="K380" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E380,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15539,7 +15560,7 @@
         <v>43</v>
       </c>
       <c r="E381" s="3">
-        <f>IF($A381="","",$A381-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F381" s="4">
@@ -15558,7 +15579,7 @@
         <v>0</v>
       </c>
       <c r="K381" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E381,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15576,7 +15597,7 @@
         <v>60</v>
       </c>
       <c r="E382" s="3">
-        <f>IF($A382="","",$A382-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F382" s="4">
@@ -15595,7 +15616,7 @@
         <v>0</v>
       </c>
       <c r="K382" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E382,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15613,7 +15634,7 @@
         <v>71</v>
       </c>
       <c r="E383" s="3">
-        <f>IF($A383="","",$A383-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F383" s="4">
@@ -15632,7 +15653,7 @@
         <v>0</v>
       </c>
       <c r="K383" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E383,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15650,7 +15671,7 @@
         <v>160</v>
       </c>
       <c r="E384" s="3">
-        <f>IF($A384="","",$A384-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F384" s="4">
@@ -15669,7 +15690,7 @@
         <v>0</v>
       </c>
       <c r="K384" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E384,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15687,7 +15708,7 @@
         <v>29</v>
       </c>
       <c r="E385" s="3">
-        <f>IF($A385="","",$A385-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F385" s="4">
@@ -15706,7 +15727,7 @@
         <v>0</v>
       </c>
       <c r="K385" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E385,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15724,7 +15745,7 @@
         <v>23</v>
       </c>
       <c r="E386" s="3">
-        <f>IF($A386="","",$A386-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F386" s="4">
@@ -15743,7 +15764,7 @@
         <v>0</v>
       </c>
       <c r="K386" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E386,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15761,7 +15782,7 @@
         <v>39</v>
       </c>
       <c r="E387" s="3">
-        <f>IF($A387="","",$A387-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F387" s="4">
@@ -15780,7 +15801,7 @@
         <v>0</v>
       </c>
       <c r="K387" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E387,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15798,7 +15819,7 @@
         <v>29</v>
       </c>
       <c r="E388" s="3">
-        <f>IF($A388="","",$A388-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F388" s="4">
@@ -15817,7 +15838,7 @@
         <v>0</v>
       </c>
       <c r="K388" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E388,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15835,7 +15856,7 @@
         <v>35</v>
       </c>
       <c r="E389" s="3">
-        <f>IF($A389="","",$A389-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F389" s="4">
@@ -15854,7 +15875,7 @@
         <v>0</v>
       </c>
       <c r="K389" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E389,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15872,7 +15893,7 @@
         <v>15</v>
       </c>
       <c r="E390" s="3">
-        <f>IF($A390="","",$A390-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F390" s="4">
@@ -15891,7 +15912,7 @@
         <v>0</v>
       </c>
       <c r="K390" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E390,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15909,7 +15930,7 @@
         <v>99</v>
       </c>
       <c r="E391" s="3">
-        <f>IF($A391="","",$A391-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F391" s="4">
@@ -15928,7 +15949,7 @@
         <v>0</v>
       </c>
       <c r="K391" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E391,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15946,7 +15967,7 @@
         <v>23</v>
       </c>
       <c r="E392" s="3">
-        <f>IF($A392="","",$A392-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F392" s="4">
@@ -15965,7 +15986,7 @@
         <v>0</v>
       </c>
       <c r="K392" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E392,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -15983,7 +16004,7 @@
         <v>162</v>
       </c>
       <c r="E393" s="3">
-        <f>IF($A393="","",$A393-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F393" s="4">
@@ -16002,7 +16023,7 @@
         <v>0</v>
       </c>
       <c r="K393" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E393,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16020,7 +16041,7 @@
         <v>31</v>
       </c>
       <c r="E394" s="3">
-        <f>IF($A394="","",$A394-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F394" s="4">
@@ -16039,7 +16060,7 @@
         <v>0</v>
       </c>
       <c r="K394" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E394,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16057,7 +16078,7 @@
         <v>35</v>
       </c>
       <c r="E395" s="3">
-        <f>IF($A395="","",$A395-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F395" s="4">
@@ -16076,7 +16097,7 @@
         <v>0</v>
       </c>
       <c r="K395" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E395,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16094,7 +16115,7 @@
         <v>71</v>
       </c>
       <c r="E396" s="3">
-        <f>IF($A396="","",$A396-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F396" s="4">
@@ -16113,7 +16134,7 @@
         <v>0</v>
       </c>
       <c r="K396" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E396,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16131,7 +16152,7 @@
         <v>29</v>
       </c>
       <c r="E397" s="3">
-        <f>IF($A397="","",$A397-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F397" s="4">
@@ -16150,7 +16171,7 @@
         <v>0</v>
       </c>
       <c r="K397" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E397,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16168,7 +16189,7 @@
         <v>13</v>
       </c>
       <c r="E398" s="3">
-        <f>IF($A398="","",$A398-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F398" s="4">
@@ -16187,7 +16208,7 @@
         <v>0</v>
       </c>
       <c r="K398" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E398,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16205,7 +16226,7 @@
         <v>39</v>
       </c>
       <c r="E399" s="3">
-        <f>IF($A399="","",$A399-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F399" s="4">
@@ -16218,13 +16239,13 @@
         <v>1</v>
       </c>
       <c r="I399" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J399" s="1">
         <v>0</v>
       </c>
       <c r="K399" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E399,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16242,7 +16263,7 @@
         <v>35</v>
       </c>
       <c r="E400" s="3">
-        <f>IF($A400="","",$A400-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F400" s="4">
@@ -16261,7 +16282,7 @@
         <v>0</v>
       </c>
       <c r="K400" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E400,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16279,7 +16300,7 @@
         <v>45</v>
       </c>
       <c r="E401" s="3">
-        <f>IF($A401="","",$A401-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F401" s="4">
@@ -16298,7 +16319,7 @@
         <v>0</v>
       </c>
       <c r="K401" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E401,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16316,7 +16337,7 @@
         <v>29</v>
       </c>
       <c r="E402" s="3">
-        <f>IF($A402="","",$A402-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F402" s="4">
@@ -16335,7 +16356,7 @@
         <v>0</v>
       </c>
       <c r="K402" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E402,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16353,7 +16374,7 @@
         <v>43</v>
       </c>
       <c r="E403" s="3">
-        <f>IF($A403="","",$A403-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F403" s="4">
@@ -16372,7 +16393,7 @@
         <v>0</v>
       </c>
       <c r="K403" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E403,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16390,7 +16411,7 @@
         <v>17</v>
       </c>
       <c r="E404" s="3">
-        <f>IF($A404="","",$A404-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F404" s="4">
@@ -16409,7 +16430,7 @@
         <v>0</v>
       </c>
       <c r="K404" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E404,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16427,7 +16448,7 @@
         <v>45</v>
       </c>
       <c r="E405" s="3">
-        <f>IF($A405="","",$A405-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F405" s="4">
@@ -16446,7 +16467,7 @@
         <v>0</v>
       </c>
       <c r="K405" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E405,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16464,7 +16485,7 @@
         <v>124</v>
       </c>
       <c r="E406" s="3">
-        <f>IF($A406="","",$A406-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F406" s="4">
@@ -16483,7 +16504,7 @@
         <v>0</v>
       </c>
       <c r="K406" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E406,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16501,7 +16522,7 @@
         <v>23</v>
       </c>
       <c r="E407" s="3">
-        <f>IF($A407="","",$A407-1)</f>
+        <f t="shared" si="26"/>
         <v>45029</v>
       </c>
       <c r="F407" s="4">
@@ -16520,7 +16541,7 @@
         <v>0</v>
       </c>
       <c r="K407" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E407,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
     </row>
@@ -16538,7 +16559,7 @@
         <v>124</v>
       </c>
       <c r="E408" s="3">
-        <f>IF($A408="","",$A408-1)</f>
+        <f t="shared" si="26"/>
         <v>45030</v>
       </c>
       <c r="F408" s="4">
@@ -16557,24 +16578,1686 @@
         <v>0</v>
       </c>
       <c r="K408" s="1">
-        <f>IFERROR(ROUND((VALUE(TEXT($E408,"DD"))),0),"")</f>
+        <f t="shared" si="27"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A409" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B409" s="6">
+        <v>9404</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E409" s="3">
+        <f>IF($A409="","",$A409-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F409" s="4">
+        <v>1</v>
+      </c>
+      <c r="G409" s="1">
+        <v>0</v>
+      </c>
+      <c r="H409" s="1">
+        <v>0</v>
+      </c>
+      <c r="I409" s="1">
+        <v>0</v>
+      </c>
+      <c r="J409" s="1">
+        <v>0</v>
+      </c>
+      <c r="K409" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E409,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A410" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B410" s="6">
+        <v>3348</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E410" s="3">
+        <f>IF($A410="","",$A410-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F410" s="4">
+        <v>1</v>
+      </c>
+      <c r="G410" s="1">
+        <v>0</v>
+      </c>
+      <c r="H410" s="1">
+        <v>0</v>
+      </c>
+      <c r="I410" s="1">
+        <v>0</v>
+      </c>
+      <c r="J410" s="1">
+        <v>0</v>
+      </c>
+      <c r="K410" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E410,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A411" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B411" s="6">
+        <v>4657</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E411" s="3">
+        <f>IF($A411="","",$A411-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F411" s="4">
+        <v>1</v>
+      </c>
+      <c r="G411" s="1">
+        <v>0</v>
+      </c>
+      <c r="H411" s="1">
+        <v>1</v>
+      </c>
+      <c r="I411" s="1">
+        <v>0</v>
+      </c>
+      <c r="J411" s="1">
+        <v>1</v>
+      </c>
+      <c r="K411" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E411,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A412" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B412" s="6">
+        <v>5679</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E412" s="3">
+        <f>IF($A412="","",$A412-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F412" s="4">
+        <v>1</v>
+      </c>
+      <c r="G412" s="1">
+        <v>0</v>
+      </c>
+      <c r="H412" s="1">
+        <v>0</v>
+      </c>
+      <c r="I412" s="1">
+        <v>1</v>
+      </c>
+      <c r="J412" s="1">
+        <v>0</v>
+      </c>
+      <c r="K412" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E412,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A413" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B413" s="6">
+        <v>3717</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E413" s="3">
+        <f>IF($A413="","",$A413-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F413" s="4">
+        <v>1</v>
+      </c>
+      <c r="G413" s="1">
+        <v>0</v>
+      </c>
+      <c r="H413" s="1">
+        <v>0</v>
+      </c>
+      <c r="I413" s="1">
+        <v>0</v>
+      </c>
+      <c r="J413" s="1">
+        <v>0</v>
+      </c>
+      <c r="K413" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E413,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A414" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B414" s="6">
+        <v>9664</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E414" s="3">
+        <f>IF($A414="","",$A414-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F414" s="4">
+        <v>1</v>
+      </c>
+      <c r="G414" s="1">
+        <v>0</v>
+      </c>
+      <c r="H414" s="1">
+        <v>0</v>
+      </c>
+      <c r="I414" s="1">
+        <v>0</v>
+      </c>
+      <c r="J414" s="1">
+        <v>0</v>
+      </c>
+      <c r="K414" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E414,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A415" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B415" s="6">
+        <v>5900</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E415" s="3">
+        <f>IF($A415="","",$A415-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F415" s="4">
+        <v>1</v>
+      </c>
+      <c r="G415" s="1">
+        <v>1</v>
+      </c>
+      <c r="H415" s="1">
+        <v>1</v>
+      </c>
+      <c r="I415" s="1">
+        <v>1</v>
+      </c>
+      <c r="J415" s="1">
+        <v>0</v>
+      </c>
+      <c r="K415" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E415,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A416" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B416" s="6">
+        <v>9117</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E416" s="3">
+        <f>IF($A416="","",$A416-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F416" s="4">
+        <v>1</v>
+      </c>
+      <c r="G416" s="1">
+        <v>0</v>
+      </c>
+      <c r="H416" s="1">
+        <v>0</v>
+      </c>
+      <c r="I416" s="1">
+        <v>0</v>
+      </c>
+      <c r="J416" s="1">
+        <v>0</v>
+      </c>
+      <c r="K416" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E416,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A417" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B417" s="6">
+        <v>3667</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E417" s="3">
+        <f>IF($A417="","",$A417-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F417" s="4">
+        <v>1</v>
+      </c>
+      <c r="G417" s="1">
+        <v>1</v>
+      </c>
+      <c r="H417" s="1">
+        <v>1</v>
+      </c>
+      <c r="I417" s="1">
+        <v>0</v>
+      </c>
+      <c r="J417" s="1">
+        <v>0</v>
+      </c>
+      <c r="K417" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E417,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A418" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B418" s="6">
+        <v>9952</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E418" s="3">
+        <f>IF($A418="","",$A418-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F418" s="4">
+        <v>1</v>
+      </c>
+      <c r="G418" s="1">
+        <v>0</v>
+      </c>
+      <c r="H418" s="1">
+        <v>0</v>
+      </c>
+      <c r="I418" s="1">
+        <v>0</v>
+      </c>
+      <c r="J418" s="1">
+        <v>0</v>
+      </c>
+      <c r="K418" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E418,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A419" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B419" s="6">
+        <v>3372</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E419" s="3">
+        <f>IF($A419="","",$A419-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F419" s="4">
+        <v>1</v>
+      </c>
+      <c r="G419" s="1">
+        <v>0</v>
+      </c>
+      <c r="H419" s="1">
+        <v>0</v>
+      </c>
+      <c r="I419" s="1">
+        <v>0</v>
+      </c>
+      <c r="J419" s="1">
+        <v>0</v>
+      </c>
+      <c r="K419" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E419,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A420" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B420" s="6">
+        <v>4058</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D420" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E420" s="3">
+        <f>IF($A420="","",$A420-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F420" s="4">
+        <v>1</v>
+      </c>
+      <c r="G420" s="1">
+        <v>0</v>
+      </c>
+      <c r="H420" s="1">
+        <v>0</v>
+      </c>
+      <c r="I420" s="1">
+        <v>0</v>
+      </c>
+      <c r="J420" s="1">
+        <v>0</v>
+      </c>
+      <c r="K420" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E420,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A421" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B421" s="6">
+        <v>8367</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E421" s="3">
+        <f>IF($A421="","",$A421-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F421" s="4">
+        <v>1</v>
+      </c>
+      <c r="G421" s="1">
+        <v>0</v>
+      </c>
+      <c r="H421" s="1">
+        <v>0</v>
+      </c>
+      <c r="I421" s="1">
+        <v>0</v>
+      </c>
+      <c r="J421" s="1">
+        <v>0</v>
+      </c>
+      <c r="K421" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E421,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A422" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B422" s="6">
+        <v>5051</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E422" s="3">
+        <f>IF($A422="","",$A422-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F422" s="4">
+        <v>0</v>
+      </c>
+      <c r="G422" s="1">
+        <v>1</v>
+      </c>
+      <c r="H422" s="1">
+        <v>0</v>
+      </c>
+      <c r="I422" s="1">
+        <v>0</v>
+      </c>
+      <c r="J422" s="1">
+        <v>0</v>
+      </c>
+      <c r="K422" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E422,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A423" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B423" s="6">
+        <v>91</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E423" s="3">
+        <f>IF($A423="","",$A423-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F423" s="4">
+        <v>0</v>
+      </c>
+      <c r="G423" s="1">
+        <v>1</v>
+      </c>
+      <c r="H423" s="1">
+        <v>0</v>
+      </c>
+      <c r="I423" s="1">
+        <v>0</v>
+      </c>
+      <c r="J423" s="1">
+        <v>0</v>
+      </c>
+      <c r="K423" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E423,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A424" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B424" s="6">
+        <v>2284</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E424" s="3">
+        <f>IF($A424="","",$A424-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F424" s="4">
+        <v>0</v>
+      </c>
+      <c r="G424" s="1">
+        <v>1</v>
+      </c>
+      <c r="H424" s="1">
+        <v>0</v>
+      </c>
+      <c r="I424" s="1">
+        <v>0</v>
+      </c>
+      <c r="J424" s="1">
+        <v>0</v>
+      </c>
+      <c r="K424" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E424,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A425" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B425" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E425" s="3">
+        <f>IF($A425="","",$A425-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F425" s="4">
+        <v>0</v>
+      </c>
+      <c r="G425" s="1">
+        <v>1</v>
+      </c>
+      <c r="H425" s="1">
+        <v>0</v>
+      </c>
+      <c r="I425" s="1">
+        <v>0</v>
+      </c>
+      <c r="J425" s="1">
+        <v>0</v>
+      </c>
+      <c r="K425" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E425,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A426" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B426" s="6">
+        <v>7846</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E426" s="3">
+        <f>IF($A426="","",$A426-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F426" s="4">
+        <v>0</v>
+      </c>
+      <c r="G426" s="1">
+        <v>1</v>
+      </c>
+      <c r="H426" s="1">
+        <v>0</v>
+      </c>
+      <c r="I426" s="1">
+        <v>0</v>
+      </c>
+      <c r="J426" s="1">
+        <v>0</v>
+      </c>
+      <c r="K426" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E426,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A427" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B427" s="6">
+        <v>5520</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E427" s="3">
+        <f>IF($A427="","",$A427-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F427" s="4">
+        <v>0</v>
+      </c>
+      <c r="G427" s="1">
+        <v>1</v>
+      </c>
+      <c r="H427" s="1">
+        <v>0</v>
+      </c>
+      <c r="I427" s="1">
+        <v>0</v>
+      </c>
+      <c r="J427" s="1">
+        <v>0</v>
+      </c>
+      <c r="K427" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E427,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A428" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B428" s="6">
+        <v>2475</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E428" s="3">
+        <f>IF($A428="","",$A428-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F428" s="4">
+        <v>0</v>
+      </c>
+      <c r="G428" s="1">
+        <v>1</v>
+      </c>
+      <c r="H428" s="1">
+        <v>0</v>
+      </c>
+      <c r="I428" s="1">
+        <v>0</v>
+      </c>
+      <c r="J428" s="1">
+        <v>0</v>
+      </c>
+      <c r="K428" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E428,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B429" s="6">
+        <v>1270</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E429" s="3">
+        <f>IF($A429="","",$A429-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F429" s="4">
+        <v>0</v>
+      </c>
+      <c r="G429" s="1">
+        <v>1</v>
+      </c>
+      <c r="H429" s="1">
+        <v>0</v>
+      </c>
+      <c r="I429" s="1">
+        <v>0</v>
+      </c>
+      <c r="J429" s="1">
+        <v>0</v>
+      </c>
+      <c r="K429" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E429,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A430" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B430" s="6">
+        <v>1427</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E430" s="3">
+        <f>IF($A430="","",$A430-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F430" s="4">
+        <v>0</v>
+      </c>
+      <c r="G430" s="1">
+        <v>1</v>
+      </c>
+      <c r="H430" s="1">
+        <v>0</v>
+      </c>
+      <c r="I430" s="1">
+        <v>0</v>
+      </c>
+      <c r="J430" s="1">
+        <v>0</v>
+      </c>
+      <c r="K430" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E430,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A431" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B431" s="6">
+        <v>8707</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E431" s="3">
+        <f>IF($A431="","",$A431-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F431" s="4">
+        <v>0</v>
+      </c>
+      <c r="G431" s="1">
+        <v>1</v>
+      </c>
+      <c r="H431" s="1">
+        <v>0</v>
+      </c>
+      <c r="I431" s="1">
+        <v>0</v>
+      </c>
+      <c r="J431" s="1">
+        <v>0</v>
+      </c>
+      <c r="K431" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E431,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A432" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B432" s="6">
+        <v>1075</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E432" s="3">
+        <f>IF($A432="","",$A432-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F432" s="4">
+        <v>0</v>
+      </c>
+      <c r="G432" s="1">
+        <v>1</v>
+      </c>
+      <c r="H432" s="1">
+        <v>1</v>
+      </c>
+      <c r="I432" s="1">
+        <v>0</v>
+      </c>
+      <c r="J432" s="1">
+        <v>0</v>
+      </c>
+      <c r="K432" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E432,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A433" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B433" s="6">
+        <v>2959</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E433" s="3">
+        <f>IF($A433="","",$A433-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F433" s="4">
+        <v>0</v>
+      </c>
+      <c r="G433" s="1">
+        <v>1</v>
+      </c>
+      <c r="H433" s="1">
+        <v>0</v>
+      </c>
+      <c r="I433" s="1">
+        <v>0</v>
+      </c>
+      <c r="J433" s="1">
+        <v>0</v>
+      </c>
+      <c r="K433" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E433,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A434" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B434" s="6">
+        <v>7806</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E434" s="3">
+        <f>IF($A434="","",$A434-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F434" s="4">
+        <v>0</v>
+      </c>
+      <c r="G434" s="1">
+        <v>1</v>
+      </c>
+      <c r="H434" s="1">
+        <v>0</v>
+      </c>
+      <c r="I434" s="1">
+        <v>0</v>
+      </c>
+      <c r="J434" s="1">
+        <v>0</v>
+      </c>
+      <c r="K434" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E434,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A435" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B435" s="6">
+        <v>1900</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E435" s="3">
+        <f>IF($A435="","",$A435-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F435" s="4">
+        <v>0</v>
+      </c>
+      <c r="G435" s="1">
+        <v>1</v>
+      </c>
+      <c r="H435" s="1">
+        <v>0</v>
+      </c>
+      <c r="I435" s="1">
+        <v>0</v>
+      </c>
+      <c r="J435" s="1">
+        <v>0</v>
+      </c>
+      <c r="K435" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E435,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A436" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B436" s="6">
+        <v>7735</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D436" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E436" s="3">
+        <f>IF($A436="","",$A436-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F436" s="4">
+        <v>0</v>
+      </c>
+      <c r="G436" s="1">
+        <v>1</v>
+      </c>
+      <c r="H436" s="1">
+        <v>0</v>
+      </c>
+      <c r="I436" s="1">
+        <v>0</v>
+      </c>
+      <c r="J436" s="1">
+        <v>0</v>
+      </c>
+      <c r="K436" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E436,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A437" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B437" s="6">
+        <v>5924</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E437" s="3">
+        <f>IF($A437="","",$A437-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F437" s="4">
+        <v>0</v>
+      </c>
+      <c r="G437" s="1">
+        <v>1</v>
+      </c>
+      <c r="H437" s="1">
+        <v>0</v>
+      </c>
+      <c r="I437" s="1">
+        <v>0</v>
+      </c>
+      <c r="J437" s="1">
+        <v>0</v>
+      </c>
+      <c r="K437" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E437,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A438" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B438" s="6">
+        <v>2542</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E438" s="3">
+        <f>IF($A438="","",$A438-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F438" s="4">
+        <v>0</v>
+      </c>
+      <c r="G438" s="1">
+        <v>0</v>
+      </c>
+      <c r="H438" s="1">
+        <v>1</v>
+      </c>
+      <c r="I438" s="1">
+        <v>0</v>
+      </c>
+      <c r="J438" s="1">
+        <v>0</v>
+      </c>
+      <c r="K438" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E438,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A439" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B439" s="6">
+        <v>8744</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E439" s="3">
+        <f>IF($A439="","",$A439-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F439" s="4">
+        <v>0</v>
+      </c>
+      <c r="G439" s="1">
+        <v>0</v>
+      </c>
+      <c r="H439" s="1">
+        <v>1</v>
+      </c>
+      <c r="I439" s="1">
+        <v>0</v>
+      </c>
+      <c r="J439" s="1">
+        <v>0</v>
+      </c>
+      <c r="K439" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E439,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A440" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B440" s="6">
+        <v>7784</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E440" s="3">
+        <f>IF($A440="","",$A440-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F440" s="4">
+        <v>0</v>
+      </c>
+      <c r="G440" s="1">
+        <v>0</v>
+      </c>
+      <c r="H440" s="1">
+        <v>1</v>
+      </c>
+      <c r="I440" s="1">
+        <v>0</v>
+      </c>
+      <c r="J440" s="1">
+        <v>0</v>
+      </c>
+      <c r="K440" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E440,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A441" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B441" s="6">
+        <v>4379</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D441" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E441" s="3">
+        <f>IF($A441="","",$A441-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F441" s="4">
+        <v>0</v>
+      </c>
+      <c r="G441" s="1">
+        <v>0</v>
+      </c>
+      <c r="H441" s="1">
+        <v>1</v>
+      </c>
+      <c r="I441" s="1">
+        <v>0</v>
+      </c>
+      <c r="J441" s="1">
+        <v>0</v>
+      </c>
+      <c r="K441" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E441,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A442" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B442" s="6">
+        <v>5898</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E442" s="3">
+        <f>IF($A442="","",$A442-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F442" s="4">
+        <v>0</v>
+      </c>
+      <c r="G442" s="1">
+        <v>0</v>
+      </c>
+      <c r="H442" s="1">
+        <v>1</v>
+      </c>
+      <c r="I442" s="1">
+        <v>0</v>
+      </c>
+      <c r="J442" s="1">
+        <v>0</v>
+      </c>
+      <c r="K442" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E442,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A443" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B443" s="6">
+        <v>4790</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D443" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E443" s="3">
+        <f>IF($A443="","",$A443-1)</f>
+        <v>45031</v>
+      </c>
+      <c r="F443" s="4">
+        <v>0</v>
+      </c>
+      <c r="G443" s="1">
+        <v>0</v>
+      </c>
+      <c r="H443" s="1">
+        <v>1</v>
+      </c>
+      <c r="I443" s="1">
+        <v>0</v>
+      </c>
+      <c r="J443" s="1">
+        <v>0</v>
+      </c>
+      <c r="K443" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E443,"DD"))),0),"")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A444" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B444" s="6">
+        <v>6604</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E444" s="3">
+        <f>IF($A444="","",$A444-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F444" s="4">
+        <v>0</v>
+      </c>
+      <c r="G444" s="1">
+        <v>0</v>
+      </c>
+      <c r="H444" s="1">
+        <v>1</v>
+      </c>
+      <c r="I444" s="1">
+        <v>0</v>
+      </c>
+      <c r="J444" s="1">
+        <v>1</v>
+      </c>
+      <c r="K444" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E444,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A445" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B445" s="6">
+        <v>6241</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D445" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E445" s="3">
+        <f>IF($A445="","",$A445-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F445" s="4">
+        <v>0</v>
+      </c>
+      <c r="G445" s="1">
+        <v>0</v>
+      </c>
+      <c r="H445" s="1">
+        <v>0</v>
+      </c>
+      <c r="I445" s="1">
+        <v>0</v>
+      </c>
+      <c r="J445" s="1">
+        <v>1</v>
+      </c>
+      <c r="K445" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E445,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A446" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B446" s="6">
+        <v>5675</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D446" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E446" s="3">
+        <f>IF($A446="","",$A446-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F446" s="4">
+        <v>0</v>
+      </c>
+      <c r="G446" s="1">
+        <v>0</v>
+      </c>
+      <c r="H446" s="1">
+        <v>0</v>
+      </c>
+      <c r="I446" s="1">
+        <v>0</v>
+      </c>
+      <c r="J446" s="1">
+        <v>1</v>
+      </c>
+      <c r="K446" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E446,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A447" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B447" s="6">
+        <v>450</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D447" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E447" s="3">
+        <f>IF($A447="","",$A447-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F447" s="4">
+        <v>0</v>
+      </c>
+      <c r="G447" s="1">
+        <v>0</v>
+      </c>
+      <c r="H447" s="1">
+        <v>0</v>
+      </c>
+      <c r="I447" s="1">
+        <v>1</v>
+      </c>
+      <c r="J447" s="1">
+        <v>0</v>
+      </c>
+      <c r="K447" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E447,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A448" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B448" s="6">
+        <v>8631</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D448" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E448" s="3">
+        <f>IF($A448="","",$A448-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F448" s="4">
+        <v>0</v>
+      </c>
+      <c r="G448" s="1">
+        <v>0</v>
+      </c>
+      <c r="H448" s="1">
+        <v>0</v>
+      </c>
+      <c r="I448" s="1">
+        <v>1</v>
+      </c>
+      <c r="J448" s="1">
+        <v>0</v>
+      </c>
+      <c r="K448" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E448,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A449" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B449" s="6">
+        <v>3672</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D449" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E449" s="3">
+        <f>IF($A449="","",$A449-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F449" s="4">
+        <v>0</v>
+      </c>
+      <c r="G449" s="1">
+        <v>0</v>
+      </c>
+      <c r="H449" s="1">
+        <v>0</v>
+      </c>
+      <c r="I449" s="1">
+        <v>1</v>
+      </c>
+      <c r="J449" s="1">
+        <v>0</v>
+      </c>
+      <c r="K449" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E449,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A450" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B450" s="6">
+        <v>3570</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D450" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E450" s="3">
+        <f>IF($A450="","",$A450-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F450" s="4">
+        <v>0</v>
+      </c>
+      <c r="G450" s="1">
+        <v>0</v>
+      </c>
+      <c r="H450" s="1">
+        <v>0</v>
+      </c>
+      <c r="I450" s="1">
+        <v>1</v>
+      </c>
+      <c r="J450" s="1">
+        <v>0</v>
+      </c>
+      <c r="K450" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E450,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A451" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B451" s="6">
+        <v>8581</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D451" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E451" s="3">
+        <f>IF($A451="","",$A451-1)</f>
+        <v>45029</v>
+      </c>
+      <c r="F451" s="4">
+        <v>0</v>
+      </c>
+      <c r="G451" s="1">
+        <v>0</v>
+      </c>
+      <c r="H451" s="1">
+        <v>0</v>
+      </c>
+      <c r="I451" s="1">
+        <v>1</v>
+      </c>
+      <c r="J451" s="1">
+        <v>0</v>
+      </c>
+      <c r="K451" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E451,"DD"))),0),"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A452" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B452" s="6">
+        <v>5276</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D452" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E452" s="3">
+        <f>IF($A452="","",$A452-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F452" s="4">
+        <v>0</v>
+      </c>
+      <c r="G452" s="1">
+        <v>0</v>
+      </c>
+      <c r="H452" s="1">
+        <v>0</v>
+      </c>
+      <c r="I452" s="1">
+        <v>1</v>
+      </c>
+      <c r="J452" s="1">
+        <v>0</v>
+      </c>
+      <c r="K452" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E452,"DD"))),0),"")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A453" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B453" s="6">
+        <v>7364</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D453" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E453" s="3">
+        <f>IF($A453="","",$A453-1)</f>
+        <v>45030</v>
+      </c>
+      <c r="F453" s="4">
+        <v>0</v>
+      </c>
+      <c r="G453" s="1">
+        <v>0</v>
+      </c>
+      <c r="H453" s="1">
+        <v>0</v>
+      </c>
+      <c r="I453" s="1">
+        <v>1</v>
+      </c>
+      <c r="J453" s="1">
+        <v>0</v>
+      </c>
+      <c r="K453" s="1">
+        <f>IFERROR(ROUND((VALUE(TEXT($E453,"DD"))),0),"")</f>
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J408" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de Tipeo" error="solo es 1 u 0 para definir v o f" sqref="F2:J453" xr:uid="{8CF6DFF7-6E19-49C8-BBCC-BA3D02F40D32}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B408" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
-      <formula1>COUNTIF($B$2:$B$668,$B2)=1</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Usuario Existente" error="corrija el usuario o verifique si son correctos los datos" sqref="B2:B453" xr:uid="{7EFD80D6-4349-464B-8945-3AE549E90C43}">
+      <formula1>COUNTIF($B$2:$B$665,$B2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2 B138 B96 B198 B328" numberStoredAsText="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>